<commit_message>
Moved to readxl, fixed column headings.
</commit_message>
<xml_diff>
--- a/raw-data-prep/raw_data/Debrief_AM.xlsx
+++ b/raw-data-prep/raw_data/Debrief_AM.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
@@ -11,7 +11,7 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="122211"/>
+  <calcPr calcId="125725"/>
 </workbook>
 </file>
 
@@ -60,9 +60,6 @@
     <t>2.h</t>
   </si>
   <si>
-    <t>Game play affect distraction time</t>
-  </si>
-  <si>
     <t>Surprise</t>
   </si>
   <si>
@@ -634,13 +631,16 @@
   </si>
   <si>
     <t>To see if we were upset about the evaluation of our essays</t>
+  </si>
+  <si>
+    <t>Game.affect.distraction</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -760,7 +760,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -795,7 +794,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -971,19 +969,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:R183"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A184" sqref="A184"/>
+      <selection activeCell="R1" sqref="A1:R1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="15" max="15" width="10.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:18">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1027,19 +1025,19 @@
         <v>13</v>
       </c>
       <c r="O1" t="s">
+        <v>205</v>
+      </c>
+      <c r="P1" t="s">
         <v>14</v>
       </c>
-      <c r="P1" t="s">
+      <c r="Q1" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="R1" t="s">
         <v>16</v>
       </c>
-      <c r="R1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:18">
       <c r="A2">
         <v>32</v>
       </c>
@@ -1083,19 +1081,19 @@
         <v>1</v>
       </c>
       <c r="O2" t="s">
+        <v>17</v>
+      </c>
+      <c r="P2" t="s">
         <v>18</v>
-      </c>
-      <c r="P2" t="s">
-        <v>19</v>
       </c>
       <c r="Q2">
         <v>2</v>
       </c>
       <c r="R2" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18">
       <c r="A3">
         <v>28</v>
       </c>
@@ -1139,19 +1137,19 @@
         <v>0</v>
       </c>
       <c r="O3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="P3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="Q3">
         <v>3</v>
       </c>
       <c r="R3" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18">
       <c r="A4">
         <v>23</v>
       </c>
@@ -1195,19 +1193,19 @@
         <v>0</v>
       </c>
       <c r="O4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="P4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="Q4">
         <v>2</v>
       </c>
       <c r="R4" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18">
       <c r="A5">
         <v>5</v>
       </c>
@@ -1251,19 +1249,19 @@
         <v>0</v>
       </c>
       <c r="O5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="P5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="Q5">
         <v>1</v>
       </c>
       <c r="R5" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18">
       <c r="A6">
         <v>6</v>
       </c>
@@ -1307,19 +1305,19 @@
         <v>0</v>
       </c>
       <c r="O6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="P6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="Q6">
         <v>1</v>
       </c>
       <c r="R6" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18">
       <c r="A7">
         <v>2</v>
       </c>
@@ -1363,19 +1361,19 @@
         <v>0</v>
       </c>
       <c r="O7" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="P7" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="Q7">
         <v>4</v>
       </c>
       <c r="R7" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18">
       <c r="A8">
         <v>1</v>
       </c>
@@ -1419,19 +1417,19 @@
         <v>0</v>
       </c>
       <c r="O8" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="P8" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="Q8">
         <v>3</v>
       </c>
       <c r="R8" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="9" spans="1:18">
       <c r="A9">
         <v>3</v>
       </c>
@@ -1475,19 +1473,19 @@
         <v>0</v>
       </c>
       <c r="O9" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="P9" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="Q9">
         <v>3</v>
       </c>
       <c r="R9" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="10" spans="1:18">
       <c r="A10">
         <v>4</v>
       </c>
@@ -1531,19 +1529,19 @@
         <v>0</v>
       </c>
       <c r="O10" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="P10" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="Q10">
         <v>3</v>
       </c>
       <c r="R10" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="11" spans="1:18">
       <c r="A11">
         <v>8</v>
       </c>
@@ -1587,19 +1585,19 @@
         <v>0</v>
       </c>
       <c r="O11" t="s">
+        <v>17</v>
+      </c>
+      <c r="P11" t="s">
         <v>18</v>
-      </c>
-      <c r="P11" t="s">
-        <v>19</v>
       </c>
       <c r="Q11">
         <v>3</v>
       </c>
       <c r="R11" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="12" spans="1:18">
       <c r="A12">
         <v>7</v>
       </c>
@@ -1643,19 +1641,19 @@
         <v>0</v>
       </c>
       <c r="O12" t="s">
+        <v>17</v>
+      </c>
+      <c r="P12" t="s">
         <v>18</v>
-      </c>
-      <c r="P12" t="s">
-        <v>19</v>
       </c>
       <c r="Q12">
         <v>3</v>
       </c>
       <c r="R12" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="13" spans="1:18">
       <c r="A13">
         <v>10</v>
       </c>
@@ -1699,19 +1697,19 @@
         <v>0</v>
       </c>
       <c r="O13" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="P13" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="Q13">
         <v>4</v>
       </c>
       <c r="R13" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="14" spans="1:18">
       <c r="A14">
         <v>9</v>
       </c>
@@ -1755,19 +1753,19 @@
         <v>0</v>
       </c>
       <c r="O14" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="P14" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="Q14">
         <v>4</v>
       </c>
       <c r="R14" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="15" spans="1:18">
       <c r="A15">
         <v>12</v>
       </c>
@@ -1811,19 +1809,19 @@
         <v>0</v>
       </c>
       <c r="O15" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="P15" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="Q15">
         <v>2</v>
       </c>
       <c r="R15" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="16" spans="1:18">
       <c r="A16">
         <v>11</v>
       </c>
@@ -1867,19 +1865,19 @@
         <v>0</v>
       </c>
       <c r="O16" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="P16" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="Q16">
         <v>2</v>
       </c>
       <c r="R16" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="17" spans="1:18" x14ac:dyDescent="0.25">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="17" spans="1:18">
       <c r="A17">
         <v>14</v>
       </c>
@@ -1923,19 +1921,19 @@
         <v>0</v>
       </c>
       <c r="O17" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="P17" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="Q17">
         <v>5</v>
       </c>
       <c r="R17" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="18" spans="1:18" x14ac:dyDescent="0.25">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="18" spans="1:18">
       <c r="A18">
         <v>13</v>
       </c>
@@ -1979,19 +1977,19 @@
         <v>1</v>
       </c>
       <c r="O18" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="P18" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="Q18">
         <v>2</v>
       </c>
       <c r="R18" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="19" spans="1:18" x14ac:dyDescent="0.25">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="19" spans="1:18">
       <c r="A19">
         <v>16</v>
       </c>
@@ -2035,19 +2033,19 @@
         <v>0</v>
       </c>
       <c r="O19" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="P19" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="Q19">
         <v>2</v>
       </c>
       <c r="R19" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="20" spans="1:18" x14ac:dyDescent="0.25">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="20" spans="1:18">
       <c r="A20">
         <v>18</v>
       </c>
@@ -2091,19 +2089,19 @@
         <v>0</v>
       </c>
       <c r="O20" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="P20" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="Q20">
         <v>4</v>
       </c>
       <c r="R20" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="21" spans="1:18" x14ac:dyDescent="0.25">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="21" spans="1:18">
       <c r="A21">
         <v>21</v>
       </c>
@@ -2147,19 +2145,19 @@
         <v>0</v>
       </c>
       <c r="O21" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="P21" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="Q21">
         <v>3</v>
       </c>
       <c r="R21" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="22" spans="1:18" x14ac:dyDescent="0.25">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="22" spans="1:18">
       <c r="A22">
         <v>17</v>
       </c>
@@ -2203,19 +2201,19 @@
         <v>0</v>
       </c>
       <c r="O22" t="s">
+        <v>17</v>
+      </c>
+      <c r="P22" t="s">
         <v>18</v>
-      </c>
-      <c r="P22" t="s">
-        <v>19</v>
       </c>
       <c r="Q22">
         <v>3</v>
       </c>
       <c r="R22" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="23" spans="1:18" x14ac:dyDescent="0.25">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="23" spans="1:18">
       <c r="A23">
         <v>19</v>
       </c>
@@ -2259,19 +2257,19 @@
         <v>0</v>
       </c>
       <c r="O23" t="s">
+        <v>17</v>
+      </c>
+      <c r="P23" t="s">
         <v>18</v>
-      </c>
-      <c r="P23" t="s">
-        <v>19</v>
       </c>
       <c r="Q23">
         <v>2</v>
       </c>
       <c r="R23" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="24" spans="1:18" x14ac:dyDescent="0.25">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="24" spans="1:18">
       <c r="A24">
         <v>20</v>
       </c>
@@ -2315,19 +2313,19 @@
         <v>1</v>
       </c>
       <c r="O24" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="P24" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="Q24">
         <v>5</v>
       </c>
       <c r="R24" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="25" spans="1:18" x14ac:dyDescent="0.25">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="25" spans="1:18">
       <c r="A25">
         <v>22</v>
       </c>
@@ -2371,19 +2369,19 @@
         <v>0</v>
       </c>
       <c r="O25" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="P25" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="Q25">
         <v>4</v>
       </c>
       <c r="R25" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="26" spans="1:18" x14ac:dyDescent="0.25">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="26" spans="1:18">
       <c r="A26">
         <v>15</v>
       </c>
@@ -2427,19 +2425,19 @@
         <v>0</v>
       </c>
       <c r="O26" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="P26" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="Q26">
         <v>4</v>
       </c>
       <c r="R26" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="27" spans="1:18" x14ac:dyDescent="0.25">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="27" spans="1:18">
       <c r="A27">
         <v>24</v>
       </c>
@@ -2483,19 +2481,19 @@
         <v>0</v>
       </c>
       <c r="O27" t="s">
+        <v>17</v>
+      </c>
+      <c r="P27" t="s">
         <v>18</v>
-      </c>
-      <c r="P27" t="s">
-        <v>19</v>
       </c>
       <c r="Q27">
         <v>3</v>
       </c>
       <c r="R27" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="28" spans="1:18" x14ac:dyDescent="0.25">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="28" spans="1:18">
       <c r="A28">
         <v>26</v>
       </c>
@@ -2539,19 +2537,19 @@
         <v>0</v>
       </c>
       <c r="O28" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="P28" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="Q28">
         <v>1</v>
       </c>
       <c r="R28" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="29" spans="1:18" x14ac:dyDescent="0.25">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="29" spans="1:18">
       <c r="A29">
         <v>25</v>
       </c>
@@ -2595,19 +2593,19 @@
         <v>0</v>
       </c>
       <c r="O29" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="P29" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="Q29">
         <v>1</v>
       </c>
       <c r="R29" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="30" spans="1:18" x14ac:dyDescent="0.25">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="30" spans="1:18">
       <c r="A30">
         <v>27</v>
       </c>
@@ -2651,19 +2649,19 @@
         <v>0</v>
       </c>
       <c r="O30" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="P30" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="Q30">
         <v>3</v>
       </c>
       <c r="R30" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="31" spans="1:18" x14ac:dyDescent="0.25">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="31" spans="1:18">
       <c r="A31">
         <v>31</v>
       </c>
@@ -2707,19 +2705,19 @@
         <v>0</v>
       </c>
       <c r="O31" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="P31" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="Q31">
         <v>2</v>
       </c>
       <c r="R31" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="32" spans="1:18" x14ac:dyDescent="0.25">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="32" spans="1:18">
       <c r="A32">
         <v>29</v>
       </c>
@@ -2763,19 +2761,19 @@
         <v>0</v>
       </c>
       <c r="O32" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="P32" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="Q32">
         <v>4</v>
       </c>
       <c r="R32" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="33" spans="1:18" x14ac:dyDescent="0.25">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="33" spans="1:18">
       <c r="A33">
         <v>30</v>
       </c>
@@ -2819,19 +2817,19 @@
         <v>0</v>
       </c>
       <c r="O33" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="P33" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="Q33">
         <v>2</v>
       </c>
       <c r="R33" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="34" spans="1:18" x14ac:dyDescent="0.25">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="34" spans="1:18">
       <c r="A34">
         <v>34</v>
       </c>
@@ -2875,19 +2873,19 @@
         <v>0</v>
       </c>
       <c r="O34" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="P34" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="Q34">
         <v>1</v>
       </c>
       <c r="R34" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="35" spans="1:18" x14ac:dyDescent="0.25">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="35" spans="1:18">
       <c r="A35">
         <v>33</v>
       </c>
@@ -2931,19 +2929,19 @@
         <v>0</v>
       </c>
       <c r="O35" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="P35" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="Q35">
         <v>3</v>
       </c>
       <c r="R35" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="36" spans="1:18" x14ac:dyDescent="0.25">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="36" spans="1:18">
       <c r="A36">
         <v>36</v>
       </c>
@@ -2987,19 +2985,19 @@
         <v>0</v>
       </c>
       <c r="O36" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="P36" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="Q36">
         <v>2</v>
       </c>
       <c r="R36" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="37" spans="1:18" x14ac:dyDescent="0.25">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="37" spans="1:18">
       <c r="A37">
         <v>35</v>
       </c>
@@ -3043,19 +3041,19 @@
         <v>0</v>
       </c>
       <c r="O37" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="P37" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="Q37">
         <v>3</v>
       </c>
       <c r="R37" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="38" spans="1:18" x14ac:dyDescent="0.25">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="38" spans="1:18">
       <c r="A38">
         <v>38</v>
       </c>
@@ -3099,19 +3097,19 @@
         <v>0</v>
       </c>
       <c r="O38" t="s">
+        <v>17</v>
+      </c>
+      <c r="P38" t="s">
         <v>18</v>
-      </c>
-      <c r="P38" t="s">
-        <v>19</v>
       </c>
       <c r="Q38">
         <v>4</v>
       </c>
       <c r="R38" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="39" spans="1:18" x14ac:dyDescent="0.25">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="39" spans="1:18">
       <c r="A39">
         <v>37</v>
       </c>
@@ -3155,19 +3153,19 @@
         <v>0</v>
       </c>
       <c r="O39" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="P39" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="Q39">
         <v>4</v>
       </c>
       <c r="R39" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="40" spans="1:18" x14ac:dyDescent="0.25">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="40" spans="1:18">
       <c r="A40">
         <v>40</v>
       </c>
@@ -3211,19 +3209,19 @@
         <v>0</v>
       </c>
       <c r="O40" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="P40" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="Q40">
         <v>2</v>
       </c>
       <c r="R40" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="41" spans="1:18" x14ac:dyDescent="0.25">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="41" spans="1:18">
       <c r="A41">
         <v>39</v>
       </c>
@@ -3267,19 +3265,19 @@
         <v>0</v>
       </c>
       <c r="O41" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="P41" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="Q41">
         <v>1</v>
       </c>
       <c r="R41" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="42" spans="1:18" x14ac:dyDescent="0.25">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="42" spans="1:18">
       <c r="A42">
         <v>41</v>
       </c>
@@ -3323,19 +3321,19 @@
         <v>0</v>
       </c>
       <c r="O42" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="P42" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="Q42">
         <v>5</v>
       </c>
       <c r="R42" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="43" spans="1:18" x14ac:dyDescent="0.25">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="43" spans="1:18">
       <c r="A43">
         <v>42</v>
       </c>
@@ -3379,19 +3377,19 @@
         <v>0</v>
       </c>
       <c r="O43" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="P43" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="Q43">
         <v>3</v>
       </c>
       <c r="R43" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="44" spans="1:18" x14ac:dyDescent="0.25">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="44" spans="1:18">
       <c r="A44">
         <v>43</v>
       </c>
@@ -3435,19 +3433,19 @@
         <v>0</v>
       </c>
       <c r="O44" t="s">
+        <v>17</v>
+      </c>
+      <c r="P44" t="s">
         <v>18</v>
-      </c>
-      <c r="P44" t="s">
-        <v>19</v>
       </c>
       <c r="Q44">
         <v>4</v>
       </c>
       <c r="R44" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="45" spans="1:18" x14ac:dyDescent="0.25">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="45" spans="1:18">
       <c r="A45">
         <v>80</v>
       </c>
@@ -3491,19 +3489,19 @@
         <v>0</v>
       </c>
       <c r="O45" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="P45" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="Q45">
         <v>5</v>
       </c>
       <c r="R45" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="46" spans="1:18" x14ac:dyDescent="0.25">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="46" spans="1:18">
       <c r="A46">
         <v>81</v>
       </c>
@@ -3547,19 +3545,19 @@
         <v>0</v>
       </c>
       <c r="O46" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="P46" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="Q46">
         <v>4</v>
       </c>
       <c r="R46" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="47" spans="1:18" x14ac:dyDescent="0.25">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="47" spans="1:18">
       <c r="A47">
         <v>82</v>
       </c>
@@ -3603,19 +3601,19 @@
         <v>0</v>
       </c>
       <c r="O47" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="P47" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="Q47">
         <v>4</v>
       </c>
       <c r="R47" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="48" spans="1:18" x14ac:dyDescent="0.25">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="48" spans="1:18">
       <c r="A48">
         <v>83</v>
       </c>
@@ -3659,19 +3657,19 @@
         <v>0</v>
       </c>
       <c r="O48" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="P48" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="Q48">
         <v>4</v>
       </c>
       <c r="R48" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="49" spans="1:18" x14ac:dyDescent="0.25">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="49" spans="1:18">
       <c r="A49">
         <v>84</v>
       </c>
@@ -3715,19 +3713,19 @@
         <v>0</v>
       </c>
       <c r="O49" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="P49" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="Q49">
         <v>2</v>
       </c>
       <c r="R49" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="50" spans="1:18" x14ac:dyDescent="0.25">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="50" spans="1:18">
       <c r="A50">
         <v>85</v>
       </c>
@@ -3771,19 +3769,19 @@
         <v>0</v>
       </c>
       <c r="O50" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="P50" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="Q50">
         <v>4</v>
       </c>
       <c r="R50" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="51" spans="1:18" x14ac:dyDescent="0.25">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="51" spans="1:18">
       <c r="A51">
         <v>86</v>
       </c>
@@ -3827,19 +3825,19 @@
         <v>0</v>
       </c>
       <c r="O51" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="P51" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="Q51">
         <v>2</v>
       </c>
       <c r="R51" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="52" spans="1:18" x14ac:dyDescent="0.25">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="52" spans="1:18">
       <c r="A52">
         <v>87</v>
       </c>
@@ -3883,19 +3881,19 @@
         <v>0</v>
       </c>
       <c r="O52" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="P52" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="Q52">
         <v>2</v>
       </c>
       <c r="R52" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="53" spans="1:18" x14ac:dyDescent="0.25">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="53" spans="1:18">
       <c r="A53">
         <v>71</v>
       </c>
@@ -3939,19 +3937,19 @@
         <v>0</v>
       </c>
       <c r="O53" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="P53" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="Q53">
         <v>3</v>
       </c>
       <c r="R53" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="54" spans="1:18" x14ac:dyDescent="0.25">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="54" spans="1:18">
       <c r="A54">
         <v>73</v>
       </c>
@@ -3995,19 +3993,19 @@
         <v>0</v>
       </c>
       <c r="O54" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="P54" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="Q54">
         <v>2</v>
       </c>
       <c r="R54" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="55" spans="1:18" x14ac:dyDescent="0.25">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="55" spans="1:18">
       <c r="A55">
         <v>72</v>
       </c>
@@ -4051,19 +4049,19 @@
         <v>1</v>
       </c>
       <c r="O55" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="P55" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="Q55">
         <v>2</v>
       </c>
       <c r="R55" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="56" spans="1:18" x14ac:dyDescent="0.25">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="56" spans="1:18">
       <c r="A56">
         <v>74</v>
       </c>
@@ -4104,19 +4102,19 @@
         <v>0</v>
       </c>
       <c r="O56" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="P56" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="Q56">
         <v>4</v>
       </c>
       <c r="R56" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="57" spans="1:18" x14ac:dyDescent="0.25">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="57" spans="1:18">
       <c r="A57">
         <v>75</v>
       </c>
@@ -4160,19 +4158,19 @@
         <v>0</v>
       </c>
       <c r="O57" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="P57" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="Q57">
         <v>4</v>
       </c>
       <c r="R57" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="58" spans="1:18" x14ac:dyDescent="0.25">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="58" spans="1:18">
       <c r="A58">
         <v>76</v>
       </c>
@@ -4216,19 +4214,19 @@
         <v>0</v>
       </c>
       <c r="O58" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="P58" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="Q58">
         <v>4</v>
       </c>
       <c r="R58" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="59" spans="1:18" x14ac:dyDescent="0.25">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="59" spans="1:18">
       <c r="A59">
         <v>77</v>
       </c>
@@ -4272,19 +4270,19 @@
         <v>0</v>
       </c>
       <c r="O59" t="s">
+        <v>17</v>
+      </c>
+      <c r="P59" t="s">
         <v>18</v>
       </c>
-      <c r="P59" t="s">
-        <v>19</v>
-      </c>
       <c r="Q59">
         <v>1</v>
       </c>
       <c r="R59" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="60" spans="1:18" x14ac:dyDescent="0.25">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="60" spans="1:18">
       <c r="A60">
         <v>78</v>
       </c>
@@ -4328,19 +4326,19 @@
         <v>0</v>
       </c>
       <c r="O60" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="P60" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="Q60">
         <v>5</v>
       </c>
       <c r="R60" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="61" spans="1:18" x14ac:dyDescent="0.25">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="61" spans="1:18">
       <c r="A61">
         <v>79</v>
       </c>
@@ -4384,19 +4382,19 @@
         <v>0</v>
       </c>
       <c r="O61" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="P61" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="Q61">
         <v>4</v>
       </c>
       <c r="R61" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="62" spans="1:18" x14ac:dyDescent="0.25">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="62" spans="1:18">
       <c r="A62">
         <v>88</v>
       </c>
@@ -4440,19 +4438,19 @@
         <v>0</v>
       </c>
       <c r="O62" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="P62" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="Q62">
         <v>3</v>
       </c>
       <c r="R62" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="63" spans="1:18" x14ac:dyDescent="0.25">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="63" spans="1:18">
       <c r="A63">
         <v>90</v>
       </c>
@@ -4496,19 +4494,19 @@
         <v>0</v>
       </c>
       <c r="O63" t="s">
+        <v>17</v>
+      </c>
+      <c r="P63" t="s">
         <v>18</v>
-      </c>
-      <c r="P63" t="s">
-        <v>19</v>
       </c>
       <c r="Q63">
         <v>2</v>
       </c>
       <c r="R63" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="64" spans="1:18" x14ac:dyDescent="0.25">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="64" spans="1:18">
       <c r="A64">
         <v>89</v>
       </c>
@@ -4552,19 +4550,19 @@
         <v>0</v>
       </c>
       <c r="O64" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="P64" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="Q64">
         <v>5</v>
       </c>
       <c r="R64" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="65" spans="1:18" x14ac:dyDescent="0.25">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="65" spans="1:18">
       <c r="A65">
         <v>92</v>
       </c>
@@ -4608,19 +4606,19 @@
         <v>0</v>
       </c>
       <c r="O65" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="P65" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="Q65">
         <v>3</v>
       </c>
       <c r="R65" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="66" spans="1:18" x14ac:dyDescent="0.25">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="66" spans="1:18">
       <c r="A66">
         <v>91</v>
       </c>
@@ -4664,19 +4662,19 @@
         <v>0</v>
       </c>
       <c r="O66" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="P66" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="Q66">
         <v>2</v>
       </c>
       <c r="R66" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="67" spans="1:18" x14ac:dyDescent="0.25">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="67" spans="1:18">
       <c r="A67">
         <v>94</v>
       </c>
@@ -4720,19 +4718,19 @@
         <v>0</v>
       </c>
       <c r="O67" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="P67" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="Q67">
         <v>4</v>
       </c>
       <c r="R67" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="68" spans="1:18" x14ac:dyDescent="0.25">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="68" spans="1:18">
       <c r="A68">
         <v>96</v>
       </c>
@@ -4776,19 +4774,19 @@
         <v>0</v>
       </c>
       <c r="O68" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="P68" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="Q68">
         <v>3</v>
       </c>
       <c r="R68" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="69" spans="1:18" x14ac:dyDescent="0.25">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="69" spans="1:18">
       <c r="A69">
         <v>95</v>
       </c>
@@ -4832,19 +4830,19 @@
         <v>0</v>
       </c>
       <c r="O69" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="P69" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="Q69">
         <v>1</v>
       </c>
       <c r="R69" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="70" spans="1:18" x14ac:dyDescent="0.25">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="70" spans="1:18">
       <c r="A70">
         <v>98</v>
       </c>
@@ -4888,19 +4886,19 @@
         <v>0</v>
       </c>
       <c r="O70" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="P70" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="Q70">
         <v>4</v>
       </c>
       <c r="R70" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="71" spans="1:18" x14ac:dyDescent="0.25">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="71" spans="1:18">
       <c r="A71">
         <v>97</v>
       </c>
@@ -4944,19 +4942,19 @@
         <v>0</v>
       </c>
       <c r="O71" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="P71" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="Q71">
         <v>1</v>
       </c>
       <c r="R71" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="72" spans="1:18" x14ac:dyDescent="0.25">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="72" spans="1:18">
       <c r="A72">
         <v>99</v>
       </c>
@@ -5000,19 +4998,19 @@
         <v>0</v>
       </c>
       <c r="O72" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="P72" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="Q72">
         <v>2</v>
       </c>
       <c r="R72" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="73" spans="1:18" x14ac:dyDescent="0.25">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="73" spans="1:18">
       <c r="A73">
         <v>100</v>
       </c>
@@ -5056,19 +5054,19 @@
         <v>0</v>
       </c>
       <c r="O73" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="P73" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="Q73">
         <v>5</v>
       </c>
       <c r="R73" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="74" spans="1:18" x14ac:dyDescent="0.25">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="74" spans="1:18">
       <c r="A74">
         <v>102</v>
       </c>
@@ -5112,19 +5110,19 @@
         <v>0</v>
       </c>
       <c r="O74" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="P74" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="Q74">
         <v>2</v>
       </c>
       <c r="R74" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="75" spans="1:18" x14ac:dyDescent="0.25">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="75" spans="1:18">
       <c r="A75">
         <v>101</v>
       </c>
@@ -5168,19 +5166,19 @@
         <v>0</v>
       </c>
       <c r="O75" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="P75" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="Q75">
         <v>4</v>
       </c>
       <c r="R75" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="76" spans="1:18" x14ac:dyDescent="0.25">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="76" spans="1:18">
       <c r="A76">
         <v>52</v>
       </c>
@@ -5224,19 +5222,19 @@
         <v>0</v>
       </c>
       <c r="O76" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="P76" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="Q76">
         <v>3</v>
       </c>
       <c r="R76" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="77" spans="1:18" x14ac:dyDescent="0.25">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="77" spans="1:18">
       <c r="A77">
         <v>104</v>
       </c>
@@ -5280,19 +5278,19 @@
         <v>0</v>
       </c>
       <c r="O77" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="P77" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="Q77">
         <v>4</v>
       </c>
       <c r="R77" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="78" spans="1:18" x14ac:dyDescent="0.25">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="78" spans="1:18">
       <c r="A78">
         <v>103</v>
       </c>
@@ -5336,19 +5334,19 @@
         <v>0</v>
       </c>
       <c r="O78" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="P78" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="Q78">
         <v>2</v>
       </c>
       <c r="R78" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="79" spans="1:18" x14ac:dyDescent="0.25">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="79" spans="1:18">
       <c r="A79">
         <v>106</v>
       </c>
@@ -5392,19 +5390,19 @@
         <v>0</v>
       </c>
       <c r="O79" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="P79" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="Q79">
         <v>4</v>
       </c>
       <c r="R79" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="80" spans="1:18" x14ac:dyDescent="0.25">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="80" spans="1:18">
       <c r="A80">
         <v>105</v>
       </c>
@@ -5448,19 +5446,19 @@
         <v>0</v>
       </c>
       <c r="O80" t="s">
+        <v>17</v>
+      </c>
+      <c r="P80" t="s">
         <v>18</v>
-      </c>
-      <c r="P80" t="s">
-        <v>19</v>
       </c>
       <c r="Q80">
         <v>2</v>
       </c>
       <c r="R80" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="81" spans="1:18" x14ac:dyDescent="0.25">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="81" spans="1:18">
       <c r="A81">
         <v>107</v>
       </c>
@@ -5504,19 +5502,19 @@
         <v>0</v>
       </c>
       <c r="O81" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="P81" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="Q81">
         <v>2</v>
       </c>
       <c r="R81" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="82" spans="1:18" x14ac:dyDescent="0.25">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="82" spans="1:18">
       <c r="A82">
         <v>108</v>
       </c>
@@ -5560,19 +5558,19 @@
         <v>0</v>
       </c>
       <c r="O82" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="P82" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="Q82">
         <v>3</v>
       </c>
       <c r="R82" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="83" spans="1:18" x14ac:dyDescent="0.25">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="83" spans="1:18">
       <c r="A83">
         <v>109</v>
       </c>
@@ -5616,19 +5614,19 @@
         <v>0</v>
       </c>
       <c r="O83" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="P83" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="Q83">
         <v>2</v>
       </c>
       <c r="R83" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="84" spans="1:18" x14ac:dyDescent="0.25">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="84" spans="1:18">
       <c r="A84">
         <v>110</v>
       </c>
@@ -5672,19 +5670,19 @@
         <v>0</v>
       </c>
       <c r="O84" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="P84" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="Q84">
         <v>2</v>
       </c>
       <c r="R84" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="85" spans="1:18" x14ac:dyDescent="0.25">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="85" spans="1:18">
       <c r="A85">
         <v>111</v>
       </c>
@@ -5728,19 +5726,19 @@
         <v>0</v>
       </c>
       <c r="O85" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="P85" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="Q85">
         <v>1</v>
       </c>
       <c r="R85" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="86" spans="1:18" x14ac:dyDescent="0.25">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="86" spans="1:18">
       <c r="A86">
         <v>112</v>
       </c>
@@ -5784,19 +5782,19 @@
         <v>0</v>
       </c>
       <c r="O86" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="P86" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="Q86">
         <v>3</v>
       </c>
       <c r="R86" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="87" spans="1:18" x14ac:dyDescent="0.25">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="87" spans="1:18">
       <c r="A87">
         <v>113</v>
       </c>
@@ -5840,19 +5838,19 @@
         <v>0</v>
       </c>
       <c r="O87" t="s">
+        <v>17</v>
+      </c>
+      <c r="P87" t="s">
         <v>18</v>
-      </c>
-      <c r="P87" t="s">
-        <v>19</v>
       </c>
       <c r="Q87">
         <v>2</v>
       </c>
       <c r="R87" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="88" spans="1:18" x14ac:dyDescent="0.25">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="88" spans="1:18">
       <c r="A88">
         <v>114</v>
       </c>
@@ -5896,19 +5894,19 @@
         <v>0</v>
       </c>
       <c r="O88" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="P88" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="Q88">
         <v>4</v>
       </c>
       <c r="R88" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="89" spans="1:18" x14ac:dyDescent="0.25">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="89" spans="1:18">
       <c r="A89">
         <v>115</v>
       </c>
@@ -5952,19 +5950,19 @@
         <v>0</v>
       </c>
       <c r="O89" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="P89" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="Q89">
         <v>4</v>
       </c>
       <c r="R89" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="90" spans="1:18" x14ac:dyDescent="0.25">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="90" spans="1:18">
       <c r="A90">
         <v>116</v>
       </c>
@@ -6008,19 +6006,19 @@
         <v>0</v>
       </c>
       <c r="O90" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="P90" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="Q90">
         <v>2</v>
       </c>
       <c r="R90" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="91" spans="1:18" x14ac:dyDescent="0.25">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="91" spans="1:18">
       <c r="A91">
         <v>117</v>
       </c>
@@ -6064,19 +6062,19 @@
         <v>0</v>
       </c>
       <c r="O91" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="P91" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="Q91">
         <v>5</v>
       </c>
       <c r="R91" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="92" spans="1:18" x14ac:dyDescent="0.25">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="92" spans="1:18">
       <c r="A92">
         <v>119</v>
       </c>
@@ -6120,19 +6118,19 @@
         <v>0</v>
       </c>
       <c r="O92" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="P92" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="Q92">
         <v>4</v>
       </c>
       <c r="R92" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="93" spans="1:18" x14ac:dyDescent="0.25">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="93" spans="1:18">
       <c r="A93">
         <v>118</v>
       </c>
@@ -6176,19 +6174,19 @@
         <v>0</v>
       </c>
       <c r="O93" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="P93" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="Q93">
         <v>2</v>
       </c>
       <c r="R93" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="94" spans="1:18" x14ac:dyDescent="0.25">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="94" spans="1:18">
       <c r="A94">
         <v>120</v>
       </c>
@@ -6232,19 +6230,19 @@
         <v>0</v>
       </c>
       <c r="O94" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="P94" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="Q94">
         <v>2</v>
       </c>
       <c r="R94" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="95" spans="1:18" x14ac:dyDescent="0.25">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="95" spans="1:18">
       <c r="A95">
         <v>121</v>
       </c>
@@ -6288,19 +6286,19 @@
         <v>0</v>
       </c>
       <c r="O95" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="P95" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="Q95">
         <v>1</v>
       </c>
       <c r="R95" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="96" spans="1:18" x14ac:dyDescent="0.25">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="96" spans="1:18">
       <c r="A96">
         <v>122</v>
       </c>
@@ -6344,19 +6342,19 @@
         <v>0</v>
       </c>
       <c r="O96" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="P96" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="Q96">
         <v>4</v>
       </c>
       <c r="R96" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="97" spans="1:18" x14ac:dyDescent="0.25">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="97" spans="1:18">
       <c r="A97">
         <v>123</v>
       </c>
@@ -6400,19 +6398,19 @@
         <v>0</v>
       </c>
       <c r="O97" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="P97" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="Q97">
         <v>2</v>
       </c>
       <c r="R97" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="98" spans="1:18" x14ac:dyDescent="0.25">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="98" spans="1:18">
       <c r="A98">
         <v>64</v>
       </c>
@@ -6456,19 +6454,19 @@
         <v>0</v>
       </c>
       <c r="O98" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="P98" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="Q98">
         <v>1</v>
       </c>
       <c r="R98" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="99" spans="1:18" x14ac:dyDescent="0.25">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="99" spans="1:18">
       <c r="A99">
         <v>63</v>
       </c>
@@ -6512,19 +6510,19 @@
         <v>0</v>
       </c>
       <c r="O99" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="P99" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="Q99">
         <v>4</v>
       </c>
       <c r="R99" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="100" spans="1:18" x14ac:dyDescent="0.25">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="100" spans="1:18">
       <c r="A100">
         <v>62</v>
       </c>
@@ -6568,19 +6566,19 @@
         <v>0</v>
       </c>
       <c r="O100" t="s">
+        <v>17</v>
+      </c>
+      <c r="P100" t="s">
         <v>18</v>
-      </c>
-      <c r="P100" t="s">
-        <v>19</v>
       </c>
       <c r="Q100">
         <v>2</v>
       </c>
       <c r="R100" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="101" spans="1:18" x14ac:dyDescent="0.25">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="101" spans="1:18">
       <c r="A101">
         <v>61</v>
       </c>
@@ -6624,19 +6622,19 @@
         <v>0</v>
       </c>
       <c r="O101" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="P101" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="Q101">
         <v>2</v>
       </c>
       <c r="R101" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="102" spans="1:18" x14ac:dyDescent="0.25">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="102" spans="1:18">
       <c r="A102">
         <v>60</v>
       </c>
@@ -6680,19 +6678,19 @@
         <v>0</v>
       </c>
       <c r="O102" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="P102" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="Q102">
         <v>1</v>
       </c>
       <c r="R102" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="103" spans="1:18" x14ac:dyDescent="0.25">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="103" spans="1:18">
       <c r="A103">
         <v>58</v>
       </c>
@@ -6736,19 +6734,19 @@
         <v>0</v>
       </c>
       <c r="O103" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="P103" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="Q103">
         <v>1</v>
       </c>
       <c r="R103" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="104" spans="1:18" x14ac:dyDescent="0.25">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="104" spans="1:18">
       <c r="A104">
         <v>57</v>
       </c>
@@ -6792,19 +6790,19 @@
         <v>0</v>
       </c>
       <c r="O104" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="P104" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="Q104">
         <v>3</v>
       </c>
       <c r="R104" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="105" spans="1:18" x14ac:dyDescent="0.25">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="105" spans="1:18">
       <c r="A105">
         <v>59</v>
       </c>
@@ -6848,19 +6846,19 @@
         <v>0</v>
       </c>
       <c r="O105" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="P105" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="Q105">
         <v>2</v>
       </c>
       <c r="R105" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="106" spans="1:18" x14ac:dyDescent="0.25">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="106" spans="1:18">
       <c r="A106">
         <v>56</v>
       </c>
@@ -6904,19 +6902,19 @@
         <v>0</v>
       </c>
       <c r="O106" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="P106" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="Q106">
         <v>2</v>
       </c>
       <c r="R106" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="107" spans="1:18" x14ac:dyDescent="0.25">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="107" spans="1:18">
       <c r="A107">
         <v>55</v>
       </c>
@@ -6960,19 +6958,19 @@
         <v>0</v>
       </c>
       <c r="O107" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="P107" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="Q107">
         <v>3</v>
       </c>
       <c r="R107" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="108" spans="1:18" x14ac:dyDescent="0.25">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="108" spans="1:18">
       <c r="A108">
         <v>54</v>
       </c>
@@ -7016,19 +7014,19 @@
         <v>0</v>
       </c>
       <c r="O108" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="P108" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="Q108">
         <v>3</v>
       </c>
       <c r="R108" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="109" spans="1:18" x14ac:dyDescent="0.25">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="109" spans="1:18">
       <c r="A109">
         <v>53</v>
       </c>
@@ -7072,19 +7070,19 @@
         <v>0</v>
       </c>
       <c r="O109" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="P109" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="Q109">
         <v>3</v>
       </c>
       <c r="R109" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="110" spans="1:18" x14ac:dyDescent="0.25">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="110" spans="1:18">
       <c r="A110">
         <v>50</v>
       </c>
@@ -7128,19 +7126,19 @@
         <v>0</v>
       </c>
       <c r="O110" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="P110" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="Q110">
         <v>2</v>
       </c>
       <c r="R110" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="111" spans="1:18" x14ac:dyDescent="0.25">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="111" spans="1:18">
       <c r="A111">
         <v>51</v>
       </c>
@@ -7184,19 +7182,19 @@
         <v>0</v>
       </c>
       <c r="O111" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="P111" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="Q111">
         <v>2</v>
       </c>
       <c r="R111" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="112" spans="1:18" x14ac:dyDescent="0.25">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="112" spans="1:18">
       <c r="A112">
         <v>48</v>
       </c>
@@ -7240,19 +7238,19 @@
         <v>0</v>
       </c>
       <c r="O112" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="P112" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="Q112">
         <v>5</v>
       </c>
       <c r="R112" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="113" spans="1:18" x14ac:dyDescent="0.25">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="113" spans="1:18">
       <c r="A113">
         <v>49</v>
       </c>
@@ -7296,19 +7294,19 @@
         <v>0</v>
       </c>
       <c r="O113" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="P113" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="Q113">
         <v>2</v>
       </c>
       <c r="R113" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="114" spans="1:18" x14ac:dyDescent="0.25">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="114" spans="1:18">
       <c r="A114">
         <v>46</v>
       </c>
@@ -7352,19 +7350,19 @@
         <v>0</v>
       </c>
       <c r="O114" t="s">
+        <v>17</v>
+      </c>
+      <c r="P114" t="s">
         <v>18</v>
-      </c>
-      <c r="P114" t="s">
-        <v>19</v>
       </c>
       <c r="Q114">
         <v>4</v>
       </c>
       <c r="R114" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="115" spans="1:18" x14ac:dyDescent="0.25">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="115" spans="1:18">
       <c r="A115">
         <v>47</v>
       </c>
@@ -7408,19 +7406,19 @@
         <v>0</v>
       </c>
       <c r="O115" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="P115" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="Q115">
         <v>2</v>
       </c>
       <c r="R115" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="116" spans="1:18" x14ac:dyDescent="0.25">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="116" spans="1:18">
       <c r="A116">
         <v>44</v>
       </c>
@@ -7464,19 +7462,19 @@
         <v>0</v>
       </c>
       <c r="O116" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="P116" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="Q116">
         <v>3</v>
       </c>
       <c r="R116" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="117" spans="1:18" x14ac:dyDescent="0.25">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="117" spans="1:18">
       <c r="A117">
         <v>45</v>
       </c>
@@ -7520,19 +7518,19 @@
         <v>0</v>
       </c>
       <c r="O117" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="P117" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="Q117">
         <v>2</v>
       </c>
       <c r="R117" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="118" spans="1:18" x14ac:dyDescent="0.25">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="118" spans="1:18">
       <c r="A118">
         <v>93</v>
       </c>
@@ -7576,19 +7574,19 @@
         <v>0</v>
       </c>
       <c r="O118" t="s">
+        <v>17</v>
+      </c>
+      <c r="P118" t="s">
         <v>18</v>
-      </c>
-      <c r="P118" t="s">
-        <v>19</v>
       </c>
       <c r="Q118">
         <v>4</v>
       </c>
       <c r="R118" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="119" spans="1:18" x14ac:dyDescent="0.25">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="119" spans="1:18">
       <c r="A119">
         <v>70</v>
       </c>
@@ -7632,19 +7630,19 @@
         <v>1</v>
       </c>
       <c r="O119" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="P119" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="Q119">
         <v>3</v>
       </c>
       <c r="R119" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="120" spans="1:18" x14ac:dyDescent="0.25">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="120" spans="1:18">
       <c r="A120">
         <v>66</v>
       </c>
@@ -7688,19 +7686,19 @@
         <v>0</v>
       </c>
       <c r="O120" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="P120" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="Q120">
         <v>3</v>
       </c>
       <c r="R120" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="121" spans="1:18" x14ac:dyDescent="0.25">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="121" spans="1:18">
       <c r="A121">
         <v>65</v>
       </c>
@@ -7744,19 +7742,19 @@
         <v>0</v>
       </c>
       <c r="O121" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="P121" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="Q121">
         <v>5</v>
       </c>
       <c r="R121" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="122" spans="1:18" x14ac:dyDescent="0.25">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="122" spans="1:18">
       <c r="A122">
         <v>67</v>
       </c>
@@ -7800,19 +7798,19 @@
         <v>0</v>
       </c>
       <c r="O122" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="P122" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="Q122">
         <v>2</v>
       </c>
       <c r="R122" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="123" spans="1:18" x14ac:dyDescent="0.25">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="123" spans="1:18">
       <c r="A123">
         <v>68</v>
       </c>
@@ -7856,19 +7854,19 @@
         <v>0</v>
       </c>
       <c r="O123" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="P123" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="Q123">
         <v>4</v>
       </c>
       <c r="R123" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="124" spans="1:18" x14ac:dyDescent="0.25">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="124" spans="1:18">
       <c r="A124">
         <v>69</v>
       </c>
@@ -7912,19 +7910,19 @@
         <v>0</v>
       </c>
       <c r="O124" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="P124" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="Q124">
         <v>2</v>
       </c>
       <c r="R124" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="125" spans="1:18" x14ac:dyDescent="0.25">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="125" spans="1:18">
       <c r="A125">
         <v>124</v>
       </c>
@@ -7968,19 +7966,19 @@
         <v>0</v>
       </c>
       <c r="O125" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="P125" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="Q125">
         <v>2</v>
       </c>
       <c r="R125" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="126" spans="1:18" x14ac:dyDescent="0.25">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="126" spans="1:18">
       <c r="A126">
         <v>125</v>
       </c>
@@ -8024,19 +8022,19 @@
         <v>0</v>
       </c>
       <c r="O126" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="P126" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="Q126">
         <v>2</v>
       </c>
       <c r="R126" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="127" spans="1:18" x14ac:dyDescent="0.25">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="127" spans="1:18">
       <c r="A127">
         <v>127</v>
       </c>
@@ -8080,19 +8078,19 @@
         <v>0</v>
       </c>
       <c r="O127" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="P127" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="Q127">
         <v>1</v>
       </c>
       <c r="R127" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="128" spans="1:18" x14ac:dyDescent="0.25">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="128" spans="1:18">
       <c r="A128">
         <v>126</v>
       </c>
@@ -8136,19 +8134,19 @@
         <v>0</v>
       </c>
       <c r="O128" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="P128" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="Q128">
         <v>2</v>
       </c>
       <c r="R128" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="129" spans="1:18" x14ac:dyDescent="0.25">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="129" spans="1:18">
       <c r="A129">
         <v>128</v>
       </c>
@@ -8192,19 +8190,19 @@
         <v>0</v>
       </c>
       <c r="O129" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="P129" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="Q129">
         <v>1</v>
       </c>
       <c r="R129" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="130" spans="1:18" x14ac:dyDescent="0.25">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="130" spans="1:18">
       <c r="A130">
         <v>129</v>
       </c>
@@ -8248,19 +8246,19 @@
         <v>0</v>
       </c>
       <c r="O130" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="P130" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="Q130">
         <v>5</v>
       </c>
       <c r="R130" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="131" spans="1:18" x14ac:dyDescent="0.25">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="131" spans="1:18">
       <c r="A131">
         <v>130</v>
       </c>
@@ -8304,19 +8302,19 @@
         <v>0</v>
       </c>
       <c r="O131" t="s">
+        <v>17</v>
+      </c>
+      <c r="P131" t="s">
         <v>18</v>
-      </c>
-      <c r="P131" t="s">
-        <v>19</v>
       </c>
       <c r="Q131">
         <v>2</v>
       </c>
       <c r="R131" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="132" spans="1:18" x14ac:dyDescent="0.25">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="132" spans="1:18">
       <c r="A132">
         <v>131</v>
       </c>
@@ -8360,19 +8358,19 @@
         <v>0</v>
       </c>
       <c r="O132" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="P132" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="Q132">
         <v>3</v>
       </c>
       <c r="R132" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="133" spans="1:18" x14ac:dyDescent="0.25">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="133" spans="1:18">
       <c r="A133">
         <v>132</v>
       </c>
@@ -8416,19 +8414,19 @@
         <v>0</v>
       </c>
       <c r="O133" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="P133" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="Q133">
         <v>4</v>
       </c>
       <c r="R133" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="134" spans="1:18" x14ac:dyDescent="0.25">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="134" spans="1:18">
       <c r="A134">
         <v>133</v>
       </c>
@@ -8472,19 +8470,19 @@
         <v>0</v>
       </c>
       <c r="O134" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="P134" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="Q134">
         <v>4</v>
       </c>
       <c r="R134" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="135" spans="1:18" x14ac:dyDescent="0.25">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="135" spans="1:18">
       <c r="A135">
         <v>135</v>
       </c>
@@ -8528,19 +8526,19 @@
         <v>0</v>
       </c>
       <c r="O135" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="P135" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="Q135">
         <v>1</v>
       </c>
       <c r="R135" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="136" spans="1:18" x14ac:dyDescent="0.25">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="136" spans="1:18">
       <c r="A136">
         <v>134</v>
       </c>
@@ -8584,19 +8582,19 @@
         <v>0</v>
       </c>
       <c r="O136" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="P136" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="Q136">
         <v>3</v>
       </c>
       <c r="R136" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="137" spans="1:18" x14ac:dyDescent="0.25">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="137" spans="1:18">
       <c r="A137">
         <v>137</v>
       </c>
@@ -8640,19 +8638,19 @@
         <v>0</v>
       </c>
       <c r="O137" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="P137" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="Q137">
         <v>4</v>
       </c>
       <c r="R137" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="138" spans="1:18" x14ac:dyDescent="0.25">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="138" spans="1:18">
       <c r="A138">
         <v>136</v>
       </c>
@@ -8696,19 +8694,19 @@
         <v>0</v>
       </c>
       <c r="O138" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="P138" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="Q138">
         <v>2</v>
       </c>
       <c r="R138" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="139" spans="1:18" x14ac:dyDescent="0.25">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="139" spans="1:18">
       <c r="A139">
         <v>138</v>
       </c>
@@ -8752,19 +8750,19 @@
         <v>1</v>
       </c>
       <c r="O139" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="P139" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="Q139">
         <v>4</v>
       </c>
       <c r="R139" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="140" spans="1:18" x14ac:dyDescent="0.25">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="140" spans="1:18">
       <c r="A140">
         <v>139</v>
       </c>
@@ -8808,19 +8806,19 @@
         <v>0</v>
       </c>
       <c r="O140" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="P140" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="Q140">
         <v>2</v>
       </c>
       <c r="R140" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="141" spans="1:18" x14ac:dyDescent="0.25">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="141" spans="1:18">
       <c r="A141">
         <v>140</v>
       </c>
@@ -8864,19 +8862,19 @@
         <v>0</v>
       </c>
       <c r="O141" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="P141" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="Q141">
         <v>3</v>
       </c>
       <c r="R141" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="142" spans="1:18" x14ac:dyDescent="0.25">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="142" spans="1:18">
       <c r="A142">
         <v>141</v>
       </c>
@@ -8920,19 +8918,19 @@
         <v>0</v>
       </c>
       <c r="O142" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="P142" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="Q142">
         <v>3</v>
       </c>
       <c r="R142" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="143" spans="1:18" x14ac:dyDescent="0.25">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="143" spans="1:18">
       <c r="A143">
         <v>142</v>
       </c>
@@ -8976,19 +8974,19 @@
         <v>0</v>
       </c>
       <c r="O143" t="s">
+        <v>17</v>
+      </c>
+      <c r="P143" t="s">
         <v>18</v>
       </c>
-      <c r="P143" t="s">
-        <v>19</v>
-      </c>
       <c r="Q143">
         <v>1</v>
       </c>
       <c r="R143" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="144" spans="1:18" x14ac:dyDescent="0.25">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="144" spans="1:18">
       <c r="A144">
         <v>143</v>
       </c>
@@ -9032,19 +9030,19 @@
         <v>0</v>
       </c>
       <c r="O144" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="P144" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="Q144">
         <v>4</v>
       </c>
       <c r="R144" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="145" spans="1:18" x14ac:dyDescent="0.25">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="145" spans="1:18">
       <c r="A145">
         <v>144</v>
       </c>
@@ -9088,19 +9086,19 @@
         <v>0</v>
       </c>
       <c r="O145" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="P145" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="Q145">
         <v>1</v>
       </c>
       <c r="R145" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="146" spans="1:18" x14ac:dyDescent="0.25">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="146" spans="1:18">
       <c r="A146">
         <v>145</v>
       </c>
@@ -9144,19 +9142,19 @@
         <v>0</v>
       </c>
       <c r="O146" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="P146" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="Q146">
         <v>2</v>
       </c>
       <c r="R146" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="147" spans="1:18" x14ac:dyDescent="0.25">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="147" spans="1:18">
       <c r="A147">
         <v>146</v>
       </c>
@@ -9200,19 +9198,19 @@
         <v>0</v>
       </c>
       <c r="O147" t="s">
+        <v>17</v>
+      </c>
+      <c r="P147" t="s">
         <v>18</v>
-      </c>
-      <c r="P147" t="s">
-        <v>19</v>
       </c>
       <c r="Q147">
         <v>3</v>
       </c>
       <c r="R147" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="148" spans="1:18" x14ac:dyDescent="0.25">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="148" spans="1:18">
       <c r="A148">
         <v>147</v>
       </c>
@@ -9256,19 +9254,19 @@
         <v>0</v>
       </c>
       <c r="O148" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="P148" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="Q148">
         <v>5</v>
       </c>
       <c r="R148" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="149" spans="1:18" x14ac:dyDescent="0.25">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="149" spans="1:18">
       <c r="A149">
         <v>148</v>
       </c>
@@ -9312,19 +9310,19 @@
         <v>0</v>
       </c>
       <c r="O149" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="P149" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="Q149">
         <v>4</v>
       </c>
       <c r="R149" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="150" spans="1:18" x14ac:dyDescent="0.25">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="150" spans="1:18">
       <c r="A150">
         <v>150</v>
       </c>
@@ -9368,19 +9366,19 @@
         <v>0</v>
       </c>
       <c r="O150" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="P150" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="Q150">
         <v>4</v>
       </c>
       <c r="R150" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="151" spans="1:18" x14ac:dyDescent="0.25">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="151" spans="1:18">
       <c r="A151">
         <v>149</v>
       </c>
@@ -9424,19 +9422,19 @@
         <v>0</v>
       </c>
       <c r="O151" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="P151" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="Q151">
         <v>5</v>
       </c>
       <c r="R151" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="152" spans="1:18" x14ac:dyDescent="0.25">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="152" spans="1:18">
       <c r="A152">
         <v>152</v>
       </c>
@@ -9480,19 +9478,19 @@
         <v>0</v>
       </c>
       <c r="O152" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="P152" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="Q152">
         <v>2</v>
       </c>
       <c r="R152" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="153" spans="1:18" x14ac:dyDescent="0.25">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="153" spans="1:18">
       <c r="A153">
         <v>151</v>
       </c>
@@ -9536,19 +9534,19 @@
         <v>0</v>
       </c>
       <c r="O153" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="P153" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="Q153">
         <v>1</v>
       </c>
       <c r="R153" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="154" spans="1:18" x14ac:dyDescent="0.25">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="154" spans="1:18">
       <c r="A154">
         <v>153</v>
       </c>
@@ -9592,19 +9590,19 @@
         <v>0</v>
       </c>
       <c r="O154" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="P154" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="Q154">
         <v>1</v>
       </c>
       <c r="R154" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="155" spans="1:18" x14ac:dyDescent="0.25">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="155" spans="1:18">
       <c r="A155">
         <v>154</v>
       </c>
@@ -9648,19 +9646,19 @@
         <v>0</v>
       </c>
       <c r="O155" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="P155" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="Q155">
         <v>2</v>
       </c>
       <c r="R155" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="156" spans="1:18" x14ac:dyDescent="0.25">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="156" spans="1:18">
       <c r="A156">
         <v>156</v>
       </c>
@@ -9704,19 +9702,19 @@
         <v>0</v>
       </c>
       <c r="O156" t="s">
+        <v>17</v>
+      </c>
+      <c r="P156" t="s">
         <v>18</v>
       </c>
-      <c r="P156" t="s">
-        <v>19</v>
-      </c>
       <c r="Q156">
         <v>1</v>
       </c>
       <c r="R156" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="157" spans="1:18" x14ac:dyDescent="0.25">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="157" spans="1:18">
       <c r="A157">
         <v>155</v>
       </c>
@@ -9760,19 +9758,19 @@
         <v>0</v>
       </c>
       <c r="O157" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="P157" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="Q157">
         <v>2</v>
       </c>
       <c r="R157" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="158" spans="1:18" x14ac:dyDescent="0.25">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="158" spans="1:18">
       <c r="A158">
         <v>158</v>
       </c>
@@ -9816,19 +9814,19 @@
         <v>0</v>
       </c>
       <c r="O158" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="P158" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="Q158">
         <v>2</v>
       </c>
       <c r="R158" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="159" spans="1:18" x14ac:dyDescent="0.25">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="159" spans="1:18">
       <c r="A159">
         <v>157</v>
       </c>
@@ -9872,19 +9870,19 @@
         <v>0</v>
       </c>
       <c r="O159" t="s">
+        <v>17</v>
+      </c>
+      <c r="P159" t="s">
         <v>18</v>
-      </c>
-      <c r="P159" t="s">
-        <v>19</v>
       </c>
       <c r="Q159">
         <v>2</v>
       </c>
       <c r="R159" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="160" spans="1:18" x14ac:dyDescent="0.25">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="160" spans="1:18">
       <c r="A160">
         <v>159</v>
       </c>
@@ -9928,19 +9926,19 @@
         <v>0</v>
       </c>
       <c r="O160" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="P160" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="Q160">
         <v>2</v>
       </c>
       <c r="R160" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="161" spans="1:18" x14ac:dyDescent="0.25">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="161" spans="1:18">
       <c r="A161">
         <v>160</v>
       </c>
@@ -9984,19 +9982,19 @@
         <v>0</v>
       </c>
       <c r="O161" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="P161" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="Q161">
         <v>4</v>
       </c>
       <c r="R161" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="162" spans="1:18" x14ac:dyDescent="0.25">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="162" spans="1:18">
       <c r="A162">
         <v>161</v>
       </c>
@@ -10040,19 +10038,19 @@
         <v>0</v>
       </c>
       <c r="O162" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="P162" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="Q162">
         <v>4</v>
       </c>
       <c r="R162" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="163" spans="1:18" x14ac:dyDescent="0.25">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="163" spans="1:18">
       <c r="A163">
         <v>163</v>
       </c>
@@ -10096,19 +10094,19 @@
         <v>0</v>
       </c>
       <c r="O163" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="P163" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="Q163">
         <v>3</v>
       </c>
       <c r="R163" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="164" spans="1:18" x14ac:dyDescent="0.25">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="164" spans="1:18">
       <c r="A164">
         <v>162</v>
       </c>
@@ -10152,19 +10150,19 @@
         <v>0</v>
       </c>
       <c r="O164" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="P164" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="Q164">
         <v>5</v>
       </c>
       <c r="R164" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="165" spans="1:18" x14ac:dyDescent="0.25">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="165" spans="1:18">
       <c r="A165">
         <v>164</v>
       </c>
@@ -10208,21 +10206,21 @@
         <v>0</v>
       </c>
       <c r="O165" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="P165" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="Q165">
         <v>2</v>
       </c>
       <c r="R165" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="166" spans="1:18" x14ac:dyDescent="0.25">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="166" spans="1:18">
       <c r="A166" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B166">
         <v>1</v>
@@ -10264,21 +10262,21 @@
         <v>0</v>
       </c>
       <c r="O166" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="P166" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="Q166">
         <v>1</v>
       </c>
       <c r="R166" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="167" spans="1:18" x14ac:dyDescent="0.25">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="167" spans="1:18">
       <c r="A167" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B167">
         <v>1</v>
@@ -10320,22 +10318,22 @@
         <v>0</v>
       </c>
       <c r="O167" t="s">
+        <v>17</v>
+      </c>
+      <c r="P167" t="s">
         <v>18</v>
-      </c>
-      <c r="P167" t="s">
-        <v>19</v>
       </c>
       <c r="Q167">
         <v>3</v>
       </c>
       <c r="R167" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="168" spans="1:18">
+      <c r="A168" t="s">
         <v>203</v>
       </c>
-    </row>
-    <row r="168" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A168" t="s">
-        <v>204</v>
-      </c>
       <c r="B168">
         <v>0</v>
       </c>
@@ -10376,19 +10374,19 @@
         <v>0</v>
       </c>
       <c r="O168" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="P168" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="Q168">
         <v>3</v>
       </c>
       <c r="R168" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="169" spans="1:18" x14ac:dyDescent="0.25">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="169" spans="1:18">
       <c r="A169">
         <v>168</v>
       </c>
@@ -10432,19 +10430,19 @@
         <v>0</v>
       </c>
       <c r="O169" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="P169" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="Q169">
         <v>5</v>
       </c>
       <c r="R169" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="170" spans="1:18" x14ac:dyDescent="0.25">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="170" spans="1:18">
       <c r="A170">
         <v>169</v>
       </c>
@@ -10488,19 +10486,19 @@
         <v>0</v>
       </c>
       <c r="O170" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="P170" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="Q170">
         <v>4</v>
       </c>
       <c r="R170" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="171" spans="1:18" x14ac:dyDescent="0.25">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="171" spans="1:18">
       <c r="A171">
         <v>170</v>
       </c>
@@ -10544,19 +10542,19 @@
         <v>0</v>
       </c>
       <c r="O171" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="P171" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="Q171">
         <v>5</v>
       </c>
       <c r="R171" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="172" spans="1:18" x14ac:dyDescent="0.25">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="172" spans="1:18">
       <c r="A172">
         <v>171</v>
       </c>
@@ -10600,19 +10598,19 @@
         <v>0</v>
       </c>
       <c r="O172" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="P172" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="Q172">
         <v>3</v>
       </c>
       <c r="R172" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="173" spans="1:18" x14ac:dyDescent="0.25">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="173" spans="1:18">
       <c r="A173">
         <v>172</v>
       </c>
@@ -10656,19 +10654,19 @@
         <v>0</v>
       </c>
       <c r="O173" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="P173" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="Q173">
         <v>1</v>
       </c>
       <c r="R173" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="174" spans="1:18" x14ac:dyDescent="0.25">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="174" spans="1:18">
       <c r="A174">
         <v>173</v>
       </c>
@@ -10712,19 +10710,19 @@
         <v>0</v>
       </c>
       <c r="O174" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="P174" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="Q174">
         <v>2</v>
       </c>
       <c r="R174" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="175" spans="1:18" x14ac:dyDescent="0.25">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="175" spans="1:18">
       <c r="A175">
         <v>174</v>
       </c>
@@ -10768,19 +10766,19 @@
         <v>0</v>
       </c>
       <c r="O175" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="P175" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="Q175">
         <v>1</v>
       </c>
       <c r="R175" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="176" spans="1:18" x14ac:dyDescent="0.25">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="176" spans="1:18">
       <c r="A176">
         <v>175</v>
       </c>
@@ -10824,19 +10822,19 @@
         <v>0</v>
       </c>
       <c r="O176" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="P176" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="Q176">
         <v>3</v>
       </c>
       <c r="R176" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="177" spans="1:18" x14ac:dyDescent="0.25">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="177" spans="1:18">
       <c r="A177">
         <v>176</v>
       </c>
@@ -10880,19 +10878,19 @@
         <v>0</v>
       </c>
       <c r="O177" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="P177" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="Q177">
         <v>3</v>
       </c>
       <c r="R177" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="178" spans="1:18" x14ac:dyDescent="0.25">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="178" spans="1:18">
       <c r="A178">
         <v>177</v>
       </c>
@@ -10936,19 +10934,19 @@
         <v>0</v>
       </c>
       <c r="O178" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="P178" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="Q178">
         <v>4</v>
       </c>
       <c r="R178" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="179" spans="1:18" x14ac:dyDescent="0.25">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="179" spans="1:18">
       <c r="A179">
         <v>178</v>
       </c>
@@ -10992,19 +10990,19 @@
         <v>0</v>
       </c>
       <c r="O179" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="P179" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="Q179">
         <v>4</v>
       </c>
       <c r="R179" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="180" spans="1:18" x14ac:dyDescent="0.25">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="180" spans="1:18">
       <c r="A180">
         <v>180</v>
       </c>
@@ -11048,19 +11046,19 @@
         <v>0</v>
       </c>
       <c r="O180" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="P180" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="Q180">
         <v>2</v>
       </c>
       <c r="R180" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="181" spans="1:18" x14ac:dyDescent="0.25">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="181" spans="1:18">
       <c r="A181">
         <v>179</v>
       </c>
@@ -11104,19 +11102,19 @@
         <v>0</v>
       </c>
       <c r="O181" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="P181" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="Q181">
         <v>2</v>
       </c>
       <c r="R181" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="182" spans="1:18" x14ac:dyDescent="0.25">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="182" spans="1:18">
       <c r="A182">
         <v>182</v>
       </c>
@@ -11160,19 +11158,19 @@
         <v>0</v>
       </c>
       <c r="O182" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="P182" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="Q182">
         <v>3</v>
       </c>
       <c r="R182" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="183" spans="1:18" x14ac:dyDescent="0.25">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="183" spans="1:18">
       <c r="A183">
         <v>181</v>
       </c>
@@ -11216,16 +11214,16 @@
         <v>0</v>
       </c>
       <c r="O183" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="P183" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="Q183">
         <v>2</v>
       </c>
       <c r="R183" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
   </sheetData>
@@ -11234,24 +11232,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Lots of minor changes trying to enforce class in RA-coded datasheets.
</commit_message>
<xml_diff>
--- a/raw-data-prep/raw_data/Debrief_AM.xlsx
+++ b/raw-data-prep/raw_data/Debrief_AM.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
@@ -11,6 +11,9 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$R$183</definedName>
+  </definedNames>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
@@ -66,9 +69,6 @@
     <t>Suspected</t>
   </si>
   <si>
-    <t xml:space="preserve">Why </t>
-  </si>
-  <si>
     <t>Maybe</t>
   </si>
   <si>
@@ -634,13 +634,16 @@
   </si>
   <si>
     <t>Game.affect.distraction</t>
+  </si>
+  <si>
+    <t>Why_t</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -760,6 +763,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -794,6 +798,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -969,19 +974,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R183"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="R1" sqref="A1:R1"/>
+      <selection activeCell="R2" sqref="R2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="15" max="15" width="10.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1025,7 +1030,7 @@
         <v>13</v>
       </c>
       <c r="O1" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="P1" t="s">
         <v>14</v>
@@ -1034,10 +1039,10 @@
         <v>15</v>
       </c>
       <c r="R1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="2" spans="1:18">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>32</v>
       </c>
@@ -1081,19 +1086,19 @@
         <v>1</v>
       </c>
       <c r="O2" t="s">
+        <v>16</v>
+      </c>
+      <c r="P2" t="s">
         <v>17</v>
-      </c>
-      <c r="P2" t="s">
-        <v>18</v>
       </c>
       <c r="Q2">
         <v>2</v>
       </c>
       <c r="R2" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="3" spans="1:18">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>28</v>
       </c>
@@ -1137,19 +1142,19 @@
         <v>0</v>
       </c>
       <c r="O3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="P3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="Q3">
         <v>3</v>
       </c>
       <c r="R3" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="4" spans="1:18">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>23</v>
       </c>
@@ -1193,19 +1198,19 @@
         <v>0</v>
       </c>
       <c r="O4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="P4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="Q4">
         <v>2</v>
       </c>
       <c r="R4" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="5" spans="1:18">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>5</v>
       </c>
@@ -1249,19 +1254,19 @@
         <v>0</v>
       </c>
       <c r="O5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="P5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="Q5">
         <v>1</v>
       </c>
       <c r="R5" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="6" spans="1:18">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>6</v>
       </c>
@@ -1305,19 +1310,19 @@
         <v>0</v>
       </c>
       <c r="O6" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="P6" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="Q6">
         <v>1</v>
       </c>
       <c r="R6" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="7" spans="1:18">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>2</v>
       </c>
@@ -1361,19 +1366,19 @@
         <v>0</v>
       </c>
       <c r="O7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="P7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="Q7">
         <v>4</v>
       </c>
       <c r="R7" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="8" spans="1:18">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>1</v>
       </c>
@@ -1417,19 +1422,19 @@
         <v>0</v>
       </c>
       <c r="O8" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="P8" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="Q8">
         <v>3</v>
       </c>
       <c r="R8" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="9" spans="1:18">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>3</v>
       </c>
@@ -1473,19 +1478,19 @@
         <v>0</v>
       </c>
       <c r="O9" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="P9" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="Q9">
         <v>3</v>
       </c>
       <c r="R9" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="10" spans="1:18">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>4</v>
       </c>
@@ -1529,19 +1534,19 @@
         <v>0</v>
       </c>
       <c r="O10" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="P10" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="Q10">
         <v>3</v>
       </c>
       <c r="R10" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="11" spans="1:18">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>8</v>
       </c>
@@ -1585,19 +1590,19 @@
         <v>0</v>
       </c>
       <c r="O11" t="s">
+        <v>16</v>
+      </c>
+      <c r="P11" t="s">
         <v>17</v>
-      </c>
-      <c r="P11" t="s">
-        <v>18</v>
       </c>
       <c r="Q11">
         <v>3</v>
       </c>
       <c r="R11" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="12" spans="1:18">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>7</v>
       </c>
@@ -1641,19 +1646,19 @@
         <v>0</v>
       </c>
       <c r="O12" t="s">
+        <v>16</v>
+      </c>
+      <c r="P12" t="s">
         <v>17</v>
-      </c>
-      <c r="P12" t="s">
-        <v>18</v>
       </c>
       <c r="Q12">
         <v>3</v>
       </c>
       <c r="R12" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="13" spans="1:18">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>10</v>
       </c>
@@ -1697,19 +1702,19 @@
         <v>0</v>
       </c>
       <c r="O13" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="P13" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="Q13">
         <v>4</v>
       </c>
       <c r="R13" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="14" spans="1:18">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>9</v>
       </c>
@@ -1753,19 +1758,19 @@
         <v>0</v>
       </c>
       <c r="O14" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="P14" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="Q14">
         <v>4</v>
       </c>
       <c r="R14" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="15" spans="1:18">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>12</v>
       </c>
@@ -1809,19 +1814,19 @@
         <v>0</v>
       </c>
       <c r="O15" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="P15" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="Q15">
         <v>2</v>
       </c>
       <c r="R15" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="16" spans="1:18">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>11</v>
       </c>
@@ -1865,19 +1870,19 @@
         <v>0</v>
       </c>
       <c r="O16" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="P16" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="Q16">
         <v>2</v>
       </c>
       <c r="R16" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="17" spans="1:18">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="17" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>14</v>
       </c>
@@ -1921,19 +1926,19 @@
         <v>0</v>
       </c>
       <c r="O17" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="P17" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="Q17">
         <v>5</v>
       </c>
       <c r="R17" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="18" spans="1:18">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="18" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>13</v>
       </c>
@@ -1977,19 +1982,19 @@
         <v>1</v>
       </c>
       <c r="O18" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="P18" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="Q18">
         <v>2</v>
       </c>
       <c r="R18" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="19" spans="1:18">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="19" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>16</v>
       </c>
@@ -2033,19 +2038,19 @@
         <v>0</v>
       </c>
       <c r="O19" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="P19" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="Q19">
         <v>2</v>
       </c>
       <c r="R19" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="20" spans="1:18">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="20" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>18</v>
       </c>
@@ -2089,19 +2094,19 @@
         <v>0</v>
       </c>
       <c r="O20" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="P20" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="Q20">
         <v>4</v>
       </c>
       <c r="R20" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="21" spans="1:18">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="21" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>21</v>
       </c>
@@ -2145,19 +2150,19 @@
         <v>0</v>
       </c>
       <c r="O21" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="P21" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="Q21">
         <v>3</v>
       </c>
       <c r="R21" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="22" spans="1:18">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="22" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>17</v>
       </c>
@@ -2201,19 +2206,19 @@
         <v>0</v>
       </c>
       <c r="O22" t="s">
+        <v>16</v>
+      </c>
+      <c r="P22" t="s">
         <v>17</v>
-      </c>
-      <c r="P22" t="s">
-        <v>18</v>
       </c>
       <c r="Q22">
         <v>3</v>
       </c>
       <c r="R22" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="23" spans="1:18">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="23" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>19</v>
       </c>
@@ -2257,19 +2262,19 @@
         <v>0</v>
       </c>
       <c r="O23" t="s">
+        <v>16</v>
+      </c>
+      <c r="P23" t="s">
         <v>17</v>
-      </c>
-      <c r="P23" t="s">
-        <v>18</v>
       </c>
       <c r="Q23">
         <v>2</v>
       </c>
       <c r="R23" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="24" spans="1:18">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="24" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>20</v>
       </c>
@@ -2313,19 +2318,19 @@
         <v>1</v>
       </c>
       <c r="O24" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="P24" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="Q24">
         <v>5</v>
       </c>
       <c r="R24" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="25" spans="1:18">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="25" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>22</v>
       </c>
@@ -2369,19 +2374,19 @@
         <v>0</v>
       </c>
       <c r="O25" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="P25" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="Q25">
         <v>4</v>
       </c>
       <c r="R25" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="26" spans="1:18">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="26" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>15</v>
       </c>
@@ -2425,19 +2430,19 @@
         <v>0</v>
       </c>
       <c r="O26" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="P26" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="Q26">
         <v>4</v>
       </c>
       <c r="R26" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="27" spans="1:18">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="27" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>24</v>
       </c>
@@ -2481,19 +2486,19 @@
         <v>0</v>
       </c>
       <c r="O27" t="s">
+        <v>16</v>
+      </c>
+      <c r="P27" t="s">
         <v>17</v>
-      </c>
-      <c r="P27" t="s">
-        <v>18</v>
       </c>
       <c r="Q27">
         <v>3</v>
       </c>
       <c r="R27" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="28" spans="1:18">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="28" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>26</v>
       </c>
@@ -2537,19 +2542,19 @@
         <v>0</v>
       </c>
       <c r="O28" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="P28" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="Q28">
         <v>1</v>
       </c>
       <c r="R28" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="29" spans="1:18">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="29" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>25</v>
       </c>
@@ -2593,19 +2598,19 @@
         <v>0</v>
       </c>
       <c r="O29" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="P29" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="Q29">
         <v>1</v>
       </c>
       <c r="R29" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="30" spans="1:18">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="30" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>27</v>
       </c>
@@ -2649,19 +2654,19 @@
         <v>0</v>
       </c>
       <c r="O30" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="P30" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="Q30">
         <v>3</v>
       </c>
       <c r="R30" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="31" spans="1:18">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="31" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>31</v>
       </c>
@@ -2705,19 +2710,19 @@
         <v>0</v>
       </c>
       <c r="O31" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="P31" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="Q31">
         <v>2</v>
       </c>
       <c r="R31" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="32" spans="1:18">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="32" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>29</v>
       </c>
@@ -2761,19 +2766,19 @@
         <v>0</v>
       </c>
       <c r="O32" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="P32" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="Q32">
         <v>4</v>
       </c>
       <c r="R32" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="33" spans="1:18">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="33" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>30</v>
       </c>
@@ -2817,19 +2822,19 @@
         <v>0</v>
       </c>
       <c r="O33" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="P33" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="Q33">
         <v>2</v>
       </c>
       <c r="R33" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="34" spans="1:18">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="34" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>34</v>
       </c>
@@ -2873,19 +2878,19 @@
         <v>0</v>
       </c>
       <c r="O34" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="P34" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="Q34">
         <v>1</v>
       </c>
       <c r="R34" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="35" spans="1:18">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="35" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>33</v>
       </c>
@@ -2929,19 +2934,19 @@
         <v>0</v>
       </c>
       <c r="O35" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="P35" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="Q35">
         <v>3</v>
       </c>
       <c r="R35" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="36" spans="1:18">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="36" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>36</v>
       </c>
@@ -2985,19 +2990,19 @@
         <v>0</v>
       </c>
       <c r="O36" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="P36" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="Q36">
         <v>2</v>
       </c>
       <c r="R36" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="37" spans="1:18">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="37" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>35</v>
       </c>
@@ -3041,19 +3046,19 @@
         <v>0</v>
       </c>
       <c r="O37" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="P37" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="Q37">
         <v>3</v>
       </c>
       <c r="R37" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="38" spans="1:18">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="38" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>38</v>
       </c>
@@ -3097,19 +3102,19 @@
         <v>0</v>
       </c>
       <c r="O38" t="s">
+        <v>16</v>
+      </c>
+      <c r="P38" t="s">
         <v>17</v>
-      </c>
-      <c r="P38" t="s">
-        <v>18</v>
       </c>
       <c r="Q38">
         <v>4</v>
       </c>
       <c r="R38" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="39" spans="1:18">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="39" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>37</v>
       </c>
@@ -3153,19 +3158,19 @@
         <v>0</v>
       </c>
       <c r="O39" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="P39" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="Q39">
         <v>4</v>
       </c>
       <c r="R39" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="40" spans="1:18">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="40" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>40</v>
       </c>
@@ -3209,19 +3214,19 @@
         <v>0</v>
       </c>
       <c r="O40" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="P40" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="Q40">
         <v>2</v>
       </c>
       <c r="R40" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="41" spans="1:18">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="41" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>39</v>
       </c>
@@ -3265,19 +3270,19 @@
         <v>0</v>
       </c>
       <c r="O41" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="P41" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="Q41">
         <v>1</v>
       </c>
       <c r="R41" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="42" spans="1:18">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="42" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>41</v>
       </c>
@@ -3321,19 +3326,19 @@
         <v>0</v>
       </c>
       <c r="O42" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="P42" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="Q42">
         <v>5</v>
       </c>
       <c r="R42" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="43" spans="1:18">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="43" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>42</v>
       </c>
@@ -3377,19 +3382,19 @@
         <v>0</v>
       </c>
       <c r="O43" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="P43" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="Q43">
         <v>3</v>
       </c>
       <c r="R43" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="44" spans="1:18">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="44" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>43</v>
       </c>
@@ -3433,19 +3438,19 @@
         <v>0</v>
       </c>
       <c r="O44" t="s">
+        <v>16</v>
+      </c>
+      <c r="P44" t="s">
         <v>17</v>
-      </c>
-      <c r="P44" t="s">
-        <v>18</v>
       </c>
       <c r="Q44">
         <v>4</v>
       </c>
       <c r="R44" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="45" spans="1:18">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="45" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>80</v>
       </c>
@@ -3489,19 +3494,19 @@
         <v>0</v>
       </c>
       <c r="O45" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="P45" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="Q45">
         <v>5</v>
       </c>
       <c r="R45" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="46" spans="1:18">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="46" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>81</v>
       </c>
@@ -3545,19 +3550,19 @@
         <v>0</v>
       </c>
       <c r="O46" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="P46" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="Q46">
         <v>4</v>
       </c>
       <c r="R46" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="47" spans="1:18">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="47" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>82</v>
       </c>
@@ -3601,19 +3606,19 @@
         <v>0</v>
       </c>
       <c r="O47" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="P47" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="Q47">
         <v>4</v>
       </c>
       <c r="R47" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="48" spans="1:18">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="48" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>83</v>
       </c>
@@ -3657,19 +3662,19 @@
         <v>0</v>
       </c>
       <c r="O48" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="P48" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="Q48">
         <v>4</v>
       </c>
       <c r="R48" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="49" spans="1:18">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="49" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>84</v>
       </c>
@@ -3713,19 +3718,19 @@
         <v>0</v>
       </c>
       <c r="O49" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="P49" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="Q49">
         <v>2</v>
       </c>
       <c r="R49" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="50" spans="1:18">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="50" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>85</v>
       </c>
@@ -3769,19 +3774,19 @@
         <v>0</v>
       </c>
       <c r="O50" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="P50" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="Q50">
         <v>4</v>
       </c>
       <c r="R50" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="51" spans="1:18">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="51" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>86</v>
       </c>
@@ -3825,19 +3830,19 @@
         <v>0</v>
       </c>
       <c r="O51" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="P51" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="Q51">
         <v>2</v>
       </c>
       <c r="R51" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="52" spans="1:18">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="52" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>87</v>
       </c>
@@ -3881,19 +3886,19 @@
         <v>0</v>
       </c>
       <c r="O52" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="P52" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="Q52">
         <v>2</v>
       </c>
       <c r="R52" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="53" spans="1:18">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="53" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>71</v>
       </c>
@@ -3937,19 +3942,19 @@
         <v>0</v>
       </c>
       <c r="O53" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="P53" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="Q53">
         <v>3</v>
       </c>
       <c r="R53" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="54" spans="1:18">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="54" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>73</v>
       </c>
@@ -3993,19 +3998,19 @@
         <v>0</v>
       </c>
       <c r="O54" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="P54" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="Q54">
         <v>2</v>
       </c>
       <c r="R54" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="55" spans="1:18">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="55" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>72</v>
       </c>
@@ -4049,19 +4054,19 @@
         <v>1</v>
       </c>
       <c r="O55" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="P55" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="Q55">
         <v>2</v>
       </c>
       <c r="R55" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="56" spans="1:18">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="56" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>74</v>
       </c>
@@ -4102,19 +4107,19 @@
         <v>0</v>
       </c>
       <c r="O56" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="P56" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="Q56">
         <v>4</v>
       </c>
       <c r="R56" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="57" spans="1:18">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="57" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>75</v>
       </c>
@@ -4158,19 +4163,19 @@
         <v>0</v>
       </c>
       <c r="O57" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="P57" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="Q57">
         <v>4</v>
       </c>
       <c r="R57" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="58" spans="1:18">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="58" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>76</v>
       </c>
@@ -4214,19 +4219,19 @@
         <v>0</v>
       </c>
       <c r="O58" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="P58" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="Q58">
         <v>4</v>
       </c>
       <c r="R58" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="59" spans="1:18">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="59" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>77</v>
       </c>
@@ -4270,19 +4275,19 @@
         <v>0</v>
       </c>
       <c r="O59" t="s">
+        <v>16</v>
+      </c>
+      <c r="P59" t="s">
         <v>17</v>
       </c>
-      <c r="P59" t="s">
-        <v>18</v>
-      </c>
       <c r="Q59">
         <v>1</v>
       </c>
       <c r="R59" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="60" spans="1:18">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="60" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>78</v>
       </c>
@@ -4326,19 +4331,19 @@
         <v>0</v>
       </c>
       <c r="O60" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="P60" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="Q60">
         <v>5</v>
       </c>
       <c r="R60" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="61" spans="1:18">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="61" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>79</v>
       </c>
@@ -4382,19 +4387,19 @@
         <v>0</v>
       </c>
       <c r="O61" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="P61" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="Q61">
         <v>4</v>
       </c>
       <c r="R61" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="62" spans="1:18">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="62" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A62">
         <v>88</v>
       </c>
@@ -4438,19 +4443,19 @@
         <v>0</v>
       </c>
       <c r="O62" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="P62" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="Q62">
         <v>3</v>
       </c>
       <c r="R62" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="63" spans="1:18">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="63" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A63">
         <v>90</v>
       </c>
@@ -4494,19 +4499,19 @@
         <v>0</v>
       </c>
       <c r="O63" t="s">
+        <v>16</v>
+      </c>
+      <c r="P63" t="s">
         <v>17</v>
-      </c>
-      <c r="P63" t="s">
-        <v>18</v>
       </c>
       <c r="Q63">
         <v>2</v>
       </c>
       <c r="R63" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="64" spans="1:18">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="64" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A64">
         <v>89</v>
       </c>
@@ -4550,19 +4555,19 @@
         <v>0</v>
       </c>
       <c r="O64" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="P64" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="Q64">
         <v>5</v>
       </c>
       <c r="R64" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="65" spans="1:18">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="65" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A65">
         <v>92</v>
       </c>
@@ -4606,19 +4611,19 @@
         <v>0</v>
       </c>
       <c r="O65" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="P65" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="Q65">
         <v>3</v>
       </c>
       <c r="R65" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="66" spans="1:18">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="66" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A66">
         <v>91</v>
       </c>
@@ -4662,19 +4667,19 @@
         <v>0</v>
       </c>
       <c r="O66" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="P66" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="Q66">
         <v>2</v>
       </c>
       <c r="R66" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="67" spans="1:18">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="67" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A67">
         <v>94</v>
       </c>
@@ -4718,19 +4723,19 @@
         <v>0</v>
       </c>
       <c r="O67" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="P67" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="Q67">
         <v>4</v>
       </c>
       <c r="R67" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="68" spans="1:18">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="68" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A68">
         <v>96</v>
       </c>
@@ -4774,19 +4779,19 @@
         <v>0</v>
       </c>
       <c r="O68" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="P68" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="Q68">
         <v>3</v>
       </c>
       <c r="R68" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="69" spans="1:18">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="69" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A69">
         <v>95</v>
       </c>
@@ -4830,19 +4835,19 @@
         <v>0</v>
       </c>
       <c r="O69" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="P69" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="Q69">
         <v>1</v>
       </c>
       <c r="R69" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="70" spans="1:18">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="70" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A70">
         <v>98</v>
       </c>
@@ -4886,19 +4891,19 @@
         <v>0</v>
       </c>
       <c r="O70" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="P70" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="Q70">
         <v>4</v>
       </c>
       <c r="R70" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="71" spans="1:18">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="71" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A71">
         <v>97</v>
       </c>
@@ -4942,19 +4947,19 @@
         <v>0</v>
       </c>
       <c r="O71" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="P71" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="Q71">
         <v>1</v>
       </c>
       <c r="R71" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="72" spans="1:18">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="72" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A72">
         <v>99</v>
       </c>
@@ -4998,19 +5003,19 @@
         <v>0</v>
       </c>
       <c r="O72" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="P72" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="Q72">
         <v>2</v>
       </c>
       <c r="R72" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="73" spans="1:18">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="73" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A73">
         <v>100</v>
       </c>
@@ -5054,19 +5059,19 @@
         <v>0</v>
       </c>
       <c r="O73" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="P73" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="Q73">
         <v>5</v>
       </c>
       <c r="R73" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="74" spans="1:18">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="74" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A74">
         <v>102</v>
       </c>
@@ -5110,19 +5115,19 @@
         <v>0</v>
       </c>
       <c r="O74" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="P74" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="Q74">
         <v>2</v>
       </c>
       <c r="R74" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="75" spans="1:18">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="75" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A75">
         <v>101</v>
       </c>
@@ -5166,19 +5171,19 @@
         <v>0</v>
       </c>
       <c r="O75" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="P75" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="Q75">
         <v>4</v>
       </c>
       <c r="R75" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="76" spans="1:18">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="76" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A76">
         <v>52</v>
       </c>
@@ -5222,19 +5227,19 @@
         <v>0</v>
       </c>
       <c r="O76" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="P76" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="Q76">
         <v>3</v>
       </c>
       <c r="R76" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="77" spans="1:18">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="77" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A77">
         <v>104</v>
       </c>
@@ -5278,19 +5283,19 @@
         <v>0</v>
       </c>
       <c r="O77" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="P77" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="Q77">
         <v>4</v>
       </c>
       <c r="R77" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="78" spans="1:18">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="78" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A78">
         <v>103</v>
       </c>
@@ -5334,19 +5339,19 @@
         <v>0</v>
       </c>
       <c r="O78" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="P78" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="Q78">
         <v>2</v>
       </c>
       <c r="R78" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="79" spans="1:18">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="79" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A79">
         <v>106</v>
       </c>
@@ -5390,19 +5395,19 @@
         <v>0</v>
       </c>
       <c r="O79" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="P79" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="Q79">
         <v>4</v>
       </c>
       <c r="R79" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="80" spans="1:18">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="80" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A80">
         <v>105</v>
       </c>
@@ -5446,19 +5451,19 @@
         <v>0</v>
       </c>
       <c r="O80" t="s">
+        <v>16</v>
+      </c>
+      <c r="P80" t="s">
         <v>17</v>
-      </c>
-      <c r="P80" t="s">
-        <v>18</v>
       </c>
       <c r="Q80">
         <v>2</v>
       </c>
       <c r="R80" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="81" spans="1:18">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="81" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A81">
         <v>107</v>
       </c>
@@ -5502,19 +5507,19 @@
         <v>0</v>
       </c>
       <c r="O81" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="P81" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="Q81">
         <v>2</v>
       </c>
       <c r="R81" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="82" spans="1:18">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="82" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A82">
         <v>108</v>
       </c>
@@ -5558,19 +5563,19 @@
         <v>0</v>
       </c>
       <c r="O82" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="P82" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="Q82">
         <v>3</v>
       </c>
       <c r="R82" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="83" spans="1:18">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="83" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A83">
         <v>109</v>
       </c>
@@ -5614,19 +5619,19 @@
         <v>0</v>
       </c>
       <c r="O83" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="P83" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="Q83">
         <v>2</v>
       </c>
       <c r="R83" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="84" spans="1:18">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="84" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A84">
         <v>110</v>
       </c>
@@ -5670,19 +5675,19 @@
         <v>0</v>
       </c>
       <c r="O84" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="P84" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="Q84">
         <v>2</v>
       </c>
       <c r="R84" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="85" spans="1:18">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="85" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A85">
         <v>111</v>
       </c>
@@ -5726,19 +5731,19 @@
         <v>0</v>
       </c>
       <c r="O85" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="P85" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="Q85">
         <v>1</v>
       </c>
       <c r="R85" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="86" spans="1:18">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="86" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A86">
         <v>112</v>
       </c>
@@ -5782,19 +5787,19 @@
         <v>0</v>
       </c>
       <c r="O86" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="P86" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="Q86">
         <v>3</v>
       </c>
       <c r="R86" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="87" spans="1:18">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="87" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A87">
         <v>113</v>
       </c>
@@ -5838,19 +5843,19 @@
         <v>0</v>
       </c>
       <c r="O87" t="s">
+        <v>16</v>
+      </c>
+      <c r="P87" t="s">
         <v>17</v>
-      </c>
-      <c r="P87" t="s">
-        <v>18</v>
       </c>
       <c r="Q87">
         <v>2</v>
       </c>
       <c r="R87" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="88" spans="1:18">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="88" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A88">
         <v>114</v>
       </c>
@@ -5894,19 +5899,19 @@
         <v>0</v>
       </c>
       <c r="O88" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="P88" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="Q88">
         <v>4</v>
       </c>
       <c r="R88" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="89" spans="1:18">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="89" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A89">
         <v>115</v>
       </c>
@@ -5950,19 +5955,19 @@
         <v>0</v>
       </c>
       <c r="O89" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="P89" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="Q89">
         <v>4</v>
       </c>
       <c r="R89" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="90" spans="1:18">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="90" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A90">
         <v>116</v>
       </c>
@@ -6006,19 +6011,19 @@
         <v>0</v>
       </c>
       <c r="O90" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="P90" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="Q90">
         <v>2</v>
       </c>
       <c r="R90" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="91" spans="1:18">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="91" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A91">
         <v>117</v>
       </c>
@@ -6062,19 +6067,19 @@
         <v>0</v>
       </c>
       <c r="O91" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="P91" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="Q91">
         <v>5</v>
       </c>
       <c r="R91" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="92" spans="1:18">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="92" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A92">
         <v>119</v>
       </c>
@@ -6118,19 +6123,19 @@
         <v>0</v>
       </c>
       <c r="O92" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="P92" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="Q92">
         <v>4</v>
       </c>
       <c r="R92" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="93" spans="1:18">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="93" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A93">
         <v>118</v>
       </c>
@@ -6174,19 +6179,19 @@
         <v>0</v>
       </c>
       <c r="O93" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="P93" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="Q93">
         <v>2</v>
       </c>
       <c r="R93" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="94" spans="1:18">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="94" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A94">
         <v>120</v>
       </c>
@@ -6230,19 +6235,19 @@
         <v>0</v>
       </c>
       <c r="O94" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="P94" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="Q94">
         <v>2</v>
       </c>
       <c r="R94" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="95" spans="1:18">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="95" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A95">
         <v>121</v>
       </c>
@@ -6286,19 +6291,19 @@
         <v>0</v>
       </c>
       <c r="O95" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="P95" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="Q95">
         <v>1</v>
       </c>
       <c r="R95" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="96" spans="1:18">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="96" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A96">
         <v>122</v>
       </c>
@@ -6342,19 +6347,19 @@
         <v>0</v>
       </c>
       <c r="O96" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="P96" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="Q96">
         <v>4</v>
       </c>
       <c r="R96" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="97" spans="1:18">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="97" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A97">
         <v>123</v>
       </c>
@@ -6398,19 +6403,19 @@
         <v>0</v>
       </c>
       <c r="O97" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="P97" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="Q97">
         <v>2</v>
       </c>
       <c r="R97" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="98" spans="1:18">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="98" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A98">
         <v>64</v>
       </c>
@@ -6454,19 +6459,19 @@
         <v>0</v>
       </c>
       <c r="O98" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="P98" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="Q98">
         <v>1</v>
       </c>
       <c r="R98" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="99" spans="1:18">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="99" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A99">
         <v>63</v>
       </c>
@@ -6510,19 +6515,19 @@
         <v>0</v>
       </c>
       <c r="O99" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="P99" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="Q99">
         <v>4</v>
       </c>
       <c r="R99" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="100" spans="1:18">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="100" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A100">
         <v>62</v>
       </c>
@@ -6566,19 +6571,19 @@
         <v>0</v>
       </c>
       <c r="O100" t="s">
+        <v>16</v>
+      </c>
+      <c r="P100" t="s">
         <v>17</v>
-      </c>
-      <c r="P100" t="s">
-        <v>18</v>
       </c>
       <c r="Q100">
         <v>2</v>
       </c>
       <c r="R100" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="101" spans="1:18">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="101" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A101">
         <v>61</v>
       </c>
@@ -6622,19 +6627,19 @@
         <v>0</v>
       </c>
       <c r="O101" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="P101" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="Q101">
         <v>2</v>
       </c>
       <c r="R101" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="102" spans="1:18">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="102" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A102">
         <v>60</v>
       </c>
@@ -6678,19 +6683,19 @@
         <v>0</v>
       </c>
       <c r="O102" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="P102" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="Q102">
         <v>1</v>
       </c>
       <c r="R102" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="103" spans="1:18">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="103" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A103">
         <v>58</v>
       </c>
@@ -6734,19 +6739,19 @@
         <v>0</v>
       </c>
       <c r="O103" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="P103" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="Q103">
         <v>1</v>
       </c>
       <c r="R103" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="104" spans="1:18">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="104" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A104">
         <v>57</v>
       </c>
@@ -6790,19 +6795,19 @@
         <v>0</v>
       </c>
       <c r="O104" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="P104" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="Q104">
         <v>3</v>
       </c>
       <c r="R104" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="105" spans="1:18">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="105" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A105">
         <v>59</v>
       </c>
@@ -6846,19 +6851,19 @@
         <v>0</v>
       </c>
       <c r="O105" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="P105" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="Q105">
         <v>2</v>
       </c>
       <c r="R105" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="106" spans="1:18">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="106" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A106">
         <v>56</v>
       </c>
@@ -6902,19 +6907,19 @@
         <v>0</v>
       </c>
       <c r="O106" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="P106" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="Q106">
         <v>2</v>
       </c>
       <c r="R106" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="107" spans="1:18">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="107" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A107">
         <v>55</v>
       </c>
@@ -6958,19 +6963,19 @@
         <v>0</v>
       </c>
       <c r="O107" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="P107" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="Q107">
         <v>3</v>
       </c>
       <c r="R107" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="108" spans="1:18">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="108" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A108">
         <v>54</v>
       </c>
@@ -7014,19 +7019,19 @@
         <v>0</v>
       </c>
       <c r="O108" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="P108" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="Q108">
         <v>3</v>
       </c>
       <c r="R108" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="109" spans="1:18">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="109" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A109">
         <v>53</v>
       </c>
@@ -7070,19 +7075,19 @@
         <v>0</v>
       </c>
       <c r="O109" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="P109" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="Q109">
         <v>3</v>
       </c>
       <c r="R109" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="110" spans="1:18">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="110" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A110">
         <v>50</v>
       </c>
@@ -7126,19 +7131,19 @@
         <v>0</v>
       </c>
       <c r="O110" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="P110" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="Q110">
         <v>2</v>
       </c>
       <c r="R110" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="111" spans="1:18">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="111" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A111">
         <v>51</v>
       </c>
@@ -7182,19 +7187,19 @@
         <v>0</v>
       </c>
       <c r="O111" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="P111" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="Q111">
         <v>2</v>
       </c>
       <c r="R111" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="112" spans="1:18">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="112" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A112">
         <v>48</v>
       </c>
@@ -7238,19 +7243,19 @@
         <v>0</v>
       </c>
       <c r="O112" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="P112" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="Q112">
         <v>5</v>
       </c>
       <c r="R112" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="113" spans="1:18">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="113" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A113">
         <v>49</v>
       </c>
@@ -7294,19 +7299,19 @@
         <v>0</v>
       </c>
       <c r="O113" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="P113" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="Q113">
         <v>2</v>
       </c>
       <c r="R113" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="114" spans="1:18">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="114" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A114">
         <v>46</v>
       </c>
@@ -7350,19 +7355,19 @@
         <v>0</v>
       </c>
       <c r="O114" t="s">
+        <v>16</v>
+      </c>
+      <c r="P114" t="s">
         <v>17</v>
-      </c>
-      <c r="P114" t="s">
-        <v>18</v>
       </c>
       <c r="Q114">
         <v>4</v>
       </c>
       <c r="R114" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="115" spans="1:18">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="115" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A115">
         <v>47</v>
       </c>
@@ -7406,19 +7411,19 @@
         <v>0</v>
       </c>
       <c r="O115" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="P115" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="Q115">
         <v>2</v>
       </c>
       <c r="R115" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="116" spans="1:18">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="116" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A116">
         <v>44</v>
       </c>
@@ -7462,19 +7467,19 @@
         <v>0</v>
       </c>
       <c r="O116" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="P116" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="Q116">
         <v>3</v>
       </c>
       <c r="R116" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="117" spans="1:18">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="117" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A117">
         <v>45</v>
       </c>
@@ -7518,19 +7523,19 @@
         <v>0</v>
       </c>
       <c r="O117" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="P117" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="Q117">
         <v>2</v>
       </c>
       <c r="R117" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="118" spans="1:18">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="118" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A118">
         <v>93</v>
       </c>
@@ -7574,19 +7579,19 @@
         <v>0</v>
       </c>
       <c r="O118" t="s">
+        <v>16</v>
+      </c>
+      <c r="P118" t="s">
         <v>17</v>
-      </c>
-      <c r="P118" t="s">
-        <v>18</v>
       </c>
       <c r="Q118">
         <v>4</v>
       </c>
       <c r="R118" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="119" spans="1:18">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="119" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A119">
         <v>70</v>
       </c>
@@ -7630,19 +7635,19 @@
         <v>1</v>
       </c>
       <c r="O119" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="P119" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="Q119">
         <v>3</v>
       </c>
       <c r="R119" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="120" spans="1:18">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="120" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A120">
         <v>66</v>
       </c>
@@ -7686,19 +7691,19 @@
         <v>0</v>
       </c>
       <c r="O120" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="P120" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="Q120">
         <v>3</v>
       </c>
       <c r="R120" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="121" spans="1:18">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="121" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A121">
         <v>65</v>
       </c>
@@ -7742,19 +7747,19 @@
         <v>0</v>
       </c>
       <c r="O121" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="P121" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="Q121">
         <v>5</v>
       </c>
       <c r="R121" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="122" spans="1:18">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="122" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A122">
         <v>67</v>
       </c>
@@ -7798,19 +7803,19 @@
         <v>0</v>
       </c>
       <c r="O122" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="P122" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="Q122">
         <v>2</v>
       </c>
       <c r="R122" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="123" spans="1:18">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="123" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A123">
         <v>68</v>
       </c>
@@ -7854,19 +7859,19 @@
         <v>0</v>
       </c>
       <c r="O123" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="P123" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="Q123">
         <v>4</v>
       </c>
       <c r="R123" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="124" spans="1:18">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="124" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A124">
         <v>69</v>
       </c>
@@ -7910,19 +7915,19 @@
         <v>0</v>
       </c>
       <c r="O124" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="P124" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="Q124">
         <v>2</v>
       </c>
       <c r="R124" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="125" spans="1:18">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="125" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A125">
         <v>124</v>
       </c>
@@ -7966,19 +7971,19 @@
         <v>0</v>
       </c>
       <c r="O125" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="P125" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="Q125">
         <v>2</v>
       </c>
       <c r="R125" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="126" spans="1:18">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="126" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A126">
         <v>125</v>
       </c>
@@ -8022,19 +8027,19 @@
         <v>0</v>
       </c>
       <c r="O126" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="P126" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="Q126">
         <v>2</v>
       </c>
       <c r="R126" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="127" spans="1:18">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="127" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A127">
         <v>127</v>
       </c>
@@ -8078,19 +8083,19 @@
         <v>0</v>
       </c>
       <c r="O127" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="P127" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="Q127">
         <v>1</v>
       </c>
       <c r="R127" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="128" spans="1:18">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="128" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A128">
         <v>126</v>
       </c>
@@ -8134,19 +8139,19 @@
         <v>0</v>
       </c>
       <c r="O128" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="P128" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="Q128">
         <v>2</v>
       </c>
       <c r="R128" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="129" spans="1:18">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="129" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A129">
         <v>128</v>
       </c>
@@ -8190,19 +8195,19 @@
         <v>0</v>
       </c>
       <c r="O129" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="P129" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="Q129">
         <v>1</v>
       </c>
       <c r="R129" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="130" spans="1:18">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="130" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A130">
         <v>129</v>
       </c>
@@ -8246,19 +8251,19 @@
         <v>0</v>
       </c>
       <c r="O130" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="P130" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="Q130">
         <v>5</v>
       </c>
       <c r="R130" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="131" spans="1:18">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="131" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A131">
         <v>130</v>
       </c>
@@ -8302,19 +8307,19 @@
         <v>0</v>
       </c>
       <c r="O131" t="s">
+        <v>16</v>
+      </c>
+      <c r="P131" t="s">
         <v>17</v>
-      </c>
-      <c r="P131" t="s">
-        <v>18</v>
       </c>
       <c r="Q131">
         <v>2</v>
       </c>
       <c r="R131" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="132" spans="1:18">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="132" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A132">
         <v>131</v>
       </c>
@@ -8358,19 +8363,19 @@
         <v>0</v>
       </c>
       <c r="O132" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="P132" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="Q132">
         <v>3</v>
       </c>
       <c r="R132" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="133" spans="1:18">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="133" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A133">
         <v>132</v>
       </c>
@@ -8414,19 +8419,19 @@
         <v>0</v>
       </c>
       <c r="O133" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="P133" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="Q133">
         <v>4</v>
       </c>
       <c r="R133" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="134" spans="1:18">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="134" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A134">
         <v>133</v>
       </c>
@@ -8470,19 +8475,19 @@
         <v>0</v>
       </c>
       <c r="O134" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="P134" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="Q134">
         <v>4</v>
       </c>
       <c r="R134" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="135" spans="1:18">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="135" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A135">
         <v>135</v>
       </c>
@@ -8526,19 +8531,19 @@
         <v>0</v>
       </c>
       <c r="O135" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="P135" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="Q135">
         <v>1</v>
       </c>
       <c r="R135" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="136" spans="1:18">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="136" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A136">
         <v>134</v>
       </c>
@@ -8582,19 +8587,19 @@
         <v>0</v>
       </c>
       <c r="O136" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="P136" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="Q136">
         <v>3</v>
       </c>
       <c r="R136" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="137" spans="1:18">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="137" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A137">
         <v>137</v>
       </c>
@@ -8638,19 +8643,19 @@
         <v>0</v>
       </c>
       <c r="O137" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="P137" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="Q137">
         <v>4</v>
       </c>
       <c r="R137" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="138" spans="1:18">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="138" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A138">
         <v>136</v>
       </c>
@@ -8694,19 +8699,19 @@
         <v>0</v>
       </c>
       <c r="O138" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="P138" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="Q138">
         <v>2</v>
       </c>
       <c r="R138" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="139" spans="1:18">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="139" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A139">
         <v>138</v>
       </c>
@@ -8750,19 +8755,19 @@
         <v>1</v>
       </c>
       <c r="O139" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="P139" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="Q139">
         <v>4</v>
       </c>
       <c r="R139" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="140" spans="1:18">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="140" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A140">
         <v>139</v>
       </c>
@@ -8806,19 +8811,19 @@
         <v>0</v>
       </c>
       <c r="O140" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="P140" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="Q140">
         <v>2</v>
       </c>
       <c r="R140" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="141" spans="1:18">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="141" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A141">
         <v>140</v>
       </c>
@@ -8862,19 +8867,19 @@
         <v>0</v>
       </c>
       <c r="O141" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="P141" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="Q141">
         <v>3</v>
       </c>
       <c r="R141" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="142" spans="1:18">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="142" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A142">
         <v>141</v>
       </c>
@@ -8918,19 +8923,19 @@
         <v>0</v>
       </c>
       <c r="O142" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="P142" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="Q142">
         <v>3</v>
       </c>
       <c r="R142" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="143" spans="1:18">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="143" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A143">
         <v>142</v>
       </c>
@@ -8974,19 +8979,19 @@
         <v>0</v>
       </c>
       <c r="O143" t="s">
+        <v>16</v>
+      </c>
+      <c r="P143" t="s">
         <v>17</v>
       </c>
-      <c r="P143" t="s">
-        <v>18</v>
-      </c>
       <c r="Q143">
         <v>1</v>
       </c>
       <c r="R143" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="144" spans="1:18">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="144" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A144">
         <v>143</v>
       </c>
@@ -9030,19 +9035,19 @@
         <v>0</v>
       </c>
       <c r="O144" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="P144" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="Q144">
         <v>4</v>
       </c>
       <c r="R144" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="145" spans="1:18">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="145" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A145">
         <v>144</v>
       </c>
@@ -9086,19 +9091,19 @@
         <v>0</v>
       </c>
       <c r="O145" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="P145" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="Q145">
         <v>1</v>
       </c>
       <c r="R145" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="146" spans="1:18">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="146" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A146">
         <v>145</v>
       </c>
@@ -9142,19 +9147,19 @@
         <v>0</v>
       </c>
       <c r="O146" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="P146" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="Q146">
         <v>2</v>
       </c>
       <c r="R146" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="147" spans="1:18">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="147" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A147">
         <v>146</v>
       </c>
@@ -9198,19 +9203,19 @@
         <v>0</v>
       </c>
       <c r="O147" t="s">
+        <v>16</v>
+      </c>
+      <c r="P147" t="s">
         <v>17</v>
-      </c>
-      <c r="P147" t="s">
-        <v>18</v>
       </c>
       <c r="Q147">
         <v>3</v>
       </c>
       <c r="R147" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="148" spans="1:18">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="148" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A148">
         <v>147</v>
       </c>
@@ -9254,19 +9259,19 @@
         <v>0</v>
       </c>
       <c r="O148" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="P148" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="Q148">
         <v>5</v>
       </c>
       <c r="R148" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="149" spans="1:18">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="149" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A149">
         <v>148</v>
       </c>
@@ -9310,19 +9315,19 @@
         <v>0</v>
       </c>
       <c r="O149" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="P149" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="Q149">
         <v>4</v>
       </c>
       <c r="R149" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="150" spans="1:18">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="150" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A150">
         <v>150</v>
       </c>
@@ -9366,19 +9371,19 @@
         <v>0</v>
       </c>
       <c r="O150" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="P150" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="Q150">
         <v>4</v>
       </c>
       <c r="R150" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="151" spans="1:18">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="151" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A151">
         <v>149</v>
       </c>
@@ -9422,19 +9427,19 @@
         <v>0</v>
       </c>
       <c r="O151" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="P151" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="Q151">
         <v>5</v>
       </c>
       <c r="R151" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="152" spans="1:18">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="152" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A152">
         <v>152</v>
       </c>
@@ -9478,19 +9483,19 @@
         <v>0</v>
       </c>
       <c r="O152" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="P152" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="Q152">
         <v>2</v>
       </c>
       <c r="R152" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="153" spans="1:18">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="153" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A153">
         <v>151</v>
       </c>
@@ -9534,19 +9539,19 @@
         <v>0</v>
       </c>
       <c r="O153" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="P153" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="Q153">
         <v>1</v>
       </c>
       <c r="R153" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="154" spans="1:18">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="154" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A154">
         <v>153</v>
       </c>
@@ -9590,19 +9595,19 @@
         <v>0</v>
       </c>
       <c r="O154" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="P154" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="Q154">
         <v>1</v>
       </c>
       <c r="R154" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="155" spans="1:18">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="155" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A155">
         <v>154</v>
       </c>
@@ -9646,19 +9651,19 @@
         <v>0</v>
       </c>
       <c r="O155" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="P155" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="Q155">
         <v>2</v>
       </c>
       <c r="R155" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="156" spans="1:18">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="156" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A156">
         <v>156</v>
       </c>
@@ -9702,19 +9707,19 @@
         <v>0</v>
       </c>
       <c r="O156" t="s">
+        <v>16</v>
+      </c>
+      <c r="P156" t="s">
         <v>17</v>
       </c>
-      <c r="P156" t="s">
-        <v>18</v>
-      </c>
       <c r="Q156">
         <v>1</v>
       </c>
       <c r="R156" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="157" spans="1:18">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="157" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A157">
         <v>155</v>
       </c>
@@ -9758,19 +9763,19 @@
         <v>0</v>
       </c>
       <c r="O157" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="P157" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="Q157">
         <v>2</v>
       </c>
       <c r="R157" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="158" spans="1:18">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="158" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A158">
         <v>158</v>
       </c>
@@ -9814,19 +9819,19 @@
         <v>0</v>
       </c>
       <c r="O158" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="P158" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="Q158">
         <v>2</v>
       </c>
       <c r="R158" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="159" spans="1:18">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="159" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A159">
         <v>157</v>
       </c>
@@ -9870,19 +9875,19 @@
         <v>0</v>
       </c>
       <c r="O159" t="s">
+        <v>16</v>
+      </c>
+      <c r="P159" t="s">
         <v>17</v>
-      </c>
-      <c r="P159" t="s">
-        <v>18</v>
       </c>
       <c r="Q159">
         <v>2</v>
       </c>
       <c r="R159" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="160" spans="1:18">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="160" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A160">
         <v>159</v>
       </c>
@@ -9926,19 +9931,19 @@
         <v>0</v>
       </c>
       <c r="O160" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="P160" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="Q160">
         <v>2</v>
       </c>
       <c r="R160" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="161" spans="1:18">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="161" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A161">
         <v>160</v>
       </c>
@@ -9982,19 +9987,19 @@
         <v>0</v>
       </c>
       <c r="O161" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="P161" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="Q161">
         <v>4</v>
       </c>
       <c r="R161" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="162" spans="1:18">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="162" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A162">
         <v>161</v>
       </c>
@@ -10038,19 +10043,19 @@
         <v>0</v>
       </c>
       <c r="O162" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="P162" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="Q162">
         <v>4</v>
       </c>
       <c r="R162" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="163" spans="1:18">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="163" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A163">
         <v>163</v>
       </c>
@@ -10094,19 +10099,19 @@
         <v>0</v>
       </c>
       <c r="O163" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="P163" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="Q163">
         <v>3</v>
       </c>
       <c r="R163" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="164" spans="1:18">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="164" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A164">
         <v>162</v>
       </c>
@@ -10150,19 +10155,19 @@
         <v>0</v>
       </c>
       <c r="O164" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="P164" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="Q164">
         <v>5</v>
       </c>
       <c r="R164" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="165" spans="1:18">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="165" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A165">
         <v>164</v>
       </c>
@@ -10206,21 +10211,21 @@
         <v>0</v>
       </c>
       <c r="O165" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="P165" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="Q165">
         <v>2</v>
       </c>
       <c r="R165" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="166" spans="1:18">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="166" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A166" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="B166">
         <v>1</v>
@@ -10262,21 +10267,21 @@
         <v>0</v>
       </c>
       <c r="O166" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="P166" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="Q166">
         <v>1</v>
       </c>
       <c r="R166" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="167" spans="1:18">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="167" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A167" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="B167">
         <v>1</v>
@@ -10318,22 +10323,22 @@
         <v>0</v>
       </c>
       <c r="O167" t="s">
+        <v>16</v>
+      </c>
+      <c r="P167" t="s">
         <v>17</v>
-      </c>
-      <c r="P167" t="s">
-        <v>18</v>
       </c>
       <c r="Q167">
         <v>3</v>
       </c>
       <c r="R167" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="168" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A168" t="s">
         <v>202</v>
       </c>
-    </row>
-    <row r="168" spans="1:18">
-      <c r="A168" t="s">
-        <v>203</v>
-      </c>
       <c r="B168">
         <v>0</v>
       </c>
@@ -10374,19 +10379,19 @@
         <v>0</v>
       </c>
       <c r="O168" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="P168" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="Q168">
         <v>3</v>
       </c>
       <c r="R168" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="169" spans="1:18">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="169" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A169">
         <v>168</v>
       </c>
@@ -10430,19 +10435,19 @@
         <v>0</v>
       </c>
       <c r="O169" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="P169" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="Q169">
         <v>5</v>
       </c>
       <c r="R169" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="170" spans="1:18">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="170" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A170">
         <v>169</v>
       </c>
@@ -10486,19 +10491,19 @@
         <v>0</v>
       </c>
       <c r="O170" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="P170" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="Q170">
         <v>4</v>
       </c>
       <c r="R170" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="171" spans="1:18">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="171" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A171">
         <v>170</v>
       </c>
@@ -10542,19 +10547,19 @@
         <v>0</v>
       </c>
       <c r="O171" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="P171" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="Q171">
         <v>5</v>
       </c>
       <c r="R171" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="172" spans="1:18">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="172" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A172">
         <v>171</v>
       </c>
@@ -10598,19 +10603,19 @@
         <v>0</v>
       </c>
       <c r="O172" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="P172" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="Q172">
         <v>3</v>
       </c>
       <c r="R172" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="173" spans="1:18">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="173" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A173">
         <v>172</v>
       </c>
@@ -10654,19 +10659,19 @@
         <v>0</v>
       </c>
       <c r="O173" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="P173" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="Q173">
         <v>1</v>
       </c>
       <c r="R173" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="174" spans="1:18">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="174" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A174">
         <v>173</v>
       </c>
@@ -10710,19 +10715,19 @@
         <v>0</v>
       </c>
       <c r="O174" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="P174" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="Q174">
         <v>2</v>
       </c>
       <c r="R174" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="175" spans="1:18">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="175" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A175">
         <v>174</v>
       </c>
@@ -10766,19 +10771,19 @@
         <v>0</v>
       </c>
       <c r="O175" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="P175" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="Q175">
         <v>1</v>
       </c>
       <c r="R175" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="176" spans="1:18">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="176" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A176">
         <v>175</v>
       </c>
@@ -10822,19 +10827,19 @@
         <v>0</v>
       </c>
       <c r="O176" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="P176" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="Q176">
         <v>3</v>
       </c>
       <c r="R176" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="177" spans="1:18">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="177" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A177">
         <v>176</v>
       </c>
@@ -10878,19 +10883,19 @@
         <v>0</v>
       </c>
       <c r="O177" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="P177" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="Q177">
         <v>3</v>
       </c>
       <c r="R177" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="178" spans="1:18">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="178" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A178">
         <v>177</v>
       </c>
@@ -10934,19 +10939,19 @@
         <v>0</v>
       </c>
       <c r="O178" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="P178" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="Q178">
         <v>4</v>
       </c>
       <c r="R178" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="179" spans="1:18">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="179" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A179">
         <v>178</v>
       </c>
@@ -10990,19 +10995,19 @@
         <v>0</v>
       </c>
       <c r="O179" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="P179" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="Q179">
         <v>4</v>
       </c>
       <c r="R179" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="180" spans="1:18">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="180" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A180">
         <v>180</v>
       </c>
@@ -11046,19 +11051,19 @@
         <v>0</v>
       </c>
       <c r="O180" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="P180" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="Q180">
         <v>2</v>
       </c>
       <c r="R180" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="181" spans="1:18">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="181" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A181">
         <v>179</v>
       </c>
@@ -11102,19 +11107,19 @@
         <v>0</v>
       </c>
       <c r="O181" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="P181" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="Q181">
         <v>2</v>
       </c>
       <c r="R181" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="182" spans="1:18">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="182" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A182">
         <v>182</v>
       </c>
@@ -11158,19 +11163,19 @@
         <v>0</v>
       </c>
       <c r="O182" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="P182" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="Q182">
         <v>3</v>
       </c>
       <c r="R182" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="183" spans="1:18">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="183" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A183">
         <v>181</v>
       </c>
@@ -11214,42 +11219,43 @@
         <v>0</v>
       </c>
       <c r="O183" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="P183" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="Q183">
         <v>2</v>
       </c>
       <c r="R183" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:R183"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Major improvements to merge process in 0_data_agg.R -Column names altered to begin with non-numeric -tester split into merge.chr and merge.num -debugger outputs all cols in original order
</commit_message>
<xml_diff>
--- a/raw-data-prep/raw_data/Debrief_AM.xlsx
+++ b/raw-data-prep/raw_data/Debrief_AM.xlsx
@@ -19,50 +19,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="567" uniqueCount="206">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="567" uniqueCount="205">
   <si>
     <t>Subject</t>
   </si>
   <si>
-    <t>1.a</t>
-  </si>
-  <si>
-    <t>1.b</t>
-  </si>
-  <si>
-    <t>1.c</t>
-  </si>
-  <si>
-    <t>1.d</t>
-  </si>
-  <si>
-    <t>1.e</t>
-  </si>
-  <si>
-    <t>2.a</t>
-  </si>
-  <si>
-    <t>2.b</t>
-  </si>
-  <si>
-    <t>2.c</t>
-  </si>
-  <si>
-    <t>2.d</t>
-  </si>
-  <si>
-    <t>2.e</t>
-  </si>
-  <si>
-    <t>2.f</t>
-  </si>
-  <si>
-    <t>2.g</t>
-  </si>
-  <si>
-    <t>2.h</t>
-  </si>
-  <si>
     <t>Surprise</t>
   </si>
   <si>
@@ -597,9 +558,6 @@
     <t xml:space="preserve">To see if we would be distracted </t>
   </si>
   <si>
-    <t>165 or 166?</t>
-  </si>
-  <si>
     <t>To see if the review our partner gave affected how much distraction was given</t>
   </si>
   <si>
@@ -627,9 +585,6 @@
     <t>To see if the more negative the response, the longer a person would assign distraction.</t>
   </si>
   <si>
-    <t>167?</t>
-  </si>
-  <si>
     <t>To see if we were upset about the evaluation of our essays</t>
   </si>
   <si>
@@ -637,6 +592,48 @@
   </si>
   <si>
     <t>Why_t</t>
+  </si>
+  <si>
+    <t>NA</t>
+  </si>
+  <si>
+    <t>Q1.a</t>
+  </si>
+  <si>
+    <t>Q1.b</t>
+  </si>
+  <si>
+    <t>Q1.c</t>
+  </si>
+  <si>
+    <t>Q1.d</t>
+  </si>
+  <si>
+    <t>Q1.e</t>
+  </si>
+  <si>
+    <t>Q2.a</t>
+  </si>
+  <si>
+    <t>Q2.b</t>
+  </si>
+  <si>
+    <t>Q2.c</t>
+  </si>
+  <si>
+    <t>Q2.d</t>
+  </si>
+  <si>
+    <t>Q2.e</t>
+  </si>
+  <si>
+    <t>Q2.f</t>
+  </si>
+  <si>
+    <t>Q2.g</t>
+  </si>
+  <si>
+    <t>Q2.h</t>
   </si>
 </sst>
 </file>
@@ -981,7 +978,7 @@
   <dimension ref="A1:R183"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O9" sqref="O9"/>
+      <selection activeCell="B1" sqref="B1:N1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -994,55 +991,55 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>1</v>
+        <v>192</v>
       </c>
       <c r="C1" t="s">
+        <v>193</v>
+      </c>
+      <c r="D1" t="s">
+        <v>194</v>
+      </c>
+      <c r="E1" t="s">
+        <v>195</v>
+      </c>
+      <c r="F1" t="s">
+        <v>196</v>
+      </c>
+      <c r="G1" t="s">
+        <v>197</v>
+      </c>
+      <c r="H1" t="s">
+        <v>198</v>
+      </c>
+      <c r="I1" t="s">
+        <v>199</v>
+      </c>
+      <c r="J1" t="s">
+        <v>200</v>
+      </c>
+      <c r="K1" t="s">
+        <v>201</v>
+      </c>
+      <c r="L1" t="s">
+        <v>202</v>
+      </c>
+      <c r="M1" t="s">
+        <v>203</v>
+      </c>
+      <c r="N1" t="s">
+        <v>204</v>
+      </c>
+      <c r="O1" t="s">
+        <v>189</v>
+      </c>
+      <c r="P1" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" t="s">
-        <v>8</v>
-      </c>
-      <c r="J1" t="s">
-        <v>9</v>
-      </c>
-      <c r="K1" t="s">
-        <v>10</v>
-      </c>
-      <c r="L1" t="s">
-        <v>11</v>
-      </c>
-      <c r="M1" t="s">
-        <v>12</v>
-      </c>
-      <c r="N1" t="s">
-        <v>13</v>
-      </c>
-      <c r="O1" t="s">
-        <v>204</v>
-      </c>
-      <c r="P1" t="s">
-        <v>14</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>15</v>
-      </c>
       <c r="R1" t="s">
-        <v>205</v>
+        <v>190</v>
       </c>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.25">
@@ -1089,16 +1086,16 @@
         <v>0</v>
       </c>
       <c r="O2" t="s">
-        <v>19</v>
+        <v>6</v>
       </c>
       <c r="P2" t="s">
-        <v>19</v>
+        <v>6</v>
       </c>
       <c r="Q2">
         <v>3</v>
       </c>
       <c r="R2" t="s">
-        <v>25</v>
+        <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.25">
@@ -1145,16 +1142,16 @@
         <v>0</v>
       </c>
       <c r="O3" t="s">
-        <v>19</v>
+        <v>6</v>
       </c>
       <c r="P3" t="s">
-        <v>19</v>
+        <v>6</v>
       </c>
       <c r="Q3">
         <v>4</v>
       </c>
       <c r="R3" t="s">
-        <v>24</v>
+        <v>11</v>
       </c>
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.25">
@@ -1201,16 +1198,16 @@
         <v>0</v>
       </c>
       <c r="O4" t="s">
-        <v>17</v>
+        <v>4</v>
       </c>
       <c r="P4" t="s">
-        <v>19</v>
+        <v>6</v>
       </c>
       <c r="Q4">
         <v>3</v>
       </c>
       <c r="R4" t="s">
-        <v>26</v>
+        <v>13</v>
       </c>
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.25">
@@ -1257,16 +1254,16 @@
         <v>0</v>
       </c>
       <c r="O5" t="s">
-        <v>27</v>
+        <v>14</v>
       </c>
       <c r="P5" t="s">
-        <v>19</v>
+        <v>6</v>
       </c>
       <c r="Q5">
         <v>3</v>
       </c>
       <c r="R5" t="s">
-        <v>28</v>
+        <v>15</v>
       </c>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.25">
@@ -1313,16 +1310,16 @@
         <v>0</v>
       </c>
       <c r="O6" t="s">
-        <v>19</v>
+        <v>6</v>
       </c>
       <c r="P6" t="s">
-        <v>19</v>
+        <v>6</v>
       </c>
       <c r="Q6">
         <v>1</v>
       </c>
       <c r="R6" t="s">
-        <v>22</v>
+        <v>9</v>
       </c>
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.25">
@@ -1369,16 +1366,16 @@
         <v>0</v>
       </c>
       <c r="O7" t="s">
-        <v>16</v>
+        <v>3</v>
       </c>
       <c r="P7" t="s">
-        <v>16</v>
+        <v>3</v>
       </c>
       <c r="Q7">
         <v>1</v>
       </c>
       <c r="R7" t="s">
-        <v>23</v>
+        <v>10</v>
       </c>
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.25">
@@ -1425,16 +1422,16 @@
         <v>0</v>
       </c>
       <c r="O8" t="s">
-        <v>16</v>
+        <v>3</v>
       </c>
       <c r="P8" t="s">
-        <v>17</v>
+        <v>4</v>
       </c>
       <c r="Q8">
         <v>3</v>
       </c>
       <c r="R8" t="s">
-        <v>30</v>
+        <v>17</v>
       </c>
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.25">
@@ -1481,16 +1478,16 @@
         <v>0</v>
       </c>
       <c r="O9" t="s">
-        <v>16</v>
+        <v>3</v>
       </c>
       <c r="P9" t="s">
-        <v>17</v>
+        <v>4</v>
       </c>
       <c r="Q9">
         <v>3</v>
       </c>
       <c r="R9" t="s">
-        <v>29</v>
+        <v>16</v>
       </c>
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.25">
@@ -1537,16 +1534,16 @@
         <v>0</v>
       </c>
       <c r="O10" t="s">
-        <v>19</v>
+        <v>6</v>
       </c>
       <c r="P10" t="s">
-        <v>17</v>
+        <v>4</v>
       </c>
       <c r="Q10">
         <v>4</v>
       </c>
       <c r="R10" t="s">
-        <v>32</v>
+        <v>19</v>
       </c>
     </row>
     <row r="11" spans="1:18" x14ac:dyDescent="0.25">
@@ -1593,16 +1590,16 @@
         <v>0</v>
       </c>
       <c r="O11" t="s">
-        <v>17</v>
+        <v>4</v>
       </c>
       <c r="P11" t="s">
-        <v>19</v>
+        <v>6</v>
       </c>
       <c r="Q11">
         <v>4</v>
       </c>
       <c r="R11" t="s">
-        <v>31</v>
+        <v>18</v>
       </c>
     </row>
     <row r="12" spans="1:18" x14ac:dyDescent="0.25">
@@ -1649,16 +1646,16 @@
         <v>0</v>
       </c>
       <c r="O12" t="s">
-        <v>19</v>
+        <v>6</v>
       </c>
       <c r="P12" t="s">
-        <v>19</v>
+        <v>6</v>
       </c>
       <c r="Q12">
         <v>2</v>
       </c>
       <c r="R12" t="s">
-        <v>35</v>
+        <v>22</v>
       </c>
     </row>
     <row r="13" spans="1:18" x14ac:dyDescent="0.25">
@@ -1705,16 +1702,16 @@
         <v>0</v>
       </c>
       <c r="O13" t="s">
-        <v>33</v>
+        <v>20</v>
       </c>
       <c r="P13" t="s">
-        <v>19</v>
+        <v>6</v>
       </c>
       <c r="Q13">
         <v>2</v>
       </c>
       <c r="R13" t="s">
-        <v>34</v>
+        <v>21</v>
       </c>
     </row>
     <row r="14" spans="1:18" x14ac:dyDescent="0.25">
@@ -1761,16 +1758,16 @@
         <v>1</v>
       </c>
       <c r="O14" t="s">
-        <v>16</v>
+        <v>3</v>
       </c>
       <c r="P14" t="s">
-        <v>19</v>
+        <v>6</v>
       </c>
       <c r="Q14">
         <v>2</v>
       </c>
       <c r="R14" t="s">
-        <v>37</v>
+        <v>24</v>
       </c>
     </row>
     <row r="15" spans="1:18" x14ac:dyDescent="0.25">
@@ -1817,16 +1814,16 @@
         <v>0</v>
       </c>
       <c r="O15" t="s">
-        <v>19</v>
+        <v>6</v>
       </c>
       <c r="P15" t="s">
-        <v>19</v>
+        <v>6</v>
       </c>
       <c r="Q15">
         <v>5</v>
       </c>
       <c r="R15" t="s">
-        <v>36</v>
+        <v>23</v>
       </c>
     </row>
     <row r="16" spans="1:18" x14ac:dyDescent="0.25">
@@ -1873,16 +1870,16 @@
         <v>0</v>
       </c>
       <c r="O16" t="s">
-        <v>16</v>
+        <v>3</v>
       </c>
       <c r="P16" t="s">
-        <v>19</v>
+        <v>6</v>
       </c>
       <c r="Q16">
         <v>4</v>
       </c>
       <c r="R16" t="s">
-        <v>45</v>
+        <v>32</v>
       </c>
     </row>
     <row r="17" spans="1:18" x14ac:dyDescent="0.25">
@@ -1929,16 +1926,16 @@
         <v>0</v>
       </c>
       <c r="O17" t="s">
-        <v>33</v>
+        <v>20</v>
       </c>
       <c r="P17" t="s">
-        <v>17</v>
+        <v>4</v>
       </c>
       <c r="Q17">
         <v>2</v>
       </c>
       <c r="R17" t="s">
-        <v>38</v>
+        <v>25</v>
       </c>
     </row>
     <row r="18" spans="1:18" x14ac:dyDescent="0.25">
@@ -1985,16 +1982,16 @@
         <v>0</v>
       </c>
       <c r="O18" t="s">
-        <v>16</v>
+        <v>3</v>
       </c>
       <c r="P18" t="s">
-        <v>17</v>
+        <v>4</v>
       </c>
       <c r="Q18">
         <v>3</v>
       </c>
       <c r="R18" t="s">
-        <v>41</v>
+        <v>28</v>
       </c>
     </row>
     <row r="19" spans="1:18" x14ac:dyDescent="0.25">
@@ -2041,16 +2038,16 @@
         <v>0</v>
       </c>
       <c r="O19" t="s">
-        <v>19</v>
+        <v>6</v>
       </c>
       <c r="P19" t="s">
-        <v>19</v>
+        <v>6</v>
       </c>
       <c r="Q19">
         <v>4</v>
       </c>
       <c r="R19" t="s">
-        <v>39</v>
+        <v>26</v>
       </c>
     </row>
     <row r="20" spans="1:18" x14ac:dyDescent="0.25">
@@ -2097,16 +2094,16 @@
         <v>0</v>
       </c>
       <c r="O20" t="s">
-        <v>16</v>
+        <v>3</v>
       </c>
       <c r="P20" t="s">
-        <v>17</v>
+        <v>4</v>
       </c>
       <c r="Q20">
         <v>2</v>
       </c>
       <c r="R20" t="s">
-        <v>42</v>
+        <v>29</v>
       </c>
     </row>
     <row r="21" spans="1:18" x14ac:dyDescent="0.25">
@@ -2153,16 +2150,16 @@
         <v>1</v>
       </c>
       <c r="O21" t="s">
-        <v>19</v>
+        <v>6</v>
       </c>
       <c r="P21" t="s">
-        <v>17</v>
+        <v>4</v>
       </c>
       <c r="Q21">
         <v>5</v>
       </c>
       <c r="R21" t="s">
-        <v>43</v>
+        <v>30</v>
       </c>
     </row>
     <row r="22" spans="1:18" x14ac:dyDescent="0.25">
@@ -2209,16 +2206,16 @@
         <v>0</v>
       </c>
       <c r="O22" t="s">
-        <v>19</v>
+        <v>6</v>
       </c>
       <c r="P22" t="s">
-        <v>19</v>
+        <v>6</v>
       </c>
       <c r="Q22">
         <v>3</v>
       </c>
       <c r="R22" t="s">
-        <v>40</v>
+        <v>27</v>
       </c>
     </row>
     <row r="23" spans="1:18" x14ac:dyDescent="0.25">
@@ -2265,16 +2262,16 @@
         <v>0</v>
       </c>
       <c r="O23" t="s">
-        <v>19</v>
+        <v>6</v>
       </c>
       <c r="P23" t="s">
-        <v>17</v>
+        <v>4</v>
       </c>
       <c r="Q23">
         <v>4</v>
       </c>
       <c r="R23" t="s">
-        <v>44</v>
+        <v>31</v>
       </c>
     </row>
     <row r="24" spans="1:18" x14ac:dyDescent="0.25">
@@ -2321,16 +2318,16 @@
         <v>0</v>
       </c>
       <c r="O24" t="s">
-        <v>19</v>
+        <v>6</v>
       </c>
       <c r="P24" t="s">
-        <v>19</v>
+        <v>6</v>
       </c>
       <c r="Q24">
         <v>2</v>
       </c>
       <c r="R24" t="s">
-        <v>21</v>
+        <v>8</v>
       </c>
     </row>
     <row r="25" spans="1:18" x14ac:dyDescent="0.25">
@@ -2377,16 +2374,16 @@
         <v>0</v>
       </c>
       <c r="O25" t="s">
-        <v>16</v>
+        <v>3</v>
       </c>
       <c r="P25" t="s">
-        <v>17</v>
+        <v>4</v>
       </c>
       <c r="Q25">
         <v>3</v>
       </c>
       <c r="R25" t="s">
-        <v>46</v>
+        <v>33</v>
       </c>
     </row>
     <row r="26" spans="1:18" x14ac:dyDescent="0.25">
@@ -2433,16 +2430,16 @@
         <v>0</v>
       </c>
       <c r="O26" t="s">
-        <v>16</v>
+        <v>3</v>
       </c>
       <c r="P26" t="s">
-        <v>16</v>
+        <v>3</v>
       </c>
       <c r="Q26">
         <v>1</v>
       </c>
       <c r="R26" t="s">
-        <v>48</v>
+        <v>35</v>
       </c>
     </row>
     <row r="27" spans="1:18" x14ac:dyDescent="0.25">
@@ -2489,16 +2486,16 @@
         <v>0</v>
       </c>
       <c r="O27" t="s">
-        <v>19</v>
+        <v>6</v>
       </c>
       <c r="P27" t="s">
-        <v>17</v>
+        <v>4</v>
       </c>
       <c r="Q27">
         <v>1</v>
       </c>
       <c r="R27" t="s">
-        <v>47</v>
+        <v>34</v>
       </c>
     </row>
     <row r="28" spans="1:18" x14ac:dyDescent="0.25">
@@ -2545,16 +2542,16 @@
         <v>0</v>
       </c>
       <c r="O28" t="s">
-        <v>16</v>
+        <v>3</v>
       </c>
       <c r="P28" t="s">
-        <v>19</v>
+        <v>6</v>
       </c>
       <c r="Q28">
         <v>3</v>
       </c>
       <c r="R28" t="s">
-        <v>49</v>
+        <v>36</v>
       </c>
     </row>
     <row r="29" spans="1:18" x14ac:dyDescent="0.25">
@@ -2601,16 +2598,16 @@
         <v>0</v>
       </c>
       <c r="O29" t="s">
-        <v>16</v>
+        <v>3</v>
       </c>
       <c r="P29" t="s">
-        <v>19</v>
+        <v>6</v>
       </c>
       <c r="Q29">
         <v>3</v>
       </c>
       <c r="R29" t="s">
-        <v>20</v>
+        <v>7</v>
       </c>
     </row>
     <row r="30" spans="1:18" x14ac:dyDescent="0.25">
@@ -2657,16 +2654,16 @@
         <v>0</v>
       </c>
       <c r="O30" t="s">
-        <v>19</v>
+        <v>6</v>
       </c>
       <c r="P30" t="s">
-        <v>19</v>
+        <v>6</v>
       </c>
       <c r="Q30">
         <v>4</v>
       </c>
       <c r="R30" t="s">
-        <v>51</v>
+        <v>38</v>
       </c>
     </row>
     <row r="31" spans="1:18" x14ac:dyDescent="0.25">
@@ -2713,16 +2710,16 @@
         <v>0</v>
       </c>
       <c r="O31" t="s">
-        <v>19</v>
+        <v>6</v>
       </c>
       <c r="P31" t="s">
-        <v>17</v>
+        <v>4</v>
       </c>
       <c r="Q31">
         <v>2</v>
       </c>
       <c r="R31" t="s">
-        <v>52</v>
+        <v>39</v>
       </c>
     </row>
     <row r="32" spans="1:18" x14ac:dyDescent="0.25">
@@ -2769,16 +2766,16 @@
         <v>0</v>
       </c>
       <c r="O32" t="s">
-        <v>19</v>
+        <v>6</v>
       </c>
       <c r="P32" t="s">
-        <v>17</v>
+        <v>4</v>
       </c>
       <c r="Q32">
         <v>2</v>
       </c>
       <c r="R32" t="s">
-        <v>50</v>
+        <v>37</v>
       </c>
     </row>
     <row r="33" spans="1:18" x14ac:dyDescent="0.25">
@@ -2825,16 +2822,16 @@
         <v>1</v>
       </c>
       <c r="O33" t="s">
-        <v>16</v>
+        <v>3</v>
       </c>
       <c r="P33" t="s">
-        <v>17</v>
+        <v>4</v>
       </c>
       <c r="Q33">
         <v>2</v>
       </c>
       <c r="R33" t="s">
-        <v>18</v>
+        <v>5</v>
       </c>
     </row>
     <row r="34" spans="1:18" x14ac:dyDescent="0.25">
@@ -2881,16 +2878,16 @@
         <v>0</v>
       </c>
       <c r="O34" t="s">
-        <v>19</v>
+        <v>6</v>
       </c>
       <c r="P34" t="s">
-        <v>19</v>
+        <v>6</v>
       </c>
       <c r="Q34">
         <v>3</v>
       </c>
       <c r="R34" t="s">
-        <v>54</v>
+        <v>41</v>
       </c>
     </row>
     <row r="35" spans="1:18" x14ac:dyDescent="0.25">
@@ -2937,16 +2934,16 @@
         <v>0</v>
       </c>
       <c r="O35" t="s">
-        <v>19</v>
+        <v>6</v>
       </c>
       <c r="P35" t="s">
-        <v>16</v>
+        <v>3</v>
       </c>
       <c r="Q35">
         <v>1</v>
       </c>
       <c r="R35" t="s">
-        <v>53</v>
+        <v>40</v>
       </c>
     </row>
     <row r="36" spans="1:18" x14ac:dyDescent="0.25">
@@ -2993,16 +2990,16 @@
         <v>0</v>
       </c>
       <c r="O36" t="s">
-        <v>19</v>
+        <v>6</v>
       </c>
       <c r="P36" t="s">
-        <v>19</v>
+        <v>6</v>
       </c>
       <c r="Q36">
         <v>3</v>
       </c>
       <c r="R36" t="s">
-        <v>57</v>
+        <v>44</v>
       </c>
     </row>
     <row r="37" spans="1:18" x14ac:dyDescent="0.25">
@@ -3049,16 +3046,16 @@
         <v>0</v>
       </c>
       <c r="O37" t="s">
-        <v>19</v>
+        <v>6</v>
       </c>
       <c r="P37" t="s">
-        <v>55</v>
+        <v>42</v>
       </c>
       <c r="Q37">
         <v>2</v>
       </c>
       <c r="R37" t="s">
-        <v>56</v>
+        <v>43</v>
       </c>
     </row>
     <row r="38" spans="1:18" x14ac:dyDescent="0.25">
@@ -3105,16 +3102,16 @@
         <v>0</v>
       </c>
       <c r="O38" t="s">
-        <v>19</v>
+        <v>6</v>
       </c>
       <c r="P38" t="s">
-        <v>19</v>
+        <v>6</v>
       </c>
       <c r="Q38">
         <v>4</v>
       </c>
       <c r="R38" t="s">
-        <v>59</v>
+        <v>46</v>
       </c>
     </row>
     <row r="39" spans="1:18" x14ac:dyDescent="0.25">
@@ -3161,16 +3158,16 @@
         <v>0</v>
       </c>
       <c r="O39" t="s">
-        <v>16</v>
+        <v>3</v>
       </c>
       <c r="P39" t="s">
-        <v>17</v>
+        <v>4</v>
       </c>
       <c r="Q39">
         <v>4</v>
       </c>
       <c r="R39" t="s">
-        <v>58</v>
+        <v>45</v>
       </c>
     </row>
     <row r="40" spans="1:18" x14ac:dyDescent="0.25">
@@ -3217,16 +3214,16 @@
         <v>0</v>
       </c>
       <c r="O40" t="s">
-        <v>19</v>
+        <v>6</v>
       </c>
       <c r="P40" t="s">
-        <v>19</v>
+        <v>6</v>
       </c>
       <c r="Q40">
         <v>1</v>
       </c>
       <c r="R40" t="s">
-        <v>60</v>
+        <v>47</v>
       </c>
     </row>
     <row r="41" spans="1:18" x14ac:dyDescent="0.25">
@@ -3273,16 +3270,16 @@
         <v>0</v>
       </c>
       <c r="O41" t="s">
-        <v>19</v>
+        <v>6</v>
       </c>
       <c r="P41" t="s">
-        <v>19</v>
+        <v>6</v>
       </c>
       <c r="Q41">
         <v>2</v>
       </c>
       <c r="R41" t="s">
-        <v>64</v>
+        <v>51</v>
       </c>
     </row>
     <row r="42" spans="1:18" x14ac:dyDescent="0.25">
@@ -3329,16 +3326,16 @@
         <v>0</v>
       </c>
       <c r="O42" t="s">
-        <v>19</v>
+        <v>6</v>
       </c>
       <c r="P42" t="s">
-        <v>17</v>
+        <v>4</v>
       </c>
       <c r="Q42">
         <v>5</v>
       </c>
       <c r="R42" t="s">
-        <v>61</v>
+        <v>48</v>
       </c>
     </row>
     <row r="43" spans="1:18" x14ac:dyDescent="0.25">
@@ -3385,16 +3382,16 @@
         <v>0</v>
       </c>
       <c r="O43" t="s">
-        <v>19</v>
+        <v>6</v>
       </c>
       <c r="P43" t="s">
-        <v>17</v>
+        <v>4</v>
       </c>
       <c r="Q43">
         <v>3</v>
       </c>
       <c r="R43" t="s">
-        <v>62</v>
+        <v>49</v>
       </c>
     </row>
     <row r="44" spans="1:18" x14ac:dyDescent="0.25">
@@ -3441,16 +3438,16 @@
         <v>0</v>
       </c>
       <c r="O44" t="s">
-        <v>16</v>
+        <v>3</v>
       </c>
       <c r="P44" t="s">
-        <v>17</v>
+        <v>4</v>
       </c>
       <c r="Q44">
         <v>4</v>
       </c>
       <c r="R44" t="s">
-        <v>63</v>
+        <v>50</v>
       </c>
     </row>
     <row r="45" spans="1:18" x14ac:dyDescent="0.25">
@@ -3497,16 +3494,16 @@
         <v>0</v>
       </c>
       <c r="O45" t="s">
-        <v>19</v>
+        <v>6</v>
       </c>
       <c r="P45" t="s">
-        <v>19</v>
+        <v>6</v>
       </c>
       <c r="Q45">
         <v>3</v>
       </c>
       <c r="R45" t="s">
-        <v>136</v>
+        <v>123</v>
       </c>
     </row>
     <row r="46" spans="1:18" x14ac:dyDescent="0.25">
@@ -3553,16 +3550,16 @@
         <v>0</v>
       </c>
       <c r="O46" t="s">
-        <v>19</v>
+        <v>6</v>
       </c>
       <c r="P46" t="s">
-        <v>19</v>
+        <v>6</v>
       </c>
       <c r="Q46">
         <v>2</v>
       </c>
       <c r="R46" t="s">
-        <v>137</v>
+        <v>124</v>
       </c>
     </row>
     <row r="47" spans="1:18" x14ac:dyDescent="0.25">
@@ -3609,16 +3606,16 @@
         <v>0</v>
       </c>
       <c r="O47" t="s">
-        <v>16</v>
+        <v>3</v>
       </c>
       <c r="P47" t="s">
-        <v>17</v>
+        <v>4</v>
       </c>
       <c r="Q47">
         <v>4</v>
       </c>
       <c r="R47" t="s">
-        <v>134</v>
+        <v>121</v>
       </c>
     </row>
     <row r="48" spans="1:18" x14ac:dyDescent="0.25">
@@ -3665,16 +3662,16 @@
         <v>0</v>
       </c>
       <c r="O48" t="s">
-        <v>19</v>
+        <v>6</v>
       </c>
       <c r="P48" t="s">
-        <v>17</v>
+        <v>4</v>
       </c>
       <c r="Q48">
         <v>2</v>
       </c>
       <c r="R48" t="s">
-        <v>135</v>
+        <v>122</v>
       </c>
     </row>
     <row r="49" spans="1:18" x14ac:dyDescent="0.25">
@@ -3721,16 +3718,16 @@
         <v>0</v>
       </c>
       <c r="O49" t="s">
-        <v>19</v>
+        <v>6</v>
       </c>
       <c r="P49" t="s">
-        <v>16</v>
+        <v>3</v>
       </c>
       <c r="Q49">
         <v>5</v>
       </c>
       <c r="R49" t="s">
-        <v>132</v>
+        <v>119</v>
       </c>
     </row>
     <row r="50" spans="1:18" x14ac:dyDescent="0.25">
@@ -3777,16 +3774,16 @@
         <v>0</v>
       </c>
       <c r="O50" t="s">
-        <v>19</v>
+        <v>6</v>
       </c>
       <c r="P50" t="s">
-        <v>17</v>
+        <v>4</v>
       </c>
       <c r="Q50">
         <v>2</v>
       </c>
       <c r="R50" t="s">
-        <v>133</v>
+        <v>120</v>
       </c>
     </row>
     <row r="51" spans="1:18" x14ac:dyDescent="0.25">
@@ -3833,16 +3830,16 @@
         <v>0</v>
       </c>
       <c r="O51" t="s">
-        <v>19</v>
+        <v>6</v>
       </c>
       <c r="P51" t="s">
-        <v>19</v>
+        <v>6</v>
       </c>
       <c r="Q51">
         <v>2</v>
       </c>
       <c r="R51" t="s">
-        <v>130</v>
+        <v>117</v>
       </c>
     </row>
     <row r="52" spans="1:18" x14ac:dyDescent="0.25">
@@ -3889,16 +3886,16 @@
         <v>0</v>
       </c>
       <c r="O52" t="s">
-        <v>19</v>
+        <v>6</v>
       </c>
       <c r="P52" t="s">
-        <v>19</v>
+        <v>6</v>
       </c>
       <c r="Q52">
         <v>2</v>
       </c>
       <c r="R52" t="s">
-        <v>131</v>
+        <v>118</v>
       </c>
     </row>
     <row r="53" spans="1:18" x14ac:dyDescent="0.25">
@@ -3945,16 +3942,16 @@
         <v>0</v>
       </c>
       <c r="O53" t="s">
-        <v>19</v>
+        <v>6</v>
       </c>
       <c r="P53" t="s">
-        <v>19</v>
+        <v>6</v>
       </c>
       <c r="Q53">
         <v>3</v>
       </c>
       <c r="R53" t="s">
-        <v>97</v>
+        <v>84</v>
       </c>
     </row>
     <row r="54" spans="1:18" x14ac:dyDescent="0.25">
@@ -4001,16 +3998,16 @@
         <v>0</v>
       </c>
       <c r="O54" t="s">
-        <v>33</v>
+        <v>20</v>
       </c>
       <c r="P54" t="s">
-        <v>16</v>
+        <v>3</v>
       </c>
       <c r="Q54">
         <v>3</v>
       </c>
       <c r="R54" t="s">
-        <v>129</v>
+        <v>116</v>
       </c>
     </row>
     <row r="55" spans="1:18" x14ac:dyDescent="0.25">
@@ -4057,16 +4054,16 @@
         <v>0</v>
       </c>
       <c r="O55" t="s">
-        <v>16</v>
+        <v>3</v>
       </c>
       <c r="P55" t="s">
-        <v>19</v>
+        <v>6</v>
       </c>
       <c r="Q55">
         <v>3</v>
       </c>
       <c r="R55" t="s">
-        <v>128</v>
+        <v>115</v>
       </c>
     </row>
     <row r="56" spans="1:18" x14ac:dyDescent="0.25">
@@ -4113,16 +4110,16 @@
         <v>0</v>
       </c>
       <c r="O56" t="s">
-        <v>19</v>
+        <v>6</v>
       </c>
       <c r="P56" t="s">
-        <v>19</v>
+        <v>6</v>
       </c>
       <c r="Q56">
         <v>3</v>
       </c>
       <c r="R56" t="s">
-        <v>127</v>
+        <v>114</v>
       </c>
     </row>
     <row r="57" spans="1:18" x14ac:dyDescent="0.25">
@@ -4169,16 +4166,16 @@
         <v>0</v>
       </c>
       <c r="O57" t="s">
-        <v>19</v>
+        <v>6</v>
       </c>
       <c r="P57" t="s">
-        <v>19</v>
+        <v>6</v>
       </c>
       <c r="Q57">
         <v>2</v>
       </c>
       <c r="R57" t="s">
-        <v>126</v>
+        <v>113</v>
       </c>
     </row>
     <row r="58" spans="1:18" x14ac:dyDescent="0.25">
@@ -4225,16 +4222,16 @@
         <v>0</v>
       </c>
       <c r="O58" t="s">
-        <v>33</v>
+        <v>20</v>
       </c>
       <c r="P58" t="s">
-        <v>19</v>
+        <v>6</v>
       </c>
       <c r="Q58">
         <v>3</v>
       </c>
       <c r="R58" t="s">
-        <v>124</v>
+        <v>111</v>
       </c>
     </row>
     <row r="59" spans="1:18" x14ac:dyDescent="0.25">
@@ -4281,16 +4278,16 @@
         <v>0</v>
       </c>
       <c r="O59" t="s">
-        <v>19</v>
+        <v>6</v>
       </c>
       <c r="P59" t="s">
-        <v>19</v>
+        <v>6</v>
       </c>
       <c r="Q59">
         <v>1</v>
       </c>
       <c r="R59" t="s">
-        <v>123</v>
+        <v>110</v>
       </c>
     </row>
     <row r="60" spans="1:18" x14ac:dyDescent="0.25">
@@ -4337,16 +4334,16 @@
         <v>0</v>
       </c>
       <c r="O60" t="s">
-        <v>19</v>
+        <v>6</v>
       </c>
       <c r="P60" t="s">
-        <v>19</v>
+        <v>6</v>
       </c>
       <c r="Q60">
         <v>2</v>
       </c>
       <c r="R60" t="s">
-        <v>125</v>
+        <v>112</v>
       </c>
     </row>
     <row r="61" spans="1:18" x14ac:dyDescent="0.25">
@@ -4393,16 +4390,16 @@
         <v>0</v>
       </c>
       <c r="O61" t="s">
-        <v>19</v>
+        <v>6</v>
       </c>
       <c r="P61" t="s">
-        <v>17</v>
+        <v>4</v>
       </c>
       <c r="Q61">
         <v>1</v>
       </c>
       <c r="R61" t="s">
-        <v>122</v>
+        <v>109</v>
       </c>
     </row>
     <row r="62" spans="1:18" x14ac:dyDescent="0.25">
@@ -4449,16 +4446,16 @@
         <v>0</v>
       </c>
       <c r="O62" t="s">
-        <v>19</v>
+        <v>6</v>
       </c>
       <c r="P62" t="s">
-        <v>19</v>
+        <v>6</v>
       </c>
       <c r="Q62">
         <v>2</v>
       </c>
       <c r="R62" t="s">
-        <v>121</v>
+        <v>108</v>
       </c>
     </row>
     <row r="63" spans="1:18" x14ac:dyDescent="0.25">
@@ -4505,16 +4502,16 @@
         <v>0</v>
       </c>
       <c r="O63" t="s">
-        <v>16</v>
+        <v>3</v>
       </c>
       <c r="P63" t="s">
-        <v>17</v>
+        <v>4</v>
       </c>
       <c r="Q63">
         <v>2</v>
       </c>
       <c r="R63" t="s">
-        <v>120</v>
+        <v>107</v>
       </c>
     </row>
     <row r="64" spans="1:18" x14ac:dyDescent="0.25">
@@ -4561,16 +4558,16 @@
         <v>0</v>
       </c>
       <c r="O64" t="s">
-        <v>19</v>
+        <v>6</v>
       </c>
       <c r="P64" t="s">
-        <v>19</v>
+        <v>6</v>
       </c>
       <c r="Q64">
         <v>4</v>
       </c>
       <c r="R64" t="s">
-        <v>119</v>
+        <v>106</v>
       </c>
     </row>
     <row r="65" spans="1:18" x14ac:dyDescent="0.25">
@@ -4617,16 +4614,16 @@
         <v>0</v>
       </c>
       <c r="O65" t="s">
-        <v>19</v>
+        <v>6</v>
       </c>
       <c r="P65" t="s">
-        <v>16</v>
+        <v>3</v>
       </c>
       <c r="Q65">
         <v>1</v>
       </c>
       <c r="R65" t="s">
-        <v>71</v>
+        <v>58</v>
       </c>
     </row>
     <row r="66" spans="1:18" x14ac:dyDescent="0.25">
@@ -4673,16 +4670,16 @@
         <v>0</v>
       </c>
       <c r="O66" t="s">
-        <v>19</v>
+        <v>6</v>
       </c>
       <c r="P66" t="s">
-        <v>19</v>
+        <v>6</v>
       </c>
       <c r="Q66">
         <v>5</v>
       </c>
       <c r="R66" t="s">
-        <v>141</v>
+        <v>128</v>
       </c>
     </row>
     <row r="67" spans="1:18" x14ac:dyDescent="0.25">
@@ -4729,16 +4726,16 @@
         <v>0</v>
       </c>
       <c r="O67" t="s">
-        <v>19</v>
+        <v>6</v>
       </c>
       <c r="P67" t="s">
-        <v>19</v>
+        <v>6</v>
       </c>
       <c r="Q67">
         <v>3</v>
       </c>
       <c r="R67" t="s">
-        <v>140</v>
+        <v>127</v>
       </c>
     </row>
     <row r="68" spans="1:18" x14ac:dyDescent="0.25">
@@ -4785,16 +4782,16 @@
         <v>0</v>
       </c>
       <c r="O68" t="s">
-        <v>16</v>
+        <v>3</v>
       </c>
       <c r="P68" t="s">
-        <v>19</v>
+        <v>6</v>
       </c>
       <c r="Q68">
         <v>2</v>
       </c>
       <c r="R68" t="s">
-        <v>142</v>
+        <v>129</v>
       </c>
     </row>
     <row r="69" spans="1:18" x14ac:dyDescent="0.25">
@@ -4841,16 +4838,16 @@
         <v>0</v>
       </c>
       <c r="O69" t="s">
-        <v>19</v>
+        <v>6</v>
       </c>
       <c r="P69" t="s">
-        <v>19</v>
+        <v>6</v>
       </c>
       <c r="Q69">
         <v>4</v>
       </c>
       <c r="R69" t="s">
-        <v>143</v>
+        <v>130</v>
       </c>
     </row>
     <row r="70" spans="1:18" x14ac:dyDescent="0.25">
@@ -4897,16 +4894,16 @@
         <v>0</v>
       </c>
       <c r="O70" t="s">
-        <v>19</v>
+        <v>6</v>
       </c>
       <c r="P70" t="s">
-        <v>17</v>
+        <v>4</v>
       </c>
       <c r="Q70">
         <v>2</v>
       </c>
       <c r="R70" t="s">
-        <v>144</v>
+        <v>131</v>
       </c>
     </row>
     <row r="71" spans="1:18" x14ac:dyDescent="0.25">
@@ -4953,16 +4950,16 @@
         <v>1</v>
       </c>
       <c r="O71" t="s">
-        <v>19</v>
+        <v>6</v>
       </c>
       <c r="P71" t="s">
-        <v>19</v>
+        <v>6</v>
       </c>
       <c r="Q71">
         <v>3</v>
       </c>
       <c r="R71" t="s">
-        <v>139</v>
+        <v>126</v>
       </c>
     </row>
     <row r="72" spans="1:18" x14ac:dyDescent="0.25">
@@ -5009,16 +5006,16 @@
         <v>0</v>
       </c>
       <c r="O72" t="s">
-        <v>19</v>
+        <v>6</v>
       </c>
       <c r="P72" t="s">
-        <v>19</v>
+        <v>6</v>
       </c>
       <c r="Q72">
         <v>3</v>
       </c>
       <c r="R72" t="s">
-        <v>73</v>
+        <v>60</v>
       </c>
     </row>
     <row r="73" spans="1:18" x14ac:dyDescent="0.25">
@@ -5065,16 +5062,16 @@
         <v>1</v>
       </c>
       <c r="O73" t="s">
-        <v>19</v>
+        <v>6</v>
       </c>
       <c r="P73" t="s">
-        <v>16</v>
+        <v>3</v>
       </c>
       <c r="Q73">
         <v>2</v>
       </c>
       <c r="R73" t="s">
-        <v>75</v>
+        <v>62</v>
       </c>
     </row>
     <row r="74" spans="1:18" x14ac:dyDescent="0.25">
@@ -5121,16 +5118,16 @@
         <v>0</v>
       </c>
       <c r="O74" t="s">
-        <v>19</v>
+        <v>6</v>
       </c>
       <c r="P74" t="s">
-        <v>17</v>
+        <v>4</v>
       </c>
       <c r="Q74">
         <v>2</v>
       </c>
       <c r="R74" t="s">
-        <v>74</v>
+        <v>61</v>
       </c>
     </row>
     <row r="75" spans="1:18" x14ac:dyDescent="0.25">
@@ -5174,16 +5171,16 @@
         <v>0</v>
       </c>
       <c r="O75" t="s">
-        <v>16</v>
+        <v>3</v>
       </c>
       <c r="P75" t="s">
-        <v>19</v>
+        <v>6</v>
       </c>
       <c r="Q75">
         <v>4</v>
       </c>
       <c r="R75" t="s">
-        <v>76</v>
+        <v>63</v>
       </c>
     </row>
     <row r="76" spans="1:18" x14ac:dyDescent="0.25">
@@ -5230,16 +5227,16 @@
         <v>0</v>
       </c>
       <c r="O76" t="s">
-        <v>19</v>
+        <v>6</v>
       </c>
       <c r="P76" t="s">
-        <v>19</v>
+        <v>6</v>
       </c>
       <c r="Q76">
         <v>4</v>
       </c>
       <c r="R76" t="s">
-        <v>77</v>
+        <v>64</v>
       </c>
     </row>
     <row r="77" spans="1:18" x14ac:dyDescent="0.25">
@@ -5286,16 +5283,16 @@
         <v>0</v>
       </c>
       <c r="O77" t="s">
-        <v>19</v>
+        <v>6</v>
       </c>
       <c r="P77" t="s">
-        <v>19</v>
+        <v>6</v>
       </c>
       <c r="Q77">
         <v>4</v>
       </c>
       <c r="R77" t="s">
-        <v>78</v>
+        <v>65</v>
       </c>
     </row>
     <row r="78" spans="1:18" x14ac:dyDescent="0.25">
@@ -5342,16 +5339,16 @@
         <v>0</v>
       </c>
       <c r="O78" t="s">
-        <v>16</v>
+        <v>3</v>
       </c>
       <c r="P78" t="s">
-        <v>17</v>
+        <v>4</v>
       </c>
       <c r="Q78">
         <v>1</v>
       </c>
       <c r="R78" t="s">
-        <v>79</v>
+        <v>66</v>
       </c>
     </row>
     <row r="79" spans="1:18" x14ac:dyDescent="0.25">
@@ -5398,16 +5395,16 @@
         <v>0</v>
       </c>
       <c r="O79" t="s">
-        <v>19</v>
+        <v>6</v>
       </c>
       <c r="P79" t="s">
-        <v>19</v>
+        <v>6</v>
       </c>
       <c r="Q79">
         <v>5</v>
       </c>
       <c r="R79" t="s">
-        <v>80</v>
+        <v>67</v>
       </c>
     </row>
     <row r="80" spans="1:18" x14ac:dyDescent="0.25">
@@ -5454,16 +5451,16 @@
         <v>0</v>
       </c>
       <c r="O80" t="s">
-        <v>16</v>
+        <v>3</v>
       </c>
       <c r="P80" t="s">
-        <v>19</v>
+        <v>6</v>
       </c>
       <c r="Q80">
         <v>4</v>
       </c>
       <c r="R80" t="s">
-        <v>81</v>
+        <v>68</v>
       </c>
     </row>
     <row r="81" spans="1:18" x14ac:dyDescent="0.25">
@@ -5510,16 +5507,16 @@
         <v>0</v>
       </c>
       <c r="O81" t="s">
-        <v>19</v>
+        <v>6</v>
       </c>
       <c r="P81" t="s">
-        <v>19</v>
+        <v>6</v>
       </c>
       <c r="Q81">
         <v>5</v>
       </c>
       <c r="R81" t="s">
-        <v>65</v>
+        <v>52</v>
       </c>
     </row>
     <row r="82" spans="1:18" x14ac:dyDescent="0.25">
@@ -5566,16 +5563,16 @@
         <v>0</v>
       </c>
       <c r="O82" t="s">
-        <v>19</v>
+        <v>6</v>
       </c>
       <c r="P82" t="s">
-        <v>19</v>
+        <v>6</v>
       </c>
       <c r="Q82">
         <v>4</v>
       </c>
       <c r="R82" t="s">
-        <v>66</v>
+        <v>53</v>
       </c>
     </row>
     <row r="83" spans="1:18" x14ac:dyDescent="0.25">
@@ -5622,16 +5619,16 @@
         <v>0</v>
       </c>
       <c r="O83" t="s">
-        <v>17</v>
+        <v>4</v>
       </c>
       <c r="P83" t="s">
-        <v>17</v>
+        <v>4</v>
       </c>
       <c r="Q83">
         <v>4</v>
       </c>
       <c r="R83" t="s">
-        <v>67</v>
+        <v>54</v>
       </c>
     </row>
     <row r="84" spans="1:18" x14ac:dyDescent="0.25">
@@ -5678,16 +5675,16 @@
         <v>0</v>
       </c>
       <c r="O84" t="s">
-        <v>19</v>
+        <v>6</v>
       </c>
       <c r="P84" t="s">
-        <v>19</v>
+        <v>6</v>
       </c>
       <c r="Q84">
         <v>4</v>
       </c>
       <c r="R84" t="s">
-        <v>68</v>
+        <v>55</v>
       </c>
     </row>
     <row r="85" spans="1:18" x14ac:dyDescent="0.25">
@@ -5734,16 +5731,16 @@
         <v>0</v>
       </c>
       <c r="O85" t="s">
-        <v>19</v>
+        <v>6</v>
       </c>
       <c r="P85" t="s">
-        <v>19</v>
+        <v>6</v>
       </c>
       <c r="Q85">
         <v>2</v>
       </c>
       <c r="R85" t="s">
-        <v>69</v>
+        <v>56</v>
       </c>
     </row>
     <row r="86" spans="1:18" x14ac:dyDescent="0.25">
@@ -5790,16 +5787,16 @@
         <v>0</v>
       </c>
       <c r="O86" t="s">
-        <v>19</v>
+        <v>6</v>
       </c>
       <c r="P86" t="s">
-        <v>19</v>
+        <v>6</v>
       </c>
       <c r="Q86">
         <v>4</v>
       </c>
       <c r="R86" t="s">
-        <v>70</v>
+        <v>57</v>
       </c>
     </row>
     <row r="87" spans="1:18" x14ac:dyDescent="0.25">
@@ -5846,16 +5843,16 @@
         <v>0</v>
       </c>
       <c r="O87" t="s">
-        <v>16</v>
+        <v>3</v>
       </c>
       <c r="P87" t="s">
-        <v>19</v>
+        <v>6</v>
       </c>
       <c r="Q87">
         <v>2</v>
       </c>
       <c r="R87" t="s">
-        <v>71</v>
+        <v>58</v>
       </c>
     </row>
     <row r="88" spans="1:18" x14ac:dyDescent="0.25">
@@ -5902,16 +5899,16 @@
         <v>0</v>
       </c>
       <c r="O88" t="s">
-        <v>19</v>
+        <v>6</v>
       </c>
       <c r="P88" t="s">
-        <v>19</v>
+        <v>6</v>
       </c>
       <c r="Q88">
         <v>2</v>
       </c>
       <c r="R88" t="s">
-        <v>72</v>
+        <v>59</v>
       </c>
     </row>
     <row r="89" spans="1:18" x14ac:dyDescent="0.25">
@@ -5958,16 +5955,16 @@
         <v>0</v>
       </c>
       <c r="O89" t="s">
-        <v>19</v>
+        <v>6</v>
       </c>
       <c r="P89" t="s">
-        <v>19</v>
+        <v>6</v>
       </c>
       <c r="Q89">
         <v>3</v>
       </c>
       <c r="R89" t="s">
-        <v>82</v>
+        <v>69</v>
       </c>
     </row>
     <row r="90" spans="1:18" x14ac:dyDescent="0.25">
@@ -6014,16 +6011,16 @@
         <v>0</v>
       </c>
       <c r="O90" t="s">
-        <v>16</v>
+        <v>3</v>
       </c>
       <c r="P90" t="s">
-        <v>19</v>
+        <v>6</v>
       </c>
       <c r="Q90">
         <v>5</v>
       </c>
       <c r="R90" t="s">
-        <v>84</v>
+        <v>71</v>
       </c>
     </row>
     <row r="91" spans="1:18" x14ac:dyDescent="0.25">
@@ -6070,16 +6067,16 @@
         <v>0</v>
       </c>
       <c r="O91" t="s">
-        <v>16</v>
+        <v>3</v>
       </c>
       <c r="P91" t="s">
-        <v>17</v>
+        <v>4</v>
       </c>
       <c r="Q91">
         <v>2</v>
       </c>
       <c r="R91" t="s">
-        <v>83</v>
+        <v>70</v>
       </c>
     </row>
     <row r="92" spans="1:18" x14ac:dyDescent="0.25">
@@ -6126,16 +6123,16 @@
         <v>0</v>
       </c>
       <c r="O92" t="s">
-        <v>16</v>
+        <v>3</v>
       </c>
       <c r="P92" t="s">
-        <v>16</v>
+        <v>3</v>
       </c>
       <c r="Q92">
         <v>2</v>
       </c>
       <c r="R92" t="s">
-        <v>86</v>
+        <v>73</v>
       </c>
     </row>
     <row r="93" spans="1:18" x14ac:dyDescent="0.25">
@@ -6182,16 +6179,16 @@
         <v>0</v>
       </c>
       <c r="O93" t="s">
-        <v>16</v>
+        <v>3</v>
       </c>
       <c r="P93" t="s">
-        <v>19</v>
+        <v>6</v>
       </c>
       <c r="Q93">
         <v>3</v>
       </c>
       <c r="R93" t="s">
-        <v>85</v>
+        <v>72</v>
       </c>
     </row>
     <row r="94" spans="1:18" x14ac:dyDescent="0.25">
@@ -6238,16 +6235,16 @@
         <v>0</v>
       </c>
       <c r="O94" t="s">
-        <v>16</v>
+        <v>3</v>
       </c>
       <c r="P94" t="s">
-        <v>17</v>
+        <v>4</v>
       </c>
       <c r="Q94">
         <v>4</v>
       </c>
       <c r="R94" t="s">
-        <v>138</v>
+        <v>125</v>
       </c>
     </row>
     <row r="95" spans="1:18" x14ac:dyDescent="0.25">
@@ -6294,16 +6291,16 @@
         <v>0</v>
       </c>
       <c r="O95" t="s">
-        <v>19</v>
+        <v>6</v>
       </c>
       <c r="P95" t="s">
-        <v>87</v>
+        <v>74</v>
       </c>
       <c r="Q95">
         <v>4</v>
       </c>
       <c r="R95" t="s">
-        <v>88</v>
+        <v>75</v>
       </c>
     </row>
     <row r="96" spans="1:18" x14ac:dyDescent="0.25">
@@ -6350,16 +6347,16 @@
         <v>0</v>
       </c>
       <c r="O96" t="s">
-        <v>19</v>
+        <v>6</v>
       </c>
       <c r="P96" t="s">
-        <v>19</v>
+        <v>6</v>
       </c>
       <c r="Q96">
         <v>1</v>
       </c>
       <c r="R96" t="s">
-        <v>90</v>
+        <v>77</v>
       </c>
     </row>
     <row r="97" spans="1:18" x14ac:dyDescent="0.25">
@@ -6406,16 +6403,16 @@
         <v>0</v>
       </c>
       <c r="O97" t="s">
-        <v>19</v>
+        <v>6</v>
       </c>
       <c r="P97" t="s">
-        <v>19</v>
+        <v>6</v>
       </c>
       <c r="Q97">
         <v>3</v>
       </c>
       <c r="R97" t="s">
-        <v>89</v>
+        <v>76</v>
       </c>
     </row>
     <row r="98" spans="1:18" x14ac:dyDescent="0.25">
@@ -6462,16 +6459,16 @@
         <v>0</v>
       </c>
       <c r="O98" t="s">
-        <v>19</v>
+        <v>6</v>
       </c>
       <c r="P98" t="s">
-        <v>17</v>
+        <v>4</v>
       </c>
       <c r="Q98">
         <v>1</v>
       </c>
       <c r="R98" t="s">
-        <v>92</v>
+        <v>79</v>
       </c>
     </row>
     <row r="99" spans="1:18" x14ac:dyDescent="0.25">
@@ -6518,16 +6515,16 @@
         <v>0</v>
       </c>
       <c r="O99" t="s">
-        <v>19</v>
+        <v>6</v>
       </c>
       <c r="P99" t="s">
-        <v>19</v>
+        <v>6</v>
       </c>
       <c r="Q99">
         <v>4</v>
       </c>
       <c r="R99" t="s">
-        <v>91</v>
+        <v>78</v>
       </c>
     </row>
     <row r="100" spans="1:18" x14ac:dyDescent="0.25">
@@ -6574,16 +6571,16 @@
         <v>0</v>
       </c>
       <c r="O100" t="s">
-        <v>19</v>
+        <v>6</v>
       </c>
       <c r="P100" t="s">
-        <v>16</v>
+        <v>3</v>
       </c>
       <c r="Q100">
         <v>2</v>
       </c>
       <c r="R100" t="s">
-        <v>93</v>
+        <v>80</v>
       </c>
     </row>
     <row r="101" spans="1:18" x14ac:dyDescent="0.25">
@@ -6630,16 +6627,16 @@
         <v>0</v>
       </c>
       <c r="O101" t="s">
-        <v>16</v>
+        <v>3</v>
       </c>
       <c r="P101" t="s">
-        <v>19</v>
+        <v>6</v>
       </c>
       <c r="Q101">
         <v>5</v>
       </c>
       <c r="R101" t="s">
-        <v>94</v>
+        <v>81</v>
       </c>
     </row>
     <row r="102" spans="1:18" x14ac:dyDescent="0.25">
@@ -6686,16 +6683,16 @@
         <v>0</v>
       </c>
       <c r="O102" t="s">
-        <v>19</v>
+        <v>6</v>
       </c>
       <c r="P102" t="s">
-        <v>17</v>
+        <v>4</v>
       </c>
       <c r="Q102">
         <v>4</v>
       </c>
       <c r="R102" t="s">
-        <v>96</v>
+        <v>83</v>
       </c>
     </row>
     <row r="103" spans="1:18" x14ac:dyDescent="0.25">
@@ -6742,16 +6739,16 @@
         <v>0</v>
       </c>
       <c r="O103" t="s">
-        <v>16</v>
+        <v>3</v>
       </c>
       <c r="P103" t="s">
-        <v>19</v>
+        <v>6</v>
       </c>
       <c r="Q103">
         <v>2</v>
       </c>
       <c r="R103" t="s">
-        <v>95</v>
+        <v>82</v>
       </c>
     </row>
     <row r="104" spans="1:18" x14ac:dyDescent="0.25">
@@ -6798,16 +6795,16 @@
         <v>0</v>
       </c>
       <c r="O104" t="s">
-        <v>19</v>
+        <v>6</v>
       </c>
       <c r="P104" t="s">
-        <v>16</v>
+        <v>3</v>
       </c>
       <c r="Q104">
         <v>2</v>
       </c>
       <c r="R104" t="s">
-        <v>99</v>
+        <v>86</v>
       </c>
     </row>
     <row r="105" spans="1:18" x14ac:dyDescent="0.25">
@@ -6854,16 +6851,16 @@
         <v>0</v>
       </c>
       <c r="O105" t="s">
-        <v>19</v>
+        <v>6</v>
       </c>
       <c r="P105" t="s">
-        <v>55</v>
+        <v>42</v>
       </c>
       <c r="Q105">
         <v>4</v>
       </c>
       <c r="R105" t="s">
-        <v>98</v>
+        <v>85</v>
       </c>
     </row>
     <row r="106" spans="1:18" x14ac:dyDescent="0.25">
@@ -6910,16 +6907,16 @@
         <v>0</v>
       </c>
       <c r="O106" t="s">
-        <v>16</v>
+        <v>3</v>
       </c>
       <c r="P106" t="s">
-        <v>17</v>
+        <v>4</v>
       </c>
       <c r="Q106">
         <v>2</v>
       </c>
       <c r="R106" t="s">
-        <v>101</v>
+        <v>88</v>
       </c>
     </row>
     <row r="107" spans="1:18" x14ac:dyDescent="0.25">
@@ -6966,16 +6963,16 @@
         <v>0</v>
       </c>
       <c r="O107" t="s">
-        <v>19</v>
+        <v>6</v>
       </c>
       <c r="P107" t="s">
-        <v>16</v>
+        <v>3</v>
       </c>
       <c r="Q107">
         <v>4</v>
       </c>
       <c r="R107" t="s">
-        <v>100</v>
+        <v>87</v>
       </c>
     </row>
     <row r="108" spans="1:18" x14ac:dyDescent="0.25">
@@ -7022,16 +7019,16 @@
         <v>0</v>
       </c>
       <c r="O108" t="s">
-        <v>19</v>
+        <v>6</v>
       </c>
       <c r="P108" t="s">
-        <v>17</v>
+        <v>4</v>
       </c>
       <c r="Q108">
         <v>2</v>
       </c>
       <c r="R108" t="s">
-        <v>102</v>
+        <v>89</v>
       </c>
     </row>
     <row r="109" spans="1:18" x14ac:dyDescent="0.25">
@@ -7078,16 +7075,16 @@
         <v>0</v>
       </c>
       <c r="O109" t="s">
-        <v>19</v>
+        <v>6</v>
       </c>
       <c r="P109" t="s">
-        <v>19</v>
+        <v>6</v>
       </c>
       <c r="Q109">
         <v>3</v>
       </c>
       <c r="R109" t="s">
-        <v>103</v>
+        <v>90</v>
       </c>
     </row>
     <row r="110" spans="1:18" x14ac:dyDescent="0.25">
@@ -7134,16 +7131,16 @@
         <v>0</v>
       </c>
       <c r="O110" t="s">
-        <v>19</v>
+        <v>6</v>
       </c>
       <c r="P110" t="s">
-        <v>19</v>
+        <v>6</v>
       </c>
       <c r="Q110">
         <v>2</v>
       </c>
       <c r="R110" t="s">
-        <v>104</v>
+        <v>91</v>
       </c>
     </row>
     <row r="111" spans="1:18" x14ac:dyDescent="0.25">
@@ -7190,16 +7187,16 @@
         <v>0</v>
       </c>
       <c r="O111" t="s">
-        <v>19</v>
+        <v>6</v>
       </c>
       <c r="P111" t="s">
-        <v>16</v>
+        <v>3</v>
       </c>
       <c r="Q111">
         <v>2</v>
       </c>
       <c r="R111" t="s">
-        <v>105</v>
+        <v>92</v>
       </c>
     </row>
     <row r="112" spans="1:18" x14ac:dyDescent="0.25">
@@ -7246,16 +7243,16 @@
         <v>0</v>
       </c>
       <c r="O112" t="s">
-        <v>19</v>
+        <v>6</v>
       </c>
       <c r="P112" t="s">
-        <v>19</v>
+        <v>6</v>
       </c>
       <c r="Q112">
         <v>1</v>
       </c>
       <c r="R112" t="s">
-        <v>106</v>
+        <v>93</v>
       </c>
     </row>
     <row r="113" spans="1:18" x14ac:dyDescent="0.25">
@@ -7302,16 +7299,16 @@
         <v>0</v>
       </c>
       <c r="O113" t="s">
-        <v>16</v>
+        <v>3</v>
       </c>
       <c r="P113" t="s">
-        <v>19</v>
+        <v>6</v>
       </c>
       <c r="Q113">
         <v>3</v>
       </c>
       <c r="R113" t="s">
-        <v>107</v>
+        <v>94</v>
       </c>
     </row>
     <row r="114" spans="1:18" x14ac:dyDescent="0.25">
@@ -7358,16 +7355,16 @@
         <v>0</v>
       </c>
       <c r="O114" t="s">
-        <v>16</v>
+        <v>3</v>
       </c>
       <c r="P114" t="s">
-        <v>17</v>
+        <v>4</v>
       </c>
       <c r="Q114">
         <v>2</v>
       </c>
       <c r="R114" t="s">
-        <v>108</v>
+        <v>95</v>
       </c>
     </row>
     <row r="115" spans="1:18" x14ac:dyDescent="0.25">
@@ -7414,16 +7411,16 @@
         <v>0</v>
       </c>
       <c r="O115" t="s">
-        <v>19</v>
+        <v>6</v>
       </c>
       <c r="P115" t="s">
-        <v>19</v>
+        <v>6</v>
       </c>
       <c r="Q115">
         <v>4</v>
       </c>
       <c r="R115" t="s">
-        <v>109</v>
+        <v>96</v>
       </c>
     </row>
     <row r="116" spans="1:18" x14ac:dyDescent="0.25">
@@ -7470,16 +7467,16 @@
         <v>0</v>
       </c>
       <c r="O116" t="s">
-        <v>19</v>
+        <v>6</v>
       </c>
       <c r="P116" t="s">
-        <v>19</v>
+        <v>6</v>
       </c>
       <c r="Q116">
         <v>4</v>
       </c>
       <c r="R116" t="s">
-        <v>110</v>
+        <v>97</v>
       </c>
     </row>
     <row r="117" spans="1:18" x14ac:dyDescent="0.25">
@@ -7526,16 +7523,16 @@
         <v>0</v>
       </c>
       <c r="O117" t="s">
-        <v>19</v>
+        <v>6</v>
       </c>
       <c r="P117" t="s">
-        <v>17</v>
+        <v>4</v>
       </c>
       <c r="Q117">
         <v>2</v>
       </c>
       <c r="R117" t="s">
-        <v>111</v>
+        <v>98</v>
       </c>
     </row>
     <row r="118" spans="1:18" x14ac:dyDescent="0.25">
@@ -7582,16 +7579,16 @@
         <v>0</v>
       </c>
       <c r="O118" t="s">
-        <v>19</v>
+        <v>6</v>
       </c>
       <c r="P118" t="s">
-        <v>19</v>
+        <v>6</v>
       </c>
       <c r="Q118">
         <v>5</v>
       </c>
       <c r="R118" t="s">
-        <v>112</v>
+        <v>99</v>
       </c>
     </row>
     <row r="119" spans="1:18" x14ac:dyDescent="0.25">
@@ -7638,16 +7635,16 @@
         <v>0</v>
       </c>
       <c r="O119" t="s">
-        <v>19</v>
+        <v>6</v>
       </c>
       <c r="P119" t="s">
-        <v>19</v>
+        <v>6</v>
       </c>
       <c r="Q119">
         <v>2</v>
       </c>
       <c r="R119" t="s">
-        <v>114</v>
+        <v>101</v>
       </c>
     </row>
     <row r="120" spans="1:18" x14ac:dyDescent="0.25">
@@ -7694,16 +7691,16 @@
         <v>0</v>
       </c>
       <c r="O120" t="s">
-        <v>19</v>
+        <v>6</v>
       </c>
       <c r="P120" t="s">
-        <v>19</v>
+        <v>6</v>
       </c>
       <c r="Q120">
         <v>4</v>
       </c>
       <c r="R120" t="s">
-        <v>113</v>
+        <v>100</v>
       </c>
     </row>
     <row r="121" spans="1:18" x14ac:dyDescent="0.25">
@@ -7750,16 +7747,16 @@
         <v>0</v>
       </c>
       <c r="O121" t="s">
-        <v>16</v>
+        <v>3</v>
       </c>
       <c r="P121" t="s">
-        <v>19</v>
+        <v>6</v>
       </c>
       <c r="Q121">
         <v>2</v>
       </c>
       <c r="R121" t="s">
-        <v>115</v>
+        <v>102</v>
       </c>
     </row>
     <row r="122" spans="1:18" x14ac:dyDescent="0.25">
@@ -7806,16 +7803,16 @@
         <v>0</v>
       </c>
       <c r="O122" t="s">
-        <v>19</v>
+        <v>6</v>
       </c>
       <c r="P122" t="s">
-        <v>17</v>
+        <v>4</v>
       </c>
       <c r="Q122">
         <v>1</v>
       </c>
       <c r="R122" t="s">
-        <v>116</v>
+        <v>103</v>
       </c>
     </row>
     <row r="123" spans="1:18" x14ac:dyDescent="0.25">
@@ -7862,16 +7859,16 @@
         <v>0</v>
       </c>
       <c r="O123" t="s">
-        <v>19</v>
+        <v>6</v>
       </c>
       <c r="P123" t="s">
-        <v>19</v>
+        <v>6</v>
       </c>
       <c r="Q123">
         <v>4</v>
       </c>
       <c r="R123" t="s">
-        <v>117</v>
+        <v>104</v>
       </c>
     </row>
     <row r="124" spans="1:18" x14ac:dyDescent="0.25">
@@ -7918,16 +7915,16 @@
         <v>0</v>
       </c>
       <c r="O124" t="s">
-        <v>17</v>
+        <v>4</v>
       </c>
       <c r="P124" t="s">
-        <v>19</v>
+        <v>6</v>
       </c>
       <c r="Q124">
         <v>2</v>
       </c>
       <c r="R124" t="s">
-        <v>118</v>
+        <v>105</v>
       </c>
     </row>
     <row r="125" spans="1:18" x14ac:dyDescent="0.25">
@@ -7974,16 +7971,16 @@
         <v>0</v>
       </c>
       <c r="O125" t="s">
-        <v>19</v>
+        <v>6</v>
       </c>
       <c r="P125" t="s">
-        <v>19</v>
+        <v>6</v>
       </c>
       <c r="Q125">
         <v>2</v>
       </c>
       <c r="R125" t="s">
-        <v>145</v>
+        <v>132</v>
       </c>
     </row>
     <row r="126" spans="1:18" x14ac:dyDescent="0.25">
@@ -8030,16 +8027,16 @@
         <v>0</v>
       </c>
       <c r="O126" t="s">
-        <v>19</v>
+        <v>6</v>
       </c>
       <c r="P126" t="s">
-        <v>19</v>
+        <v>6</v>
       </c>
       <c r="Q126">
         <v>2</v>
       </c>
       <c r="R126" t="s">
-        <v>146</v>
+        <v>133</v>
       </c>
     </row>
     <row r="127" spans="1:18" x14ac:dyDescent="0.25">
@@ -8086,16 +8083,16 @@
         <v>0</v>
       </c>
       <c r="O127" t="s">
-        <v>19</v>
+        <v>6</v>
       </c>
       <c r="P127" t="s">
-        <v>17</v>
+        <v>4</v>
       </c>
       <c r="Q127">
         <v>2</v>
       </c>
       <c r="R127" t="s">
-        <v>148</v>
+        <v>135</v>
       </c>
     </row>
     <row r="128" spans="1:18" x14ac:dyDescent="0.25">
@@ -8142,16 +8139,16 @@
         <v>0</v>
       </c>
       <c r="O128" t="s">
-        <v>19</v>
+        <v>6</v>
       </c>
       <c r="P128" t="s">
-        <v>19</v>
+        <v>6</v>
       </c>
       <c r="Q128">
         <v>1</v>
       </c>
       <c r="R128" t="s">
-        <v>147</v>
+        <v>134</v>
       </c>
     </row>
     <row r="129" spans="1:18" x14ac:dyDescent="0.25">
@@ -8198,16 +8195,16 @@
         <v>0</v>
       </c>
       <c r="O129" t="s">
-        <v>19</v>
+        <v>6</v>
       </c>
       <c r="P129" t="s">
-        <v>17</v>
+        <v>4</v>
       </c>
       <c r="Q129">
         <v>1</v>
       </c>
       <c r="R129" t="s">
-        <v>149</v>
+        <v>136</v>
       </c>
     </row>
     <row r="130" spans="1:18" x14ac:dyDescent="0.25">
@@ -8254,16 +8251,16 @@
         <v>0</v>
       </c>
       <c r="O130" t="s">
-        <v>19</v>
+        <v>6</v>
       </c>
       <c r="P130" t="s">
-        <v>19</v>
+        <v>6</v>
       </c>
       <c r="Q130">
         <v>5</v>
       </c>
       <c r="R130" t="s">
-        <v>150</v>
+        <v>137</v>
       </c>
     </row>
     <row r="131" spans="1:18" x14ac:dyDescent="0.25">
@@ -8310,16 +8307,16 @@
         <v>0</v>
       </c>
       <c r="O131" t="s">
-        <v>16</v>
+        <v>3</v>
       </c>
       <c r="P131" t="s">
-        <v>17</v>
+        <v>4</v>
       </c>
       <c r="Q131">
         <v>2</v>
       </c>
       <c r="R131" t="s">
-        <v>151</v>
+        <v>138</v>
       </c>
     </row>
     <row r="132" spans="1:18" x14ac:dyDescent="0.25">
@@ -8366,16 +8363,16 @@
         <v>0</v>
       </c>
       <c r="O132" t="s">
-        <v>19</v>
+        <v>6</v>
       </c>
       <c r="P132" t="s">
-        <v>16</v>
+        <v>3</v>
       </c>
       <c r="Q132">
         <v>3</v>
       </c>
       <c r="R132" t="s">
-        <v>152</v>
+        <v>139</v>
       </c>
     </row>
     <row r="133" spans="1:18" x14ac:dyDescent="0.25">
@@ -8422,16 +8419,16 @@
         <v>0</v>
       </c>
       <c r="O133" t="s">
-        <v>19</v>
+        <v>6</v>
       </c>
       <c r="P133" t="s">
-        <v>19</v>
+        <v>6</v>
       </c>
       <c r="Q133">
         <v>4</v>
       </c>
       <c r="R133" t="s">
-        <v>153</v>
+        <v>140</v>
       </c>
     </row>
     <row r="134" spans="1:18" x14ac:dyDescent="0.25">
@@ -8478,16 +8475,16 @@
         <v>0</v>
       </c>
       <c r="O134" t="s">
-        <v>16</v>
+        <v>3</v>
       </c>
       <c r="P134" t="s">
-        <v>19</v>
+        <v>6</v>
       </c>
       <c r="Q134">
         <v>4</v>
       </c>
       <c r="R134" t="s">
-        <v>154</v>
+        <v>141</v>
       </c>
     </row>
     <row r="135" spans="1:18" x14ac:dyDescent="0.25">
@@ -8534,16 +8531,16 @@
         <v>0</v>
       </c>
       <c r="O135" t="s">
-        <v>16</v>
+        <v>3</v>
       </c>
       <c r="P135" t="s">
-        <v>19</v>
+        <v>6</v>
       </c>
       <c r="Q135">
         <v>3</v>
       </c>
       <c r="R135" t="s">
-        <v>156</v>
+        <v>143</v>
       </c>
     </row>
     <row r="136" spans="1:18" x14ac:dyDescent="0.25">
@@ -8590,16 +8587,16 @@
         <v>0</v>
       </c>
       <c r="O136" t="s">
-        <v>19</v>
+        <v>6</v>
       </c>
       <c r="P136" t="s">
-        <v>17</v>
+        <v>4</v>
       </c>
       <c r="Q136">
         <v>1</v>
       </c>
       <c r="R136" t="s">
-        <v>155</v>
+        <v>142</v>
       </c>
     </row>
     <row r="137" spans="1:18" x14ac:dyDescent="0.25">
@@ -8646,16 +8643,16 @@
         <v>0</v>
       </c>
       <c r="O137" t="s">
-        <v>19</v>
+        <v>6</v>
       </c>
       <c r="P137" t="s">
-        <v>16</v>
+        <v>3</v>
       </c>
       <c r="Q137">
         <v>2</v>
       </c>
       <c r="R137" t="s">
-        <v>158</v>
+        <v>145</v>
       </c>
     </row>
     <row r="138" spans="1:18" x14ac:dyDescent="0.25">
@@ -8702,16 +8699,16 @@
         <v>0</v>
       </c>
       <c r="O138" t="s">
-        <v>19</v>
+        <v>6</v>
       </c>
       <c r="P138" t="s">
-        <v>19</v>
+        <v>6</v>
       </c>
       <c r="Q138">
         <v>4</v>
       </c>
       <c r="R138" t="s">
-        <v>157</v>
+        <v>144</v>
       </c>
     </row>
     <row r="139" spans="1:18" x14ac:dyDescent="0.25">
@@ -8758,16 +8755,16 @@
         <v>1</v>
       </c>
       <c r="O139" t="s">
-        <v>19</v>
+        <v>6</v>
       </c>
       <c r="P139" t="s">
-        <v>19</v>
+        <v>6</v>
       </c>
       <c r="Q139">
         <v>4</v>
       </c>
       <c r="R139" t="s">
-        <v>159</v>
+        <v>146</v>
       </c>
     </row>
     <row r="140" spans="1:18" x14ac:dyDescent="0.25">
@@ -8814,16 +8811,16 @@
         <v>0</v>
       </c>
       <c r="O140" t="s">
-        <v>16</v>
+        <v>3</v>
       </c>
       <c r="P140" t="s">
-        <v>19</v>
+        <v>6</v>
       </c>
       <c r="Q140">
         <v>2</v>
       </c>
       <c r="R140" t="s">
-        <v>160</v>
+        <v>147</v>
       </c>
     </row>
     <row r="141" spans="1:18" x14ac:dyDescent="0.25">
@@ -8870,16 +8867,16 @@
         <v>0</v>
       </c>
       <c r="O141" t="s">
-        <v>16</v>
+        <v>3</v>
       </c>
       <c r="P141" t="s">
-        <v>19</v>
+        <v>6</v>
       </c>
       <c r="Q141">
         <v>3</v>
       </c>
       <c r="R141" t="s">
-        <v>161</v>
+        <v>148</v>
       </c>
     </row>
     <row r="142" spans="1:18" x14ac:dyDescent="0.25">
@@ -8926,16 +8923,16 @@
         <v>0</v>
       </c>
       <c r="O142" t="s">
-        <v>19</v>
+        <v>6</v>
       </c>
       <c r="P142" t="s">
-        <v>19</v>
+        <v>6</v>
       </c>
       <c r="Q142">
         <v>3</v>
       </c>
       <c r="R142" t="s">
-        <v>162</v>
+        <v>149</v>
       </c>
     </row>
     <row r="143" spans="1:18" x14ac:dyDescent="0.25">
@@ -8982,16 +8979,16 @@
         <v>0</v>
       </c>
       <c r="O143" t="s">
-        <v>16</v>
+        <v>3</v>
       </c>
       <c r="P143" t="s">
-        <v>17</v>
+        <v>4</v>
       </c>
       <c r="Q143">
         <v>1</v>
       </c>
       <c r="R143" t="s">
-        <v>163</v>
+        <v>150</v>
       </c>
     </row>
     <row r="144" spans="1:18" x14ac:dyDescent="0.25">
@@ -9038,16 +9035,16 @@
         <v>0</v>
       </c>
       <c r="O144" t="s">
-        <v>19</v>
+        <v>6</v>
       </c>
       <c r="P144" t="s">
-        <v>19</v>
+        <v>6</v>
       </c>
       <c r="Q144">
         <v>4</v>
       </c>
       <c r="R144" t="s">
-        <v>164</v>
+        <v>151</v>
       </c>
     </row>
     <row r="145" spans="1:18" x14ac:dyDescent="0.25">
@@ -9094,16 +9091,16 @@
         <v>0</v>
       </c>
       <c r="O145" t="s">
-        <v>19</v>
+        <v>6</v>
       </c>
       <c r="P145" t="s">
-        <v>19</v>
+        <v>6</v>
       </c>
       <c r="Q145">
         <v>1</v>
       </c>
       <c r="R145" t="s">
-        <v>165</v>
+        <v>152</v>
       </c>
     </row>
     <row r="146" spans="1:18" x14ac:dyDescent="0.25">
@@ -9150,16 +9147,16 @@
         <v>0</v>
       </c>
       <c r="O146" t="s">
-        <v>19</v>
+        <v>6</v>
       </c>
       <c r="P146" t="s">
-        <v>17</v>
+        <v>4</v>
       </c>
       <c r="Q146">
         <v>2</v>
       </c>
       <c r="R146" t="s">
-        <v>166</v>
+        <v>153</v>
       </c>
     </row>
     <row r="147" spans="1:18" x14ac:dyDescent="0.25">
@@ -9206,16 +9203,16 @@
         <v>0</v>
       </c>
       <c r="O147" t="s">
-        <v>16</v>
+        <v>3</v>
       </c>
       <c r="P147" t="s">
-        <v>17</v>
+        <v>4</v>
       </c>
       <c r="Q147">
         <v>3</v>
       </c>
       <c r="R147" t="s">
-        <v>167</v>
+        <v>154</v>
       </c>
     </row>
     <row r="148" spans="1:18" x14ac:dyDescent="0.25">
@@ -9262,16 +9259,16 @@
         <v>0</v>
       </c>
       <c r="O148" t="s">
-        <v>19</v>
+        <v>6</v>
       </c>
       <c r="P148" t="s">
-        <v>19</v>
+        <v>6</v>
       </c>
       <c r="Q148">
         <v>5</v>
       </c>
       <c r="R148" t="s">
-        <v>168</v>
+        <v>155</v>
       </c>
     </row>
     <row r="149" spans="1:18" x14ac:dyDescent="0.25">
@@ -9318,16 +9315,16 @@
         <v>0</v>
       </c>
       <c r="O149" t="s">
-        <v>19</v>
+        <v>6</v>
       </c>
       <c r="P149" t="s">
-        <v>19</v>
+        <v>6</v>
       </c>
       <c r="Q149">
         <v>4</v>
       </c>
       <c r="R149" t="s">
-        <v>169</v>
+        <v>156</v>
       </c>
     </row>
     <row r="150" spans="1:18" x14ac:dyDescent="0.25">
@@ -9374,16 +9371,16 @@
         <v>0</v>
       </c>
       <c r="O150" t="s">
-        <v>19</v>
+        <v>6</v>
       </c>
       <c r="P150" t="s">
-        <v>17</v>
+        <v>4</v>
       </c>
       <c r="Q150">
         <v>5</v>
       </c>
       <c r="R150" t="s">
-        <v>171</v>
+        <v>158</v>
       </c>
     </row>
     <row r="151" spans="1:18" x14ac:dyDescent="0.25">
@@ -9430,16 +9427,16 @@
         <v>0</v>
       </c>
       <c r="O151" t="s">
-        <v>19</v>
+        <v>6</v>
       </c>
       <c r="P151" t="s">
-        <v>19</v>
+        <v>6</v>
       </c>
       <c r="Q151">
         <v>4</v>
       </c>
       <c r="R151" t="s">
-        <v>170</v>
+        <v>157</v>
       </c>
     </row>
     <row r="152" spans="1:18" x14ac:dyDescent="0.25">
@@ -9486,16 +9483,16 @@
         <v>0</v>
       </c>
       <c r="O152" t="s">
-        <v>17</v>
+        <v>4</v>
       </c>
       <c r="P152" t="s">
-        <v>17</v>
+        <v>4</v>
       </c>
       <c r="Q152">
         <v>1</v>
       </c>
       <c r="R152" t="s">
-        <v>173</v>
+        <v>160</v>
       </c>
     </row>
     <row r="153" spans="1:18" x14ac:dyDescent="0.25">
@@ -9542,16 +9539,16 @@
         <v>0</v>
       </c>
       <c r="O153" t="s">
-        <v>19</v>
+        <v>6</v>
       </c>
       <c r="P153" t="s">
-        <v>17</v>
+        <v>4</v>
       </c>
       <c r="Q153">
         <v>2</v>
       </c>
       <c r="R153" t="s">
-        <v>172</v>
+        <v>159</v>
       </c>
     </row>
     <row r="154" spans="1:18" x14ac:dyDescent="0.25">
@@ -9598,16 +9595,16 @@
         <v>0</v>
       </c>
       <c r="O154" t="s">
-        <v>19</v>
+        <v>6</v>
       </c>
       <c r="P154" t="s">
-        <v>17</v>
+        <v>4</v>
       </c>
       <c r="Q154">
         <v>1</v>
       </c>
       <c r="R154" t="s">
-        <v>174</v>
+        <v>161</v>
       </c>
     </row>
     <row r="155" spans="1:18" x14ac:dyDescent="0.25">
@@ -9654,16 +9651,16 @@
         <v>0</v>
       </c>
       <c r="O155" t="s">
-        <v>19</v>
+        <v>6</v>
       </c>
       <c r="P155" t="s">
-        <v>17</v>
+        <v>4</v>
       </c>
       <c r="Q155">
         <v>2</v>
       </c>
       <c r="R155" t="s">
-        <v>105</v>
+        <v>92</v>
       </c>
     </row>
     <row r="156" spans="1:18" x14ac:dyDescent="0.25">
@@ -9710,16 +9707,16 @@
         <v>0</v>
       </c>
       <c r="O156" t="s">
-        <v>19</v>
+        <v>6</v>
       </c>
       <c r="P156" t="s">
-        <v>16</v>
+        <v>3</v>
       </c>
       <c r="Q156">
         <v>2</v>
       </c>
       <c r="R156" t="s">
-        <v>176</v>
+        <v>163</v>
       </c>
     </row>
     <row r="157" spans="1:18" x14ac:dyDescent="0.25">
@@ -9766,16 +9763,16 @@
         <v>0</v>
       </c>
       <c r="O157" t="s">
-        <v>16</v>
+        <v>3</v>
       </c>
       <c r="P157" t="s">
-        <v>17</v>
+        <v>4</v>
       </c>
       <c r="Q157">
         <v>1</v>
       </c>
       <c r="R157" t="s">
-        <v>175</v>
+        <v>162</v>
       </c>
     </row>
     <row r="158" spans="1:18" x14ac:dyDescent="0.25">
@@ -9822,16 +9819,16 @@
         <v>0</v>
       </c>
       <c r="O158" t="s">
-        <v>16</v>
+        <v>3</v>
       </c>
       <c r="P158" t="s">
-        <v>17</v>
+        <v>4</v>
       </c>
       <c r="Q158">
         <v>2</v>
       </c>
       <c r="R158" t="s">
-        <v>178</v>
+        <v>165</v>
       </c>
     </row>
     <row r="159" spans="1:18" x14ac:dyDescent="0.25">
@@ -9878,16 +9875,16 @@
         <v>0</v>
       </c>
       <c r="O159" t="s">
-        <v>19</v>
+        <v>6</v>
       </c>
       <c r="P159" t="s">
-        <v>17</v>
+        <v>4</v>
       </c>
       <c r="Q159">
         <v>2</v>
       </c>
       <c r="R159" t="s">
-        <v>177</v>
+        <v>164</v>
       </c>
     </row>
     <row r="160" spans="1:18" x14ac:dyDescent="0.25">
@@ -9934,16 +9931,16 @@
         <v>0</v>
       </c>
       <c r="O160" t="s">
-        <v>19</v>
+        <v>6</v>
       </c>
       <c r="P160" t="s">
-        <v>19</v>
+        <v>6</v>
       </c>
       <c r="Q160">
         <v>2</v>
       </c>
       <c r="R160" t="s">
-        <v>179</v>
+        <v>166</v>
       </c>
     </row>
     <row r="161" spans="1:18" x14ac:dyDescent="0.25">
@@ -9990,16 +9987,16 @@
         <v>0</v>
       </c>
       <c r="O161" t="s">
-        <v>19</v>
+        <v>6</v>
       </c>
       <c r="P161" t="s">
-        <v>19</v>
+        <v>6</v>
       </c>
       <c r="Q161">
         <v>4</v>
       </c>
       <c r="R161" t="s">
-        <v>180</v>
+        <v>167</v>
       </c>
     </row>
     <row r="162" spans="1:18" x14ac:dyDescent="0.25">
@@ -10046,16 +10043,16 @@
         <v>0</v>
       </c>
       <c r="O162" t="s">
-        <v>19</v>
+        <v>6</v>
       </c>
       <c r="P162" t="s">
-        <v>19</v>
+        <v>6</v>
       </c>
       <c r="Q162">
         <v>4</v>
       </c>
       <c r="R162" t="s">
-        <v>181</v>
+        <v>168</v>
       </c>
     </row>
     <row r="163" spans="1:18" x14ac:dyDescent="0.25">
@@ -10102,16 +10099,16 @@
         <v>0</v>
       </c>
       <c r="O163" t="s">
-        <v>19</v>
+        <v>6</v>
       </c>
       <c r="P163" t="s">
-        <v>19</v>
+        <v>6</v>
       </c>
       <c r="Q163">
         <v>5</v>
       </c>
       <c r="R163" t="s">
-        <v>183</v>
+        <v>170</v>
       </c>
     </row>
     <row r="164" spans="1:18" x14ac:dyDescent="0.25">
@@ -10158,16 +10155,16 @@
         <v>0</v>
       </c>
       <c r="O164" t="s">
-        <v>19</v>
+        <v>6</v>
       </c>
       <c r="P164" t="s">
-        <v>17</v>
+        <v>4</v>
       </c>
       <c r="Q164">
         <v>3</v>
       </c>
       <c r="R164" t="s">
-        <v>182</v>
+        <v>169</v>
       </c>
     </row>
     <row r="165" spans="1:18" x14ac:dyDescent="0.25">
@@ -10214,16 +10211,16 @@
         <v>0</v>
       </c>
       <c r="O165" t="s">
-        <v>17</v>
+        <v>4</v>
       </c>
       <c r="P165" t="s">
-        <v>17</v>
+        <v>4</v>
       </c>
       <c r="Q165">
         <v>2</v>
       </c>
       <c r="R165" t="s">
-        <v>105</v>
+        <v>92</v>
       </c>
     </row>
     <row r="166" spans="1:18" x14ac:dyDescent="0.25">
@@ -10270,16 +10267,16 @@
         <v>0</v>
       </c>
       <c r="O166" t="s">
-        <v>19</v>
+        <v>6</v>
       </c>
       <c r="P166" t="s">
-        <v>19</v>
+        <v>6</v>
       </c>
       <c r="Q166">
         <v>5</v>
       </c>
       <c r="R166" t="s">
-        <v>185</v>
+        <v>172</v>
       </c>
     </row>
     <row r="167" spans="1:18" x14ac:dyDescent="0.25">
@@ -10326,16 +10323,16 @@
         <v>0</v>
       </c>
       <c r="O167" t="s">
-        <v>19</v>
+        <v>6</v>
       </c>
       <c r="P167" t="s">
-        <v>19</v>
+        <v>6</v>
       </c>
       <c r="Q167">
         <v>4</v>
       </c>
       <c r="R167" t="s">
-        <v>186</v>
+        <v>173</v>
       </c>
     </row>
     <row r="168" spans="1:18" x14ac:dyDescent="0.25">
@@ -10382,16 +10379,16 @@
         <v>0</v>
       </c>
       <c r="O168" t="s">
-        <v>16</v>
+        <v>3</v>
       </c>
       <c r="P168" t="s">
-        <v>19</v>
+        <v>6</v>
       </c>
       <c r="Q168">
         <v>5</v>
       </c>
       <c r="R168" t="s">
-        <v>187</v>
+        <v>174</v>
       </c>
     </row>
     <row r="169" spans="1:18" x14ac:dyDescent="0.25">
@@ -10438,16 +10435,16 @@
         <v>0</v>
       </c>
       <c r="O169" t="s">
-        <v>19</v>
+        <v>6</v>
       </c>
       <c r="P169" t="s">
-        <v>17</v>
+        <v>4</v>
       </c>
       <c r="Q169">
         <v>3</v>
       </c>
       <c r="R169" t="s">
-        <v>188</v>
+        <v>175</v>
       </c>
     </row>
     <row r="170" spans="1:18" x14ac:dyDescent="0.25">
@@ -10494,16 +10491,16 @@
         <v>0</v>
       </c>
       <c r="O170" t="s">
-        <v>19</v>
+        <v>6</v>
       </c>
       <c r="P170" t="s">
-        <v>16</v>
+        <v>3</v>
       </c>
       <c r="Q170">
         <v>1</v>
       </c>
       <c r="R170" t="s">
-        <v>189</v>
+        <v>176</v>
       </c>
     </row>
     <row r="171" spans="1:18" x14ac:dyDescent="0.25">
@@ -10550,16 +10547,16 @@
         <v>0</v>
       </c>
       <c r="O171" t="s">
-        <v>19</v>
+        <v>6</v>
       </c>
       <c r="P171" t="s">
-        <v>19</v>
+        <v>6</v>
       </c>
       <c r="Q171">
         <v>2</v>
       </c>
       <c r="R171" t="s">
-        <v>190</v>
+        <v>177</v>
       </c>
     </row>
     <row r="172" spans="1:18" x14ac:dyDescent="0.25">
@@ -10606,16 +10603,16 @@
         <v>0</v>
       </c>
       <c r="O172" t="s">
-        <v>19</v>
+        <v>6</v>
       </c>
       <c r="P172" t="s">
-        <v>19</v>
+        <v>6</v>
       </c>
       <c r="Q172">
         <v>1</v>
       </c>
       <c r="R172" t="s">
-        <v>191</v>
+        <v>178</v>
       </c>
     </row>
     <row r="173" spans="1:18" x14ac:dyDescent="0.25">
@@ -10662,16 +10659,16 @@
         <v>0</v>
       </c>
       <c r="O173" t="s">
-        <v>16</v>
+        <v>3</v>
       </c>
       <c r="P173" t="s">
-        <v>16</v>
+        <v>3</v>
       </c>
       <c r="Q173">
         <v>3</v>
       </c>
       <c r="R173" t="s">
-        <v>193</v>
+        <v>179</v>
       </c>
     </row>
     <row r="174" spans="1:18" x14ac:dyDescent="0.25">
@@ -10718,16 +10715,16 @@
         <v>0</v>
       </c>
       <c r="O174" t="s">
-        <v>19</v>
+        <v>6</v>
       </c>
       <c r="P174" t="s">
-        <v>19</v>
+        <v>6</v>
       </c>
       <c r="Q174">
         <v>3</v>
       </c>
       <c r="R174" t="s">
-        <v>194</v>
+        <v>180</v>
       </c>
     </row>
     <row r="175" spans="1:18" x14ac:dyDescent="0.25">
@@ -10774,16 +10771,16 @@
         <v>0</v>
       </c>
       <c r="O175" t="s">
-        <v>17</v>
+        <v>4</v>
       </c>
       <c r="P175" t="s">
-        <v>19</v>
+        <v>6</v>
       </c>
       <c r="Q175">
         <v>4</v>
       </c>
       <c r="R175" t="s">
-        <v>195</v>
+        <v>181</v>
       </c>
     </row>
     <row r="176" spans="1:18" x14ac:dyDescent="0.25">
@@ -10830,16 +10827,16 @@
         <v>0</v>
       </c>
       <c r="O176" t="s">
-        <v>19</v>
+        <v>6</v>
       </c>
       <c r="P176" t="s">
-        <v>19</v>
+        <v>6</v>
       </c>
       <c r="Q176">
         <v>4</v>
       </c>
       <c r="R176" t="s">
-        <v>196</v>
+        <v>182</v>
       </c>
     </row>
     <row r="177" spans="1:18" x14ac:dyDescent="0.25">
@@ -10886,16 +10883,16 @@
         <v>0</v>
       </c>
       <c r="O177" t="s">
-        <v>19</v>
+        <v>6</v>
       </c>
       <c r="P177" t="s">
-        <v>19</v>
+        <v>6</v>
       </c>
       <c r="Q177">
         <v>2</v>
       </c>
       <c r="R177" t="s">
-        <v>198</v>
+        <v>184</v>
       </c>
     </row>
     <row r="178" spans="1:18" x14ac:dyDescent="0.25">
@@ -10942,16 +10939,16 @@
         <v>0</v>
       </c>
       <c r="O178" t="s">
-        <v>19</v>
+        <v>6</v>
       </c>
       <c r="P178" t="s">
-        <v>19</v>
+        <v>6</v>
       </c>
       <c r="Q178">
         <v>2</v>
       </c>
       <c r="R178" t="s">
-        <v>197</v>
+        <v>183</v>
       </c>
     </row>
     <row r="179" spans="1:18" x14ac:dyDescent="0.25">
@@ -10998,16 +10995,16 @@
         <v>0</v>
       </c>
       <c r="O179" t="s">
-        <v>19</v>
+        <v>6</v>
       </c>
       <c r="P179" t="s">
-        <v>19</v>
+        <v>6</v>
       </c>
       <c r="Q179">
         <v>2</v>
       </c>
       <c r="R179" t="s">
-        <v>200</v>
+        <v>186</v>
       </c>
     </row>
     <row r="180" spans="1:18" x14ac:dyDescent="0.25">
@@ -11054,21 +11051,21 @@
         <v>0</v>
       </c>
       <c r="O180" t="s">
-        <v>19</v>
+        <v>6</v>
       </c>
       <c r="P180" t="s">
-        <v>19</v>
+        <v>6</v>
       </c>
       <c r="Q180">
         <v>3</v>
       </c>
       <c r="R180" t="s">
-        <v>199</v>
+        <v>185</v>
       </c>
     </row>
     <row r="181" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A181" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="B181">
         <v>1</v>
@@ -11110,21 +11107,21 @@
         <v>0</v>
       </c>
       <c r="O181" t="s">
-        <v>17</v>
+        <v>4</v>
       </c>
       <c r="P181" t="s">
-        <v>17</v>
+        <v>4</v>
       </c>
       <c r="Q181">
         <v>1</v>
       </c>
       <c r="R181" t="s">
-        <v>184</v>
+        <v>171</v>
       </c>
     </row>
     <row r="182" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A182" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="B182">
         <v>1</v>
@@ -11166,21 +11163,21 @@
         <v>0</v>
       </c>
       <c r="O182" t="s">
-        <v>16</v>
+        <v>3</v>
       </c>
       <c r="P182" t="s">
-        <v>17</v>
+        <v>4</v>
       </c>
       <c r="Q182">
         <v>3</v>
       </c>
       <c r="R182" t="s">
-        <v>201</v>
+        <v>187</v>
       </c>
     </row>
     <row r="183" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A183" t="s">
-        <v>202</v>
+        <v>191</v>
       </c>
       <c r="B183">
         <v>0</v>
@@ -11222,16 +11219,16 @@
         <v>0</v>
       </c>
       <c r="O183" t="s">
-        <v>19</v>
+        <v>6</v>
       </c>
       <c r="P183" t="s">
-        <v>17</v>
+        <v>4</v>
       </c>
       <c r="Q183">
         <v>3</v>
       </c>
       <c r="R183" t="s">
-        <v>203</v>
+        <v>188</v>
       </c>
     </row>
   </sheetData>

</xml_diff>